<commit_message>
Coin change problem started
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27428" windowHeight="11734"/>
+    <workbookView windowWidth="27428" windowHeight="11734" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
+    <sheet name="Coin change" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Longest Common Subsequence</t>
   </si>
@@ -89,6 +90,27 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>dp init</t>
+  </si>
+  <si>
+    <t>dp formula</t>
+  </si>
+  <si>
+    <t>min(12,1+dp[1-1])</t>
+  </si>
+  <si>
+    <t>min(12,1+dp[2-1],1+dp[2-2])</t>
+  </si>
+  <si>
+    <t>dp final</t>
+  </si>
+  <si>
+    <t>coins</t>
   </si>
 </sst>
 </file>
@@ -96,10 +118,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -126,7 +148,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,31 +161,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -218,7 +225,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -227,6 +234,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -234,29 +271,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,13 +300,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,7 +402,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,13 +450,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,72 +474,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -399,66 +481,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,23 +512,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -530,22 +552,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,26 +601,15 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -605,141 +627,139 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,7 +1081,7 @@
   <sheetPr/>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A34" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
@@ -1397,16 +1417,16 @@
       <c r="B48" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="3">
         <v>4</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="3">
         <v>3</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="3">
         <v>3</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1414,16 +1434,16 @@
       <c r="B49" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="3">
         <v>5</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="3">
         <v>4</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="3">
         <v>4</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1431,4 +1451,154 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.55"/>
+  <cols>
+    <col min="1" max="1" width="10.7387387387387" customWidth="1"/>
+    <col min="3" max="3" width="18.045045045045" customWidth="1"/>
+    <col min="4" max="4" width="26.7837837837838" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2">
+        <v>9</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes to LCS algorithm
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -16,33 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
-  <si>
-    <t>dp[]</t>
-  </si>
-  <si>
-    <t>fib(0)</t>
-  </si>
-  <si>
-    <t>fib(1)</t>
-  </si>
-  <si>
-    <t>fib(2)</t>
-  </si>
-  <si>
-    <t>fib(3)</t>
-  </si>
-  <si>
-    <t>fib(4)</t>
-  </si>
-  <si>
-    <t>fib(5)</t>
-  </si>
-  <si>
-    <t>fib(6)</t>
-  </si>
-  <si>
-    <t>fib(7)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>fib(n)</t>
   </si>
   <si>
     <t>Longest Common Subsequence</t>
@@ -168,9 +147,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -196,6 +175,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -204,7 +199,90 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,59 +296,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -280,52 +305,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -334,7 +313,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,121 +328,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,61 +502,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,30 +533,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,6 +576,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -636,11 +609,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,7 +637,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -676,130 +655,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -878,15 +857,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>328930</xdr:colOff>
+      <xdr:colOff>319405</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:rowOff>8255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>394335</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147955</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -903,7 +882,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="938530" y="860425"/>
+          <a:off x="929005" y="770255"/>
           <a:ext cx="4342130" cy="2425700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1178,13 +1157,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -1197,108 +1176,85 @@
         <v>1</v>
       </c>
       <c r="D1">
-        <f t="shared" ref="D1:M1" si="0">B1+C1</f>
         <v>1</v>
       </c>
       <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="F1">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>12</v>
+      </c>
+      <c r="J1">
+        <v>13</v>
+      </c>
+      <c r="K1">
+        <v>14</v>
+      </c>
+      <c r="L1">
+        <v>15</v>
+      </c>
+      <c r="M1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:M2" si="0">C2+B2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F1">
+      <c r="F2" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G1">
+      <c r="G2" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1">
+      <c r="H2" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I1">
+      <c r="I2" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J1">
+      <c r="J2" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K1">
+      <c r="K2" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L1">
+      <c r="L2" s="5">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="M1">
+      <c r="M2" s="5">
         <f t="shared" si="0"/>
         <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2">
-        <v>13</v>
-      </c>
-      <c r="K2">
-        <v>14</v>
-      </c>
-      <c r="L2">
-        <v>15</v>
-      </c>
-      <c r="M2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1327,26 +1283,26 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="3:6">
       <c r="C3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1363,7 +1319,7 @@
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -1380,7 +1336,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <v>2</v>
@@ -1397,7 +1353,7 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1414,7 +1370,7 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1431,7 +1387,7 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -1448,36 +1404,36 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
         <v>17</v>
       </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" t="s">
-        <v>24</v>
-      </c>
       <c r="J23" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -1508,7 +1464,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1540,46 +1496,46 @@
     </row>
     <row r="27" spans="2:7">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="3:6">
       <c r="C43" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E43" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F43" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -1596,7 +1552,7 @@
     </row>
     <row r="45" spans="2:6">
       <c r="B45" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
@@ -1613,7 +1569,7 @@
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C46" s="3">
         <v>2</v>
@@ -1630,7 +1586,7 @@
     </row>
     <row r="47" spans="2:6">
       <c r="B47" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C47" s="3">
         <v>3</v>
@@ -1647,7 +1603,7 @@
     </row>
     <row r="48" spans="2:6">
       <c r="B48" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C48" s="3">
         <v>4</v>
@@ -1664,7 +1620,7 @@
     </row>
     <row r="49" spans="2:6">
       <c r="B49" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C49" s="3">
         <v>5</v>
@@ -1704,7 +1660,7 @@
   <sheetData>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1745,7 +1701,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1786,39 +1742,39 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1850,12 +1806,12 @@
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>1</v>

</xml_diff>

<commit_message>
implemented Word Break problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>n</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>WordBreak</t>
+  </si>
+  <si>
+    <t>wordDict = ["leet","code"]</t>
+  </si>
+  <si>
+    <t>s[i]</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>WB[i]</t>
+  </si>
+  <si>
+    <t>WB[0 + len("leet")]</t>
   </si>
   <si>
     <t>dp init</t>
@@ -164,12 +185,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +214,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9.75"/>
+      <color rgb="FF263238"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -201,11 +274,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -217,37 +312,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,22 +353,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -283,59 +363,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -346,187 +373,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,26 +582,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,6 +615,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -614,15 +652,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,11 +673,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,12 +685,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -676,140 +703,144 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1232,49 +1263,49 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9">
         <f t="shared" ref="D2:M2" si="0">C2+B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="9">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="9">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="9">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
@@ -1289,10 +1320,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1479,14 +1510,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="1"/>
-    <row r="19" customFormat="1"/>
     <row r="20" customFormat="1" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" customFormat="1"/>
     <row r="22" customFormat="1" spans="1:10">
       <c r="A22" t="s">
         <v>14</v>
@@ -1515,7 +1543,7 @@
       <c r="I22">
         <v>7</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="J22" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1523,35 +1551,34 @@
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>10</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="2">
         <v>9</v>
       </c>
-      <c r="D23" s="4">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4">
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
         <v>5</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="2">
         <v>3</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>7</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="2">
         <v>101</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="2">
         <v>18</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" customFormat="1"/>
     <row r="25" customFormat="1" spans="1:10">
       <c r="A25" t="s">
         <v>16</v>
@@ -1562,7 +1589,7 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>4</v>
       </c>
       <c r="E25">
@@ -1584,7 +1611,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="1"/>
     <row r="27" customFormat="1" spans="1:2">
       <c r="A27" t="s">
         <v>17</v>
@@ -1768,6 +1794,114 @@
       </c>
       <c r="F54" s="3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="11:11">
+      <c r="K66" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <v>4</v>
+      </c>
+      <c r="G67">
+        <v>5</v>
+      </c>
+      <c r="H67">
+        <v>6</v>
+      </c>
+      <c r="I67">
+        <v>7</v>
+      </c>
+      <c r="J67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1836,7 +1970,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1877,39 +2011,39 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1941,12 +2075,12 @@
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>1</v>

</xml_diff>

<commit_message>
completed ClimbingStairs and ShortestCommonSupersequence problems
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t>n</t>
   </si>
@@ -24,7 +24,7 @@
     <t>fib(n)</t>
   </si>
   <si>
-    <t>Longest Common Subsequence</t>
+    <t>LongestCommonSubsequence</t>
   </si>
   <si>
     <t>text1</t>
@@ -123,22 +123,73 @@
     <t>WordBreak</t>
   </si>
   <si>
+    <t>s[i]</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>WB[i]</t>
+  </si>
+  <si>
+    <t>WB[0 + len("leet")]</t>
+  </si>
+  <si>
     <t>wordDict = ["leet","code"]</t>
   </si>
   <si>
-    <t>s[i]</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>WB[i]</t>
-  </si>
-  <si>
-    <t>WB[0 + len("leet")]</t>
+    <t>ClimbingStairs</t>
+  </si>
+  <si>
+    <t>1 or 2 steps</t>
+  </si>
+  <si>
+    <t>dp[i]</t>
+  </si>
+  <si>
+    <t>dp[1]+dp[2]</t>
+  </si>
+  <si>
+    <t>dp[2]+dp[3]</t>
+  </si>
+  <si>
+    <t>dp[3]+dp[4]</t>
+  </si>
+  <si>
+    <t>dp[4]+dp[5]</t>
+  </si>
+  <si>
+    <t>1 or 2 or 3 steps</t>
+  </si>
+  <si>
+    <t>dp[1]+dp[2]+dp[3]</t>
+  </si>
+  <si>
+    <t>dp[2]+dp[3]+dp[4]</t>
+  </si>
+  <si>
+    <t>dp[3]+dp[4]+dp[5]</t>
+  </si>
+  <si>
+    <t>ShortestCommonSupersequence</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>1) Find Longest Common Subsequence (lcs) of two given strings. For example, lcs of “aggtab” and “gxtxayb” is “gtab”. </t>
+  </si>
+  <si>
+    <t>2) Insert non-lcs characters (in their original order in strings) to the lcs found above, and return the result. So “gtab” becomes “agxgtxayb” which is shortest common supersequence.</t>
   </si>
   <si>
     <t>dp init</t>
@@ -185,9 +236,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -220,9 +271,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -230,13 +280,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,17 +293,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,8 +355,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,28 +402,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -355,14 +414,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -373,192 +424,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -582,11 +633,58 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,22 +693,48 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="medium">
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,21 +746,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,6 +783,54 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -682,15 +839,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -700,147 +857,161 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1263,49 +1434,49 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9">
+      <c r="B2" s="23">
+        <v>0</v>
+      </c>
+      <c r="C2" s="23">
+        <v>1</v>
+      </c>
+      <c r="D2" s="23">
         <f t="shared" ref="D2:M2" si="0">C2+B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="23">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="23">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="23">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="23">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="23">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="23">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="23">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
@@ -1320,16 +1491,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="12.9238095238095" customWidth="1"/>
-    <col min="5" max="5" width="11.3904761904762" customWidth="1"/>
+    <col min="2" max="2" width="10.0761904761905" customWidth="1"/>
+    <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
+    <col min="4" max="4" width="15.3714285714286" customWidth="1"/>
+    <col min="5" max="5" width="11.5142857142857" customWidth="1"/>
     <col min="6" max="6" width="11.0380952380952" customWidth="1"/>
     <col min="7" max="7" width="11.3047619047619" customWidth="1"/>
   </cols>
@@ -1510,398 +1683,826 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="1" spans="1:1">
-      <c r="A20" s="1" t="s">
+    <row r="17" customFormat="1" spans="1:1">
+      <c r="A17" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" spans="1:10">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" spans="1:10">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>7</v>
+      </c>
+      <c r="H20" s="2">
+        <v>101</v>
+      </c>
+      <c r="I20" s="2">
+        <v>18</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:10">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>7</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" customFormat="1" spans="1:10">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="2">
-        <v>10</v>
-      </c>
-      <c r="C23" s="2">
-        <v>9</v>
-      </c>
-      <c r="D23" s="2">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
-        <v>3</v>
-      </c>
-      <c r="G23" s="2">
-        <v>7</v>
-      </c>
-      <c r="H23" s="2">
-        <v>101</v>
-      </c>
-      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" spans="1:2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" spans="1:2">
+      <c r="A25" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" customFormat="1" spans="1:10">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" spans="1:2">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27" customFormat="1" spans="1:2">
       <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="1:2">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:2">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:2">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:2">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" customFormat="1" spans="1:2">
-      <c r="A32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" customFormat="1" spans="1:2">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" customFormat="1" spans="1:2">
-      <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="1" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="3:6">
-      <c r="C48" t="s">
+    <row r="37" spans="3:6">
+      <c r="C37" t="s">
         <v>12</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D37" t="s">
         <v>30</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E37" t="s">
         <v>31</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
-      <c r="B49" t="s">
+    <row r="38" spans="2:6">
+      <c r="B38" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="2">
-        <v>0</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2">
-        <v>2</v>
-      </c>
-      <c r="F49" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50" t="s">
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="2">
-        <v>1</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2">
-        <v>2</v>
-      </c>
-      <c r="F50" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="B51" t="s">
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="2">
-        <v>2</v>
-      </c>
-      <c r="D51" s="2">
-        <v>2</v>
-      </c>
-      <c r="E51" s="2">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="B52" t="s">
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="2">
-        <v>3</v>
-      </c>
-      <c r="D52" s="2">
-        <v>2</v>
-      </c>
-      <c r="E52" s="2">
-        <v>2</v>
-      </c>
-      <c r="F52" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6">
-      <c r="B53" t="s">
+      <c r="C41" s="2">
+        <v>3</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C42" s="2">
         <v>4</v>
       </c>
-      <c r="D53" s="2">
-        <v>3</v>
-      </c>
-      <c r="E53" s="2">
-        <v>3</v>
-      </c>
-      <c r="F53" s="2">
-        <v>2</v>
+      <c r="D42" s="2">
+        <v>3</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3</v>
+      </c>
+      <c r="F42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4</v>
+      </c>
+      <c r="F43" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <v>6</v>
+      </c>
+      <c r="I49">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54" t="s">
+        <v>39</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75"/>
+    <row r="64" ht="15.75" spans="7:7">
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" ht="15.75" spans="6:7">
+      <c r="F65" s="9"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" ht="15.75" spans="5:7">
+      <c r="E66" s="9"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="10"/>
+    </row>
+    <row r="67" ht="15.75" spans="4:7">
+      <c r="D67" s="9"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" ht="15.75" spans="2:7">
+      <c r="B68" s="12"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="15"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="4">
         <v>8</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C71">
         <v>5</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" t="s">
+        <v>45</v>
+      </c>
+      <c r="D72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" ht="15.75"/>
+    <row r="77" ht="15.75" spans="7:7">
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" ht="15.75" spans="6:7">
+      <c r="F78" s="9"/>
+      <c r="G78" s="10"/>
+    </row>
+    <row r="79" ht="15.75" spans="5:7">
+      <c r="E79" s="9"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="10"/>
+    </row>
+    <row r="80" ht="15.75" spans="4:7">
+      <c r="D80" s="9"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="10"/>
+    </row>
+    <row r="81" ht="15.75" spans="2:7">
+      <c r="B81" s="12"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="15"/>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+      <c r="F82">
         <v>4</v>
       </c>
-      <c r="E54" s="2">
+      <c r="G82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="4">
+        <v>13</v>
+      </c>
+      <c r="C84">
+        <v>7</v>
+      </c>
+      <c r="D84">
         <v>4</v>
       </c>
-      <c r="F54" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="11:11">
-      <c r="K66" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>2</v>
-      </c>
-      <c r="E67">
-        <v>3</v>
-      </c>
-      <c r="F67">
+      <c r="E84">
+        <v>2</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" t="s">
+        <v>49</v>
+      </c>
+      <c r="C85" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="3:10">
+      <c r="C92" t="s">
+        <v>53</v>
+      </c>
+      <c r="D92" t="s">
+        <v>54</v>
+      </c>
+      <c r="E92" t="s">
+        <v>37</v>
+      </c>
+      <c r="F92" t="s">
+        <v>54</v>
+      </c>
+      <c r="G92" t="s">
         <v>4</v>
       </c>
-      <c r="G67">
+      <c r="H92" t="s">
+        <v>55</v>
+      </c>
+      <c r="I92" t="s">
         <v>5</v>
       </c>
-      <c r="H67">
-        <v>6</v>
-      </c>
-      <c r="I67">
-        <v>7</v>
-      </c>
-      <c r="J67" t="s">
+      <c r="J92" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
-      <c r="A68" t="s">
-        <v>36</v>
-      </c>
-      <c r="B68" s="6" t="s">
+    <row r="93" spans="2:10">
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="16">
+        <v>4</v>
+      </c>
+      <c r="D93" s="17">
+        <v>3</v>
+      </c>
+      <c r="E93" s="17">
+        <v>3</v>
+      </c>
+      <c r="F93" s="2">
+        <v>2</v>
+      </c>
+      <c r="G93" s="2">
+        <v>2</v>
+      </c>
+      <c r="H93" s="2">
+        <v>1</v>
+      </c>
+      <c r="I93" s="2">
+        <v>1</v>
+      </c>
+      <c r="J93" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10">
+      <c r="B94" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="18">
+        <v>4</v>
+      </c>
+      <c r="D94" s="17">
+        <v>3</v>
+      </c>
+      <c r="E94" s="17">
+        <v>3</v>
+      </c>
+      <c r="F94" s="2">
+        <v>2</v>
+      </c>
+      <c r="G94" s="2">
+        <v>2</v>
+      </c>
+      <c r="H94" s="2">
+        <v>1</v>
+      </c>
+      <c r="I94" s="2">
+        <v>1</v>
+      </c>
+      <c r="J94" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10">
+      <c r="B95" t="s">
+        <v>53</v>
+      </c>
+      <c r="C95" s="19">
+        <v>4</v>
+      </c>
+      <c r="D95" s="20">
+        <v>3</v>
+      </c>
+      <c r="E95" s="20">
+        <v>3</v>
+      </c>
+      <c r="F95" s="2">
+        <v>2</v>
+      </c>
+      <c r="G95" s="2">
+        <v>2</v>
+      </c>
+      <c r="H95" s="2">
+        <v>1</v>
+      </c>
+      <c r="I95" s="2">
+        <v>1</v>
+      </c>
+      <c r="J95" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10">
+      <c r="B96" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" t="s">
-        <v>39</v>
-      </c>
-      <c r="B70" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C70" t="b">
-        <v>0</v>
-      </c>
-      <c r="D70" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" t="b">
-        <v>1</v>
-      </c>
-      <c r="G70" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" t="b">
-        <v>0</v>
-      </c>
-      <c r="I70" t="b">
-        <v>0</v>
-      </c>
-      <c r="J70" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2">
-      <c r="B72" t="s">
-        <v>40</v>
+      <c r="C96" s="21">
+        <v>3</v>
+      </c>
+      <c r="D96" s="2">
+        <v>3</v>
+      </c>
+      <c r="E96" s="2">
+        <v>3</v>
+      </c>
+      <c r="F96" s="2">
+        <v>2</v>
+      </c>
+      <c r="G96" s="2">
+        <v>2</v>
+      </c>
+      <c r="H96" s="2">
+        <v>1</v>
+      </c>
+      <c r="I96" s="2">
+        <v>1</v>
+      </c>
+      <c r="J96" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10">
+      <c r="B97" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="21">
+        <v>2</v>
+      </c>
+      <c r="D97" s="2">
+        <v>2</v>
+      </c>
+      <c r="E97" s="2">
+        <v>2</v>
+      </c>
+      <c r="F97" s="2">
+        <v>2</v>
+      </c>
+      <c r="G97" s="2">
+        <v>2</v>
+      </c>
+      <c r="H97" s="2">
+        <v>1</v>
+      </c>
+      <c r="I97" s="2">
+        <v>1</v>
+      </c>
+      <c r="J97" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10">
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="21">
+        <v>1</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2">
+        <v>1</v>
+      </c>
+      <c r="F98" s="2">
+        <v>1</v>
+      </c>
+      <c r="G98" s="2">
+        <v>1</v>
+      </c>
+      <c r="H98" s="2">
+        <v>1</v>
+      </c>
+      <c r="I98" s="2">
+        <v>1</v>
+      </c>
+      <c r="J98" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10">
+      <c r="B99" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" s="22">
+        <v>0</v>
+      </c>
+      <c r="D99" s="22">
+        <v>0</v>
+      </c>
+      <c r="E99" s="22">
+        <v>0</v>
+      </c>
+      <c r="F99" s="22">
+        <v>0</v>
+      </c>
+      <c r="G99" s="22">
+        <v>0</v>
+      </c>
+      <c r="H99" s="22">
+        <v>0</v>
+      </c>
+      <c r="I99" s="22">
+        <v>0</v>
+      </c>
+      <c r="J99" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +2571,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2011,39 +2612,39 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2075,12 +2676,12 @@
     </row>
     <row r="7" spans="5:5">
       <c r="E7" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B9">
         <v>1</v>

</xml_diff>

<commit_message>
updated README with RodCutting videos and solved Knapsack
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12495" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="SCS" sheetId="4" r:id="rId3"/>
     <sheet name="Coin change" sheetId="2" r:id="rId4"/>
     <sheet name="Edit Distance" sheetId="5" r:id="rId5"/>
+    <sheet name="RodCutting" sheetId="6" r:id="rId6"/>
+    <sheet name="Knapsack" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="167">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -335,6 +337,9 @@
     <t>2) Insert non-lcs characters (in their original order in strings) to the lcs found above, and return the result. So “ek” becomes “geeke” which is shortest common supersequence.</t>
   </si>
   <si>
+    <t>CoinChange</t>
+  </si>
+  <si>
     <t>dp init</t>
   </si>
   <si>
@@ -393,19 +398,143 @@
   </si>
   <si>
     <t>1 + ED("hor","r")</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>2 5 7 8 10</t>
+  </si>
+  <si>
+    <t>N=5</t>
+  </si>
+  <si>
+    <t>1,1,1,1,1</t>
+  </si>
+  <si>
+    <t>1,1,1,2</t>
+  </si>
+  <si>
+    <t>1,1,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>1,2,2</t>
+  </si>
+  <si>
+    <t>price[2]+dp[0]</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>price[3]+dp[0]</t>
+  </si>
+  <si>
+    <t>price[4]+dp[0]</t>
+  </si>
+  <si>
+    <t>dp[5]</t>
+  </si>
+  <si>
+    <t>price[1]+dp[4]</t>
+  </si>
+  <si>
+    <t>price[2]+dp[3]</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>price[3]+dp[2]</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>price[4]+dp[1]</t>
+  </si>
+  <si>
+    <t>5,0</t>
+  </si>
+  <si>
+    <t>price[5]+dp[0]</t>
+  </si>
+  <si>
+    <t>0-1 Knapsack Problem</t>
+  </si>
+  <si>
+    <t>n=5</t>
+  </si>
+  <si>
+    <t>c=15</t>
+  </si>
+  <si>
+    <t>v[i]</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>w[i]</t>
+  </si>
+  <si>
+    <t>kgs</t>
+  </si>
+  <si>
+    <t>Max value</t>
+  </si>
+  <si>
+    <t>Items (down)</t>
+  </si>
+  <si>
+    <t>Capacity =&gt;</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>v[1]=4, w[1]=12</t>
+  </si>
+  <si>
+    <t>v[2]=2, w[2]=1</t>
+  </si>
+  <si>
+    <t>v[3]=10, w[3]=4</t>
+  </si>
+  <si>
+    <t>v[4]=1, w[4]=1</t>
+  </si>
+  <si>
+    <t>v[5]=2, w[5]=2</t>
+  </si>
+  <si>
+    <t>Maximum value that can be obtained from ‘n’ items is the max of the following two values: </t>
+  </si>
+  <si>
+    <t>- Maximum value obtained by n-1 items and W weight (excluding nth item).</t>
+  </si>
+  <si>
+    <t>- Value of nth item plus maximum value obtained by n-1 items and W minus the weight of the nth item (including nth item).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +558,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9.75"/>
       <color rgb="FF263238"/>
       <name val="Consolas"/>
@@ -441,9 +584,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -456,8 +605,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +644,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -479,15 +668,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,38 +698,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -543,14 +707,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -564,24 +721,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -600,67 +743,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,13 +755,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,13 +773,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,7 +803,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,7 +845,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,43 +905,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,8 +921,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -809,6 +952,147 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -881,19 +1165,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -937,17 +1208,56 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -967,68 +1277,29 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1046,140 +1317,159 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1189,22 +1479,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1298,6 +1588,53 @@
         <a:xfrm>
           <a:off x="929005" y="770255"/>
           <a:ext cx="4342130" cy="2425700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>151765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>116205</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>46355</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1584325" y="723265"/>
+          <a:ext cx="4304030" cy="3704590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1596,19 +1933,19 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="21" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
@@ -1619,13 +1956,13 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
@@ -1650,19 +1987,19 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="22">
         <f>IF($B$8=C$7,1+D9,MAX(C9,D8))</f>
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="21">
         <f>IF($B$8=D$7,1+E9,MAX(D9,E8))</f>
         <v>2</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="21">
         <f>IF($B$8=E$7,1+F9,MAX(E9,F8))</f>
         <v>1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1670,19 +2007,19 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="21">
         <f>IF($B$9=C$7,1+D10,MAX(C10,D9))</f>
         <v>2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="21">
         <f>IF($B$9=D$7,1+E10,MAX(D10,E9))</f>
         <v>2</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="21">
         <f>IF($B$9=E$7,1+F10,MAX(E10,F9))</f>
         <v>1</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1690,19 +2027,19 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="21">
         <f>IF($B$10=C$7,1+D11,MAX(C11,D10))</f>
         <v>2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="21">
         <f>IF($B$10=D$7,1+E11,MAX(D11,E10))</f>
         <v>2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="21">
         <f>IF($B$10=E$7,1+F11,MAX(E11,F10))</f>
         <v>1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1710,19 +2047,19 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="21">
         <f>IF($B$11=C$7,1+D12,MAX(C12,D11))</f>
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="21">
         <f>IF($B$11=D$7,1+E12,MAX(D12,E11))</f>
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="21">
         <f>IF($B$11=E$7,1+F12,MAX(E12,F11))</f>
         <v>1</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1730,19 +2067,19 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="21">
         <f>IF($B$12=C$7,1+D13,MAX(C13,D12))</f>
         <v>1</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="21">
         <f>IF($B$12=D$7,1+E13,MAX(D13,E12))</f>
         <v>1</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="21">
         <f>IF($B$12=E$7,1+F13,MAX(E13,F12))</f>
         <v>1</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1750,16 +2087,16 @@
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="C13" s="21">
+        <v>0</v>
+      </c>
+      <c r="D13" s="21">
+        <v>0</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1796,7 +2133,7 @@
       <c r="I22">
         <v>7</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="J22" s="31" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1804,31 +2141,31 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="21">
         <v>10</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="21">
         <v>9</v>
       </c>
-      <c r="D23" s="2">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="21">
+        <v>2</v>
+      </c>
+      <c r="E23" s="21">
         <v>5</v>
       </c>
-      <c r="F23" s="2">
-        <v>3</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="F23" s="21">
+        <v>3</v>
+      </c>
+      <c r="G23" s="21">
         <v>7</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="21">
         <v>101</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="21">
         <v>18</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="31" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1842,7 +2179,7 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="25">
         <v>4</v>
       </c>
       <c r="E25">
@@ -1951,16 +2288,16 @@
       <c r="B41" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="2">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2">
-        <v>2</v>
-      </c>
-      <c r="F41" s="2">
+      <c r="C41" s="21">
+        <v>0</v>
+      </c>
+      <c r="D41" s="21">
+        <v>1</v>
+      </c>
+      <c r="E41" s="21">
+        <v>2</v>
+      </c>
+      <c r="F41" s="21">
         <v>3</v>
       </c>
     </row>
@@ -1968,16 +2305,16 @@
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2">
-        <v>2</v>
-      </c>
-      <c r="F42" s="2">
+      <c r="C42" s="21">
+        <v>1</v>
+      </c>
+      <c r="D42" s="21">
+        <v>1</v>
+      </c>
+      <c r="E42" s="21">
+        <v>2</v>
+      </c>
+      <c r="F42" s="21">
         <v>3</v>
       </c>
     </row>
@@ -1985,16 +2322,16 @@
       <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="2">
-        <v>2</v>
-      </c>
-      <c r="D43" s="2">
-        <v>2</v>
-      </c>
-      <c r="E43" s="2">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2">
+      <c r="C43" s="21">
+        <v>2</v>
+      </c>
+      <c r="D43" s="21">
+        <v>2</v>
+      </c>
+      <c r="E43" s="21">
+        <v>1</v>
+      </c>
+      <c r="F43" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2002,16 +2339,16 @@
       <c r="B44" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="2">
-        <v>3</v>
-      </c>
-      <c r="D44" s="2">
-        <v>2</v>
-      </c>
-      <c r="E44" s="2">
-        <v>2</v>
-      </c>
-      <c r="F44" s="2">
+      <c r="C44" s="21">
+        <v>3</v>
+      </c>
+      <c r="D44" s="21">
+        <v>2</v>
+      </c>
+      <c r="E44" s="21">
+        <v>2</v>
+      </c>
+      <c r="F44" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2019,16 +2356,16 @@
       <c r="B45" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="21">
         <v>4</v>
       </c>
-      <c r="D45" s="2">
-        <v>3</v>
-      </c>
-      <c r="E45" s="2">
-        <v>3</v>
-      </c>
-      <c r="F45" s="2">
+      <c r="D45" s="21">
+        <v>3</v>
+      </c>
+      <c r="E45" s="21">
+        <v>3</v>
+      </c>
+      <c r="F45" s="21">
         <v>2</v>
       </c>
     </row>
@@ -2036,16 +2373,16 @@
       <c r="B46" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="21">
         <v>5</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="21">
         <v>4</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="21">
         <v>4</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="22">
         <v>3</v>
       </c>
     </row>
@@ -2090,28 +2427,28 @@
       <c r="A53" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="G53" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="H53" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="10" t="s">
+      <c r="I53" s="29" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2119,7 +2456,7 @@
       <c r="A55" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="6" t="b">
+      <c r="B55" s="25" t="b">
         <v>1</v>
       </c>
       <c r="C55" t="b">
@@ -2151,7 +2488,7 @@
       <c r="B57" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="30" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2167,30 +2504,30 @@
     </row>
     <row r="66" ht="15.75"/>
     <row r="67" ht="15.75" spans="7:7">
-      <c r="G67" s="13"/>
+      <c r="G67" s="32"/>
     </row>
     <row r="68" ht="15.75" spans="6:7">
-      <c r="F68" s="14"/>
-      <c r="G68" s="15"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="34"/>
     </row>
     <row r="69" ht="15.75" spans="5:7">
-      <c r="E69" s="14"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="15"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" ht="15.75" spans="4:7">
-      <c r="D70" s="14"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="15"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" ht="15.75" spans="2:7">
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="19"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="20"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="38"/>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
@@ -2219,7 +2556,7 @@
       <c r="A74" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="25">
         <v>8</v>
       </c>
       <c r="C74">
@@ -2259,30 +2596,30 @@
     </row>
     <row r="79" ht="15.75"/>
     <row r="80" ht="15.75" spans="7:7">
-      <c r="G80" s="13"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" ht="15.75" spans="6:7">
-      <c r="F81" s="14"/>
-      <c r="G81" s="15"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="34"/>
     </row>
     <row r="82" ht="15.75" spans="5:7">
-      <c r="E82" s="14"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="15"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="34"/>
     </row>
     <row r="83" ht="15.75" spans="4:7">
-      <c r="D83" s="14"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="15"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="34"/>
     </row>
     <row r="84" ht="15.75" spans="2:7">
-      <c r="B84" s="17"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="20"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="38"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
@@ -2311,7 +2648,7 @@
       <c r="A87" t="s">
         <v>41</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="25">
         <v>13</v>
       </c>
       <c r="C87">
@@ -2376,28 +2713,28 @@
       <c r="B96" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="21">
+      <c r="C96" s="39">
         <v>4</v>
       </c>
-      <c r="D96" s="22">
-        <v>3</v>
-      </c>
-      <c r="E96" s="22">
-        <v>3</v>
-      </c>
-      <c r="F96" s="2">
-        <v>2</v>
-      </c>
-      <c r="G96" s="2">
-        <v>2</v>
-      </c>
-      <c r="H96" s="2">
-        <v>1</v>
-      </c>
-      <c r="I96" s="2">
-        <v>1</v>
-      </c>
-      <c r="J96" s="23">
+      <c r="D96" s="40">
+        <v>3</v>
+      </c>
+      <c r="E96" s="40">
+        <v>3</v>
+      </c>
+      <c r="F96" s="21">
+        <v>2</v>
+      </c>
+      <c r="G96" s="21">
+        <v>2</v>
+      </c>
+      <c r="H96" s="21">
+        <v>1</v>
+      </c>
+      <c r="I96" s="21">
+        <v>1</v>
+      </c>
+      <c r="J96" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2405,28 +2742,28 @@
       <c r="B97" t="s">
         <v>51</v>
       </c>
-      <c r="C97" s="22">
+      <c r="C97" s="40">
         <v>4</v>
       </c>
-      <c r="D97" s="22">
-        <v>3</v>
-      </c>
-      <c r="E97" s="22">
-        <v>3</v>
-      </c>
-      <c r="F97" s="2">
-        <v>2</v>
-      </c>
-      <c r="G97" s="2">
-        <v>2</v>
-      </c>
-      <c r="H97" s="2">
-        <v>1</v>
-      </c>
-      <c r="I97" s="2">
-        <v>1</v>
-      </c>
-      <c r="J97" s="23">
+      <c r="D97" s="40">
+        <v>3</v>
+      </c>
+      <c r="E97" s="40">
+        <v>3</v>
+      </c>
+      <c r="F97" s="21">
+        <v>2</v>
+      </c>
+      <c r="G97" s="21">
+        <v>2</v>
+      </c>
+      <c r="H97" s="21">
+        <v>1</v>
+      </c>
+      <c r="I97" s="21">
+        <v>1</v>
+      </c>
+      <c r="J97" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2434,28 +2771,28 @@
       <c r="B98" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="22">
+      <c r="C98" s="40">
         <v>4</v>
       </c>
-      <c r="D98" s="22">
-        <v>3</v>
-      </c>
-      <c r="E98" s="22">
-        <v>3</v>
-      </c>
-      <c r="F98" s="2">
-        <v>2</v>
-      </c>
-      <c r="G98" s="2">
-        <v>2</v>
-      </c>
-      <c r="H98" s="2">
-        <v>1</v>
-      </c>
-      <c r="I98" s="2">
-        <v>1</v>
-      </c>
-      <c r="J98" s="23">
+      <c r="D98" s="40">
+        <v>3</v>
+      </c>
+      <c r="E98" s="40">
+        <v>3</v>
+      </c>
+      <c r="F98" s="21">
+        <v>2</v>
+      </c>
+      <c r="G98" s="21">
+        <v>2</v>
+      </c>
+      <c r="H98" s="21">
+        <v>1</v>
+      </c>
+      <c r="I98" s="21">
+        <v>1</v>
+      </c>
+      <c r="J98" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2463,28 +2800,28 @@
       <c r="B99" t="s">
         <v>35</v>
       </c>
-      <c r="C99" s="2">
-        <v>3</v>
-      </c>
-      <c r="D99" s="2">
-        <v>3</v>
-      </c>
-      <c r="E99" s="2">
-        <v>3</v>
-      </c>
-      <c r="F99" s="2">
-        <v>2</v>
-      </c>
-      <c r="G99" s="2">
-        <v>2</v>
-      </c>
-      <c r="H99" s="2">
-        <v>1</v>
-      </c>
-      <c r="I99" s="2">
-        <v>1</v>
-      </c>
-      <c r="J99" s="23">
+      <c r="C99" s="21">
+        <v>3</v>
+      </c>
+      <c r="D99" s="21">
+        <v>3</v>
+      </c>
+      <c r="E99" s="21">
+        <v>3</v>
+      </c>
+      <c r="F99" s="21">
+        <v>2</v>
+      </c>
+      <c r="G99" s="21">
+        <v>2</v>
+      </c>
+      <c r="H99" s="21">
+        <v>1</v>
+      </c>
+      <c r="I99" s="21">
+        <v>1</v>
+      </c>
+      <c r="J99" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2492,28 +2829,28 @@
       <c r="B100" t="s">
         <v>2</v>
       </c>
-      <c r="C100" s="2">
-        <v>2</v>
-      </c>
-      <c r="D100" s="2">
-        <v>2</v>
-      </c>
-      <c r="E100" s="2">
-        <v>2</v>
-      </c>
-      <c r="F100" s="2">
-        <v>2</v>
-      </c>
-      <c r="G100" s="2">
-        <v>2</v>
-      </c>
-      <c r="H100" s="2">
-        <v>1</v>
-      </c>
-      <c r="I100" s="2">
-        <v>1</v>
-      </c>
-      <c r="J100" s="23">
+      <c r="C100" s="21">
+        <v>2</v>
+      </c>
+      <c r="D100" s="21">
+        <v>2</v>
+      </c>
+      <c r="E100" s="21">
+        <v>2</v>
+      </c>
+      <c r="F100" s="21">
+        <v>2</v>
+      </c>
+      <c r="G100" s="21">
+        <v>2</v>
+      </c>
+      <c r="H100" s="21">
+        <v>1</v>
+      </c>
+      <c r="I100" s="21">
+        <v>1</v>
+      </c>
+      <c r="J100" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2521,28 +2858,28 @@
       <c r="B101" t="s">
         <v>3</v>
       </c>
-      <c r="C101" s="2">
-        <v>1</v>
-      </c>
-      <c r="D101" s="2">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2">
-        <v>1</v>
-      </c>
-      <c r="F101" s="2">
-        <v>1</v>
-      </c>
-      <c r="G101" s="2">
-        <v>1</v>
-      </c>
-      <c r="H101" s="2">
-        <v>1</v>
-      </c>
-      <c r="I101" s="2">
-        <v>1</v>
-      </c>
-      <c r="J101" s="23">
+      <c r="C101" s="21">
+        <v>1</v>
+      </c>
+      <c r="D101" s="21">
+        <v>1</v>
+      </c>
+      <c r="E101" s="21">
+        <v>1</v>
+      </c>
+      <c r="F101" s="21">
+        <v>1</v>
+      </c>
+      <c r="G101" s="21">
+        <v>1</v>
+      </c>
+      <c r="H101" s="21">
+        <v>1</v>
+      </c>
+      <c r="I101" s="21">
+        <v>1</v>
+      </c>
+      <c r="J101" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2550,28 +2887,28 @@
       <c r="B102" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="23">
-        <v>0</v>
-      </c>
-      <c r="D102" s="23">
-        <v>0</v>
-      </c>
-      <c r="E102" s="23">
-        <v>0</v>
-      </c>
-      <c r="F102" s="23">
-        <v>0</v>
-      </c>
-      <c r="G102" s="23">
-        <v>0</v>
-      </c>
-      <c r="H102" s="23">
-        <v>0</v>
-      </c>
-      <c r="I102" s="23">
-        <v>0</v>
-      </c>
-      <c r="J102" s="23">
+      <c r="C102" s="41">
+        <v>0</v>
+      </c>
+      <c r="D102" s="41">
+        <v>0</v>
+      </c>
+      <c r="E102" s="41">
+        <v>0</v>
+      </c>
+      <c r="F102" s="41">
+        <v>0</v>
+      </c>
+      <c r="G102" s="41">
+        <v>0</v>
+      </c>
+      <c r="H102" s="41">
+        <v>0</v>
+      </c>
+      <c r="I102" s="41">
+        <v>0</v>
+      </c>
+      <c r="J102" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2591,34 +2928,34 @@
       </c>
     </row>
     <row r="111" spans="7:7">
-      <c r="G111" s="24"/>
+      <c r="G111" s="42"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>57</v>
       </c>
-      <c r="B112" s="22">
-        <v>1</v>
-      </c>
-      <c r="C112" s="2">
-        <v>2</v>
-      </c>
-      <c r="D112" s="2">
-        <v>3</v>
-      </c>
-      <c r="E112" s="2">
+      <c r="B112" s="40">
+        <v>1</v>
+      </c>
+      <c r="C112" s="21">
+        <v>2</v>
+      </c>
+      <c r="D112" s="21">
+        <v>3</v>
+      </c>
+      <c r="E112" s="21">
         <v>4</v>
       </c>
-      <c r="F112" s="2">
+      <c r="F112" s="21">
         <v>5</v>
       </c>
-      <c r="G112" s="2">
+      <c r="G112" s="21">
         <v>6</v>
       </c>
-      <c r="H112" s="2">
+      <c r="H112" s="21">
         <v>7</v>
       </c>
-      <c r="I112" s="2">
+      <c r="I112" s="21">
         <v>8</v>
       </c>
     </row>
@@ -2626,28 +2963,28 @@
       <c r="A113" t="s">
         <v>58</v>
       </c>
-      <c r="B113" s="2">
-        <v>1</v>
-      </c>
-      <c r="C113" s="2">
+      <c r="B113" s="21">
+        <v>1</v>
+      </c>
+      <c r="C113" s="21">
         <v>5</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D113" s="21">
         <v>8</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113" s="21">
         <v>9</v>
       </c>
-      <c r="F113" s="2">
+      <c r="F113" s="21">
         <v>10</v>
       </c>
-      <c r="G113" s="2">
+      <c r="G113" s="21">
         <v>17</v>
       </c>
-      <c r="H113" s="2">
+      <c r="H113" s="21">
         <v>17</v>
       </c>
-      <c r="I113" s="2">
+      <c r="I113" s="21">
         <v>20</v>
       </c>
     </row>
@@ -2692,7 +3029,7 @@
       <c r="A118" t="s">
         <v>60</v>
       </c>
-      <c r="B118" s="22">
+      <c r="B118" s="40">
         <v>1</v>
       </c>
       <c r="D118" t="s">
@@ -2701,7 +3038,7 @@
       <c r="E118" t="s">
         <v>62</v>
       </c>
-      <c r="F118" s="6">
+      <c r="F118" s="25">
         <v>1</v>
       </c>
     </row>
@@ -2714,10 +3051,10 @@
       <c r="A121" t="s">
         <v>64</v>
       </c>
-      <c r="B121" s="22">
-        <v>1</v>
-      </c>
-      <c r="C121" s="2">
+      <c r="B121" s="40">
+        <v>1</v>
+      </c>
+      <c r="C121" s="21">
         <v>2</v>
       </c>
       <c r="E121" t="s">
@@ -2729,7 +3066,7 @@
       <c r="G121">
         <v>2</v>
       </c>
-      <c r="H121" s="6">
+      <c r="H121" s="25">
         <v>5</v>
       </c>
     </row>
@@ -2754,13 +3091,13 @@
       <c r="A124" t="s">
         <v>70</v>
       </c>
-      <c r="B124" s="22">
-        <v>1</v>
-      </c>
-      <c r="C124" s="2">
-        <v>2</v>
-      </c>
-      <c r="D124" s="2">
+      <c r="B124" s="40">
+        <v>1</v>
+      </c>
+      <c r="C124" s="21">
+        <v>2</v>
+      </c>
+      <c r="D124" s="21">
         <v>3</v>
       </c>
       <c r="F124" t="s">
@@ -2772,7 +3109,7 @@
       <c r="H124">
         <v>6</v>
       </c>
-      <c r="I124" s="6">
+      <c r="I124" s="25">
         <v>8</v>
       </c>
     </row>
@@ -2811,16 +3148,16 @@
       <c r="A128" t="s">
         <v>78</v>
       </c>
-      <c r="B128" s="22">
-        <v>1</v>
-      </c>
-      <c r="C128" s="2">
-        <v>2</v>
-      </c>
-      <c r="D128" s="2">
-        <v>3</v>
-      </c>
-      <c r="E128" s="2">
+      <c r="B128" s="40">
+        <v>1</v>
+      </c>
+      <c r="C128" s="21">
+        <v>2</v>
+      </c>
+      <c r="D128" s="21">
+        <v>3</v>
+      </c>
+      <c r="E128" s="21">
         <v>4</v>
       </c>
       <c r="G128" t="s">
@@ -2832,7 +3169,7 @@
       <c r="I128">
         <v>9</v>
       </c>
-      <c r="J128" s="6">
+      <c r="J128" s="25">
         <v>10</v>
       </c>
     </row>
@@ -2948,49 +3285,49 @@
       <c r="A2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="9">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9">
+      <c r="B2" s="28">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28">
+        <v>1</v>
+      </c>
+      <c r="D2" s="28">
         <f t="shared" ref="D2:M2" si="0">C2+B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="28">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="28">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="28">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="28">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="28">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="28">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="28">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="28">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="28">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
@@ -3037,16 +3374,16 @@
       <c r="A8" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3054,13 +3391,13 @@
       <c r="A9" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3068,10 +3405,10 @@
       <c r="A11" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3082,10 +3419,10 @@
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
@@ -3106,13 +3443,13 @@
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F19" t="s">
@@ -3120,16 +3457,16 @@
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="7">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="B20" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="26">
+        <v>2</v>
+      </c>
+      <c r="D20" s="23">
+        <v>2</v>
+      </c>
+      <c r="E20" s="21">
         <v>1</v>
       </c>
       <c r="F20">
@@ -3137,16 +3474,16 @@
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4">
+      <c r="B21" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="23">
         <v>1</v>
       </c>
       <c r="F21">
@@ -3157,16 +3494,16 @@
       <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="C22" s="21">
+        <v>1</v>
+      </c>
+      <c r="D22" s="21">
+        <v>1</v>
+      </c>
+      <c r="E22" s="21">
+        <v>0</v>
+      </c>
+      <c r="F22" s="27">
         <v>0</v>
       </c>
     </row>
@@ -3174,16 +3511,16 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
+      <c r="C23" s="21">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21">
+        <v>0</v>
+      </c>
+      <c r="E23" s="21">
+        <v>0</v>
+      </c>
+      <c r="F23" s="27">
         <v>0</v>
       </c>
     </row>
@@ -3200,7 +3537,7 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="27">
         <v>0</v>
       </c>
     </row>
@@ -3238,16 +3575,16 @@
       <c r="A37" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="23" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3255,13 +3592,13 @@
       <c r="A38" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3269,10 +3606,10 @@
       <c r="A40" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="21" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3286,10 +3623,10 @@
       <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="21" t="s">
         <v>102</v>
       </c>
       <c r="F41" t="s">
@@ -3307,10 +3644,10 @@
       </c>
     </row>
     <row r="47" spans="3:6">
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="25" t="s">
         <v>102</v>
       </c>
       <c r="E47" t="s">
@@ -3321,16 +3658,16 @@
       </c>
     </row>
     <row r="48" spans="2:6">
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="7">
-        <v>2</v>
-      </c>
-      <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2">
+      <c r="C48" s="26">
+        <v>2</v>
+      </c>
+      <c r="D48" s="21">
+        <v>1</v>
+      </c>
+      <c r="E48" s="21">
         <v>1</v>
       </c>
       <c r="F48">
@@ -3338,16 +3675,16 @@
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="4">
-        <v>2</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2">
+      <c r="C49" s="23">
+        <v>2</v>
+      </c>
+      <c r="D49" s="21">
+        <v>1</v>
+      </c>
+      <c r="E49" s="21">
         <v>1</v>
       </c>
       <c r="F49">
@@ -3355,16 +3692,16 @@
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="2">
-        <v>2</v>
-      </c>
-      <c r="D50" s="4">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2">
+      <c r="C50" s="21">
+        <v>2</v>
+      </c>
+      <c r="D50" s="23">
+        <v>1</v>
+      </c>
+      <c r="E50" s="21">
         <v>1</v>
       </c>
       <c r="F50">
@@ -3372,16 +3709,16 @@
       </c>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
-      <c r="D51" s="4">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2">
+      <c r="C51" s="21">
+        <v>1</v>
+      </c>
+      <c r="D51" s="23">
+        <v>1</v>
+      </c>
+      <c r="E51" s="21">
         <v>0</v>
       </c>
       <c r="F51">
@@ -3398,7 +3735,7 @@
       <c r="D52">
         <v>0</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="27">
         <v>0</v>
       </c>
       <c r="F52">
@@ -3434,7 +3771,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3448,172 +3785,180 @@
     <col min="7" max="10" width="36.352380952381" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>8</v>
-      </c>
-      <c r="K2">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="L3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>106</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J4" t="s">
-        <v>114</v>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" t="s">
         <v>115</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="5:5">
-      <c r="E7" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5">
+      <c r="E8" t="s">
         <v>117</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>118</v>
+      </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12">
         <v>5</v>
       </c>
     </row>
@@ -3628,7 +3973,7 @@
   <sheetPr/>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3641,92 +3986,92 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="21" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="3:6">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -3747,16 +4092,16 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="C18" s="21">
+        <v>0</v>
+      </c>
+      <c r="D18" s="21">
+        <v>1</v>
+      </c>
+      <c r="E18" s="21">
+        <v>2</v>
+      </c>
+      <c r="F18" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3764,16 +4109,16 @@
       <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="C19" s="21">
+        <v>1</v>
+      </c>
+      <c r="D19" s="21">
+        <v>1</v>
+      </c>
+      <c r="E19" s="21">
+        <v>2</v>
+      </c>
+      <c r="F19" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3781,16 +4126,16 @@
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="2">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="21">
+        <v>2</v>
+      </c>
+      <c r="D20" s="21">
+        <v>2</v>
+      </c>
+      <c r="E20" s="21">
+        <v>1</v>
+      </c>
+      <c r="F20" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3798,16 +4143,16 @@
       <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="2">
-        <v>3</v>
-      </c>
-      <c r="D21" s="2">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="C21" s="21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3815,16 +4160,16 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="21">
         <v>4</v>
       </c>
-      <c r="D22" s="2">
-        <v>3</v>
-      </c>
-      <c r="E22" s="2">
-        <v>3</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="D22" s="21">
+        <v>3</v>
+      </c>
+      <c r="E22" s="21">
+        <v>3</v>
+      </c>
+      <c r="F22" s="21">
         <v>2</v>
       </c>
     </row>
@@ -3832,16 +4177,16 @@
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="21">
         <v>5</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="21">
         <v>4</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="21">
         <v>4</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="22">
         <v>3</v>
       </c>
     </row>
@@ -3849,4 +4194,940 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="15.047619047619" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.8095238095238" customWidth="1"/>
+    <col min="9" max="9" width="18.0952380952381" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1"/>
+    <row r="3" ht="15.75" spans="2:12">
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="L3" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="2:12">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="19">
+        <v>2</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="2:9">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="I5" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="2:9">
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9">
+        <v>3</v>
+      </c>
+      <c r="I6" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="2:9">
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9">
+        <v>4</v>
+      </c>
+      <c r="I7" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="2:9">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13">
+        <v>5</v>
+      </c>
+      <c r="I8" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1"/>
+    <row r="10" customFormat="1" ht="15.75" spans="2:2">
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="2:9">
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="16"/>
+      <c r="H11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="8:9">
+      <c r="H12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="8:9">
+      <c r="H13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I13" s="19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="8:9">
+      <c r="H14" t="s">
+        <v>132</v>
+      </c>
+      <c r="I14" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="8:9">
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="8:9">
+      <c r="H16" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9">
+      <c r="H17" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1"/>
+    <row r="19" customFormat="1"/>
+    <row r="20" customFormat="1" spans="1:2">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="1" ht="15.75"/>
+    <row r="22" customFormat="1" ht="15.75" spans="1:5">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="18">
+        <v>1</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" ht="15.75"/>
+    <row r="24" customFormat="1" ht="15.75" spans="1:7">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="16">
+        <v>2</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13">
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="17">
+        <v>5</v>
+      </c>
+      <c r="L25" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" spans="12:13">
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:13">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="19">
+        <v>7</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13">
+      <c r="F28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="19">
+        <v>7</v>
+      </c>
+      <c r="L28">
+        <v>3</v>
+      </c>
+      <c r="M28" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="6:13">
+      <c r="F29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" s="17">
+        <v>7</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="12:13">
+      <c r="L30">
+        <v>5</v>
+      </c>
+      <c r="M30" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="1" ht="15.75"/>
+    <row r="32" ht="15.75" spans="1:9">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9">
+      <c r="G33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9">
+      <c r="G34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" t="s">
+        <v>85</v>
+      </c>
+      <c r="I34" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9">
+      <c r="G35" t="s">
+        <v>86</v>
+      </c>
+      <c r="H35" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="1"/>
+    <row r="37" customFormat="1" ht="15.75"/>
+    <row r="38" ht="15.75" spans="1:10">
+      <c r="A38" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="16">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>132</v>
+      </c>
+      <c r="I38" t="s">
+        <v>140</v>
+      </c>
+      <c r="J38" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="8:10">
+      <c r="H39" t="s">
+        <v>133</v>
+      </c>
+      <c r="I39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J39" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="8:10">
+      <c r="H40" t="s">
+        <v>142</v>
+      </c>
+      <c r="I40" t="s">
+        <v>143</v>
+      </c>
+      <c r="J40" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="8:10">
+      <c r="H41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I41" t="s">
+        <v>145</v>
+      </c>
+      <c r="J41" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="8:10">
+      <c r="H42" t="s">
+        <v>146</v>
+      </c>
+      <c r="I42" t="s">
+        <v>147</v>
+      </c>
+      <c r="J42" s="19">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="12.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="12:12">
+      <c r="L11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="12:12">
+      <c r="L12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="12:17">
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="12:18">
+      <c r="L15" t="s">
+        <v>151</v>
+      </c>
+      <c r="M15" s="3">
+        <v>4</v>
+      </c>
+      <c r="N15" s="2">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2">
+        <v>10</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>2</v>
+      </c>
+      <c r="R15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="12:18">
+      <c r="L16" t="s">
+        <v>153</v>
+      </c>
+      <c r="M16" s="3">
+        <v>12</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2">
+        <v>4</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>2</v>
+      </c>
+      <c r="R16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="12:13">
+      <c r="L19" t="s">
+        <v>155</v>
+      </c>
+      <c r="M19" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <v>6</v>
+      </c>
+      <c r="J28">
+        <v>7</v>
+      </c>
+      <c r="K28">
+        <v>8</v>
+      </c>
+      <c r="L28">
+        <v>9</v>
+      </c>
+      <c r="M28">
+        <v>10</v>
+      </c>
+      <c r="N28">
+        <v>11</v>
+      </c>
+      <c r="O28">
+        <v>12</v>
+      </c>
+      <c r="P28">
+        <v>13</v>
+      </c>
+      <c r="Q28">
+        <v>14</v>
+      </c>
+      <c r="R28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+      <c r="N30" s="3">
+        <v>0</v>
+      </c>
+      <c r="O30" s="4">
+        <v>4</v>
+      </c>
+      <c r="P30" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>4</v>
+      </c>
+      <c r="R30" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2</v>
+      </c>
+      <c r="F31" s="3">
+        <v>2</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3">
+        <v>2</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2</v>
+      </c>
+      <c r="L31" s="3">
+        <v>2</v>
+      </c>
+      <c r="M31" s="3">
+        <v>2</v>
+      </c>
+      <c r="N31" s="3">
+        <v>2</v>
+      </c>
+      <c r="O31" s="3">
+        <v>4</v>
+      </c>
+      <c r="P31" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>6</v>
+      </c>
+      <c r="R31" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3">
+        <v>10</v>
+      </c>
+      <c r="H32" s="4">
+        <v>12</v>
+      </c>
+      <c r="I32" s="3">
+        <v>12</v>
+      </c>
+      <c r="J32" s="3">
+        <v>12</v>
+      </c>
+      <c r="K32" s="3">
+        <v>12</v>
+      </c>
+      <c r="L32" s="3">
+        <v>12</v>
+      </c>
+      <c r="M32" s="3">
+        <v>12</v>
+      </c>
+      <c r="N32" s="3">
+        <v>12</v>
+      </c>
+      <c r="O32" s="2">
+        <v>12</v>
+      </c>
+      <c r="P32" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>12</v>
+      </c>
+      <c r="R32" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2</v>
+      </c>
+      <c r="F33" s="3">
+        <v>2</v>
+      </c>
+      <c r="G33" s="3">
+        <v>10</v>
+      </c>
+      <c r="H33" s="3">
+        <v>12</v>
+      </c>
+      <c r="I33" s="4">
+        <v>13</v>
+      </c>
+      <c r="J33" s="3">
+        <v>13</v>
+      </c>
+      <c r="K33" s="3">
+        <v>13</v>
+      </c>
+      <c r="L33" s="3">
+        <v>13</v>
+      </c>
+      <c r="M33" s="3">
+        <v>13</v>
+      </c>
+      <c r="N33" s="3">
+        <v>13</v>
+      </c>
+      <c r="O33" s="3">
+        <v>13</v>
+      </c>
+      <c r="P33" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>13</v>
+      </c>
+      <c r="R33" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>4</v>
+      </c>
+      <c r="G34" s="3">
+        <v>10</v>
+      </c>
+      <c r="H34" s="3">
+        <v>12</v>
+      </c>
+      <c r="I34" s="3">
+        <v>13</v>
+      </c>
+      <c r="J34" s="3">
+        <v>14</v>
+      </c>
+      <c r="K34" s="4">
+        <v>15</v>
+      </c>
+      <c r="L34" s="3">
+        <v>15</v>
+      </c>
+      <c r="M34" s="3">
+        <v>15</v>
+      </c>
+      <c r="N34" s="3">
+        <v>15</v>
+      </c>
+      <c r="O34" s="3">
+        <v>15</v>
+      </c>
+      <c r="P34" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>15</v>
+      </c>
+      <c r="R34" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated youtube link for Knapsack
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27428" windowHeight="11734"/>
+    <workbookView windowWidth="28800" windowHeight="12495" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -543,10 +543,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="26">
@@ -599,19 +599,19 @@
       <charset val="134"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -629,84 +629,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -722,7 +647,89 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -730,14 +737,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -758,7 +758,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,31 +794,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,31 +896,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,79 +914,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,13 +932,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,9 +1216,50 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1241,23 +1282,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1265,8 +1291,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1285,42 +1311,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1332,109 +1332,109 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1443,29 +1443,30 @@
     <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1484,7 +1485,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1506,8 +1506,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1600,8 +1598,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="963930" y="747395"/>
-          <a:ext cx="4586605" cy="2357120"/>
+          <a:off x="929005" y="770255"/>
+          <a:ext cx="4342130" cy="2425700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1647,8 +1645,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647190" y="706120"/>
-          <a:ext cx="4572000" cy="3590290"/>
+          <a:off x="1584325" y="723265"/>
+          <a:ext cx="4304030" cy="3704590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1924,18 +1922,18 @@
   <sheetPr/>
   <dimension ref="A1:J148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.009009009009" customWidth="1"/>
-    <col min="3" max="3" width="8.52252252252252" customWidth="1"/>
-    <col min="4" max="4" width="15.3693693693694" customWidth="1"/>
-    <col min="5" max="5" width="12.7027027027027" customWidth="1"/>
-    <col min="6" max="7" width="12.3153153153153" customWidth="1"/>
-    <col min="8" max="8" width="13.1261261261261" customWidth="1"/>
+    <col min="2" max="2" width="23.0095238095238" customWidth="1"/>
+    <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
+    <col min="4" max="4" width="15.3714285714286" customWidth="1"/>
+    <col min="5" max="5" width="12.7047619047619" customWidth="1"/>
+    <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
+    <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -1947,19 +1945,19 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
@@ -1970,13 +1968,13 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
@@ -2001,19 +1999,19 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f>IF($B$8=C$7,1+D9,MAX(C9,D8))</f>
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f>IF($B$8=D$7,1+E9,MAX(D9,E8))</f>
         <v>2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f>IF($B$8=E$7,1+F9,MAX(E9,F8))</f>
         <v>1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2021,19 +2019,19 @@
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f>IF($B$9=C$7,1+D10,MAX(C10,D9))</f>
         <v>2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f>IF($B$9=D$7,1+E10,MAX(D10,E9))</f>
         <v>2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f>IF($B$9=E$7,1+F10,MAX(E10,F9))</f>
         <v>1</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2041,19 +2039,19 @@
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f>IF($B$10=C$7,1+D11,MAX(C11,D10))</f>
         <v>2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f>IF($B$10=D$7,1+E11,MAX(D11,E10))</f>
         <v>2</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f>IF($B$10=E$7,1+F11,MAX(E11,F10))</f>
         <v>1</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2061,19 +2059,19 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f>IF($B$11=C$7,1+D12,MAX(C12,D11))</f>
         <v>1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <f>IF($B$11=D$7,1+E12,MAX(D12,E11))</f>
         <v>1</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f>IF($B$11=E$7,1+F12,MAX(E12,F11))</f>
         <v>1</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2081,19 +2079,19 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f>IF($B$12=C$7,1+D13,MAX(C13,D12))</f>
         <v>1</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f>IF($B$12=D$7,1+E13,MAX(D13,E12))</f>
         <v>1</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f>IF($B$12=E$7,1+F13,MAX(E13,F12))</f>
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2101,16 +2099,16 @@
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2155,28 +2153,28 @@
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>10</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>9</v>
       </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
         <v>5</v>
       </c>
-      <c r="F23" s="3">
-        <v>3</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="F23" s="2">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2">
         <v>7</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>101</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>18</v>
       </c>
       <c r="J23" s="28" t="s">
@@ -2193,7 +2191,7 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="23">
         <v>4</v>
       </c>
       <c r="E25">
@@ -2302,16 +2300,16 @@
       <c r="B41" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="3">
-        <v>0</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3">
-        <v>2</v>
-      </c>
-      <c r="F41" s="3">
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
         <v>3</v>
       </c>
     </row>
@@ -2319,16 +2317,16 @@
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="3">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3">
-        <v>1</v>
-      </c>
-      <c r="E42" s="3">
-        <v>2</v>
-      </c>
-      <c r="F42" s="3">
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>2</v>
+      </c>
+      <c r="F42" s="2">
         <v>3</v>
       </c>
     </row>
@@ -2336,16 +2334,16 @@
       <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="3">
-        <v>2</v>
-      </c>
-      <c r="D43" s="3">
-        <v>2</v>
-      </c>
-      <c r="E43" s="3">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3">
+      <c r="C43" s="2">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1</v>
+      </c>
+      <c r="F43" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2353,16 +2351,16 @@
       <c r="B44" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="3">
-        <v>3</v>
-      </c>
-      <c r="D44" s="3">
-        <v>2</v>
-      </c>
-      <c r="E44" s="3">
-        <v>2</v>
-      </c>
-      <c r="F44" s="3">
+      <c r="C44" s="2">
+        <v>3</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2370,16 +2368,16 @@
       <c r="B45" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>4</v>
       </c>
-      <c r="D45" s="3">
-        <v>3</v>
-      </c>
-      <c r="E45" s="3">
-        <v>3</v>
-      </c>
-      <c r="F45" s="3">
+      <c r="D45" s="2">
+        <v>3</v>
+      </c>
+      <c r="E45" s="2">
+        <v>3</v>
+      </c>
+      <c r="F45" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2387,16 +2385,16 @@
       <c r="B46" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>5</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>4</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>4</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="3">
         <v>3</v>
       </c>
     </row>
@@ -2470,7 +2468,7 @@
       <c r="A55" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="22" t="b">
+      <c r="B55" s="23" t="b">
         <v>1</v>
       </c>
       <c r="C55" t="b">
@@ -2516,28 +2514,28 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" ht="15.3"/>
-    <row r="67" ht="15.3" spans="7:7">
+    <row r="66" ht="15.75"/>
+    <row r="67" ht="15.75" spans="7:7">
       <c r="G67" s="29"/>
     </row>
-    <row r="68" ht="15.3" spans="6:7">
+    <row r="68" ht="15.75" spans="6:7">
       <c r="F68" s="30"/>
       <c r="G68" s="31"/>
     </row>
-    <row r="69" ht="15.3" spans="5:7">
+    <row r="69" ht="15.75" spans="5:7">
       <c r="E69" s="30"/>
       <c r="F69" s="32"/>
       <c r="G69" s="31"/>
     </row>
-    <row r="70" ht="15.3" spans="4:7">
+    <row r="70" ht="15.75" spans="4:7">
       <c r="D70" s="30"/>
       <c r="E70" s="32"/>
       <c r="F70" s="32"/>
       <c r="G70" s="31"/>
     </row>
-    <row r="71" ht="15.3" spans="2:7">
+    <row r="71" ht="15.75" spans="2:7">
       <c r="B71" s="33"/>
-      <c r="C71" s="11"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="34"/>
       <c r="E71" s="34"/>
       <c r="F71" s="34"/>
@@ -2570,7 +2568,7 @@
       <c r="A74" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="22">
+      <c r="B74" s="23">
         <v>8</v>
       </c>
       <c r="C74">
@@ -2608,28 +2606,28 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" ht="15.3"/>
-    <row r="80" ht="15.3" spans="7:7">
+    <row r="79" ht="15.75"/>
+    <row r="80" ht="15.75" spans="7:7">
       <c r="G80" s="29"/>
     </row>
-    <row r="81" ht="15.3" spans="6:7">
+    <row r="81" ht="15.75" spans="6:7">
       <c r="F81" s="30"/>
       <c r="G81" s="31"/>
     </row>
-    <row r="82" ht="15.3" spans="5:7">
+    <row r="82" ht="15.75" spans="5:7">
       <c r="E82" s="30"/>
       <c r="F82" s="32"/>
       <c r="G82" s="31"/>
     </row>
-    <row r="83" ht="15.3" spans="4:7">
+    <row r="83" ht="15.75" spans="4:7">
       <c r="D83" s="30"/>
       <c r="E83" s="32"/>
       <c r="F83" s="32"/>
       <c r="G83" s="31"/>
     </row>
-    <row r="84" ht="15.3" spans="2:7">
+    <row r="84" ht="15.75" spans="2:7">
       <c r="B84" s="33"/>
-      <c r="C84" s="11"/>
+      <c r="C84" s="12"/>
       <c r="D84" s="34"/>
       <c r="E84" s="34"/>
       <c r="F84" s="34"/>
@@ -2662,7 +2660,7 @@
       <c r="A87" t="s">
         <v>41</v>
       </c>
-      <c r="B87" s="22">
+      <c r="B87" s="23">
         <v>13</v>
       </c>
       <c r="C87">
@@ -2736,16 +2734,16 @@
       <c r="E96" s="37">
         <v>3</v>
       </c>
-      <c r="F96" s="3">
-        <v>2</v>
-      </c>
-      <c r="G96" s="3">
-        <v>2</v>
-      </c>
-      <c r="H96" s="3">
-        <v>1</v>
-      </c>
-      <c r="I96" s="3">
+      <c r="F96" s="2">
+        <v>2</v>
+      </c>
+      <c r="G96" s="2">
+        <v>2</v>
+      </c>
+      <c r="H96" s="2">
+        <v>1</v>
+      </c>
+      <c r="I96" s="2">
         <v>1</v>
       </c>
       <c r="J96" s="38">
@@ -2765,16 +2763,16 @@
       <c r="E97" s="37">
         <v>3</v>
       </c>
-      <c r="F97" s="3">
-        <v>2</v>
-      </c>
-      <c r="G97" s="3">
-        <v>2</v>
-      </c>
-      <c r="H97" s="3">
-        <v>1</v>
-      </c>
-      <c r="I97" s="3">
+      <c r="F97" s="2">
+        <v>2</v>
+      </c>
+      <c r="G97" s="2">
+        <v>2</v>
+      </c>
+      <c r="H97" s="2">
+        <v>1</v>
+      </c>
+      <c r="I97" s="2">
         <v>1</v>
       </c>
       <c r="J97" s="38">
@@ -2794,16 +2792,16 @@
       <c r="E98" s="37">
         <v>3</v>
       </c>
-      <c r="F98" s="3">
-        <v>2</v>
-      </c>
-      <c r="G98" s="3">
-        <v>2</v>
-      </c>
-      <c r="H98" s="3">
-        <v>1</v>
-      </c>
-      <c r="I98" s="3">
+      <c r="F98" s="2">
+        <v>2</v>
+      </c>
+      <c r="G98" s="2">
+        <v>2</v>
+      </c>
+      <c r="H98" s="2">
+        <v>1</v>
+      </c>
+      <c r="I98" s="2">
         <v>1</v>
       </c>
       <c r="J98" s="38">
@@ -2814,25 +2812,25 @@
       <c r="B99" t="s">
         <v>35</v>
       </c>
-      <c r="C99" s="3">
-        <v>3</v>
-      </c>
-      <c r="D99" s="3">
-        <v>3</v>
-      </c>
-      <c r="E99" s="3">
-        <v>3</v>
-      </c>
-      <c r="F99" s="3">
-        <v>2</v>
-      </c>
-      <c r="G99" s="3">
-        <v>2</v>
-      </c>
-      <c r="H99" s="3">
-        <v>1</v>
-      </c>
-      <c r="I99" s="3">
+      <c r="C99" s="2">
+        <v>3</v>
+      </c>
+      <c r="D99" s="2">
+        <v>3</v>
+      </c>
+      <c r="E99" s="2">
+        <v>3</v>
+      </c>
+      <c r="F99" s="2">
+        <v>2</v>
+      </c>
+      <c r="G99" s="2">
+        <v>2</v>
+      </c>
+      <c r="H99" s="2">
+        <v>1</v>
+      </c>
+      <c r="I99" s="2">
         <v>1</v>
       </c>
       <c r="J99" s="38">
@@ -2843,25 +2841,25 @@
       <c r="B100" t="s">
         <v>2</v>
       </c>
-      <c r="C100" s="3">
-        <v>2</v>
-      </c>
-      <c r="D100" s="3">
-        <v>2</v>
-      </c>
-      <c r="E100" s="3">
-        <v>2</v>
-      </c>
-      <c r="F100" s="3">
-        <v>2</v>
-      </c>
-      <c r="G100" s="3">
-        <v>2</v>
-      </c>
-      <c r="H100" s="3">
-        <v>1</v>
-      </c>
-      <c r="I100" s="3">
+      <c r="C100" s="2">
+        <v>2</v>
+      </c>
+      <c r="D100" s="2">
+        <v>2</v>
+      </c>
+      <c r="E100" s="2">
+        <v>2</v>
+      </c>
+      <c r="F100" s="2">
+        <v>2</v>
+      </c>
+      <c r="G100" s="2">
+        <v>2</v>
+      </c>
+      <c r="H100" s="2">
+        <v>1</v>
+      </c>
+      <c r="I100" s="2">
         <v>1</v>
       </c>
       <c r="J100" s="38">
@@ -2872,25 +2870,25 @@
       <c r="B101" t="s">
         <v>3</v>
       </c>
-      <c r="C101" s="3">
-        <v>1</v>
-      </c>
-      <c r="D101" s="3">
-        <v>1</v>
-      </c>
-      <c r="E101" s="3">
-        <v>1</v>
-      </c>
-      <c r="F101" s="3">
-        <v>1</v>
-      </c>
-      <c r="G101" s="3">
-        <v>1</v>
-      </c>
-      <c r="H101" s="3">
-        <v>1</v>
-      </c>
-      <c r="I101" s="3">
+      <c r="C101" s="2">
+        <v>1</v>
+      </c>
+      <c r="D101" s="2">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2">
+        <v>1</v>
+      </c>
+      <c r="G101" s="2">
+        <v>1</v>
+      </c>
+      <c r="H101" s="2">
+        <v>1</v>
+      </c>
+      <c r="I101" s="2">
         <v>1</v>
       </c>
       <c r="J101" s="38">
@@ -2951,25 +2949,25 @@
       <c r="B112" s="37">
         <v>1</v>
       </c>
-      <c r="C112" s="3">
-        <v>2</v>
-      </c>
-      <c r="D112" s="3">
-        <v>3</v>
-      </c>
-      <c r="E112" s="3">
+      <c r="C112" s="2">
+        <v>2</v>
+      </c>
+      <c r="D112" s="2">
+        <v>3</v>
+      </c>
+      <c r="E112" s="2">
         <v>4</v>
       </c>
-      <c r="F112" s="3">
+      <c r="F112" s="2">
         <v>5</v>
       </c>
-      <c r="G112" s="3">
+      <c r="G112" s="2">
         <v>6</v>
       </c>
-      <c r="H112" s="3">
+      <c r="H112" s="2">
         <v>7</v>
       </c>
-      <c r="I112" s="3">
+      <c r="I112" s="2">
         <v>8</v>
       </c>
     </row>
@@ -2977,28 +2975,28 @@
       <c r="A113" t="s">
         <v>58</v>
       </c>
-      <c r="B113" s="3">
-        <v>1</v>
-      </c>
-      <c r="C113" s="3">
+      <c r="B113" s="2">
+        <v>1</v>
+      </c>
+      <c r="C113" s="2">
         <v>5</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="2">
         <v>8</v>
       </c>
-      <c r="E113" s="3">
+      <c r="E113" s="2">
         <v>9</v>
       </c>
-      <c r="F113" s="3">
+      <c r="F113" s="2">
         <v>10</v>
       </c>
-      <c r="G113" s="3">
+      <c r="G113" s="2">
         <v>17</v>
       </c>
-      <c r="H113" s="3">
+      <c r="H113" s="2">
         <v>17</v>
       </c>
-      <c r="I113" s="3">
+      <c r="I113" s="2">
         <v>20</v>
       </c>
     </row>
@@ -3052,7 +3050,7 @@
       <c r="E118" t="s">
         <v>62</v>
       </c>
-      <c r="F118" s="22">
+      <c r="F118" s="23">
         <v>1</v>
       </c>
     </row>
@@ -3068,7 +3066,7 @@
       <c r="B121" s="37">
         <v>1</v>
       </c>
-      <c r="C121" s="3">
+      <c r="C121" s="2">
         <v>2</v>
       </c>
       <c r="E121" t="s">
@@ -3080,7 +3078,7 @@
       <c r="G121">
         <v>2</v>
       </c>
-      <c r="H121" s="22">
+      <c r="H121" s="23">
         <v>5</v>
       </c>
     </row>
@@ -3108,10 +3106,10 @@
       <c r="B124" s="37">
         <v>1</v>
       </c>
-      <c r="C124" s="3">
-        <v>2</v>
-      </c>
-      <c r="D124" s="3">
+      <c r="C124" s="2">
+        <v>2</v>
+      </c>
+      <c r="D124" s="2">
         <v>3</v>
       </c>
       <c r="F124" t="s">
@@ -3123,7 +3121,7 @@
       <c r="H124">
         <v>6</v>
       </c>
-      <c r="I124" s="22">
+      <c r="I124" s="23">
         <v>8</v>
       </c>
     </row>
@@ -3165,13 +3163,13 @@
       <c r="B128" s="37">
         <v>1</v>
       </c>
-      <c r="C128" s="3">
-        <v>2</v>
-      </c>
-      <c r="D128" s="3">
-        <v>3</v>
-      </c>
-      <c r="E128" s="3">
+      <c r="C128" s="2">
+        <v>2</v>
+      </c>
+      <c r="D128" s="2">
+        <v>3</v>
+      </c>
+      <c r="E128" s="2">
         <v>4</v>
       </c>
       <c r="G128" t="s">
@@ -3183,7 +3181,7 @@
       <c r="I128">
         <v>9</v>
       </c>
-      <c r="J128" s="22">
+      <c r="J128" s="23">
         <v>10</v>
       </c>
     </row>
@@ -3266,19 +3264,19 @@
       <c r="A142" t="s">
         <v>13</v>
       </c>
-      <c r="B142" s="40">
-        <v>2</v>
-      </c>
-      <c r="C142" s="40">
+      <c r="B142" s="2">
+        <v>2</v>
+      </c>
+      <c r="C142" s="2">
         <v>7</v>
       </c>
-      <c r="D142" s="40">
+      <c r="D142" s="2">
         <v>9</v>
       </c>
-      <c r="E142" s="40">
-        <v>3</v>
-      </c>
-      <c r="F142" s="40">
+      <c r="E142" s="2">
+        <v>3</v>
+      </c>
+      <c r="F142" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3330,7 +3328,7 @@
       <c r="B148" t="s">
         <v>93</v>
       </c>
-      <c r="D148" s="41">
+      <c r="D148" s="23">
         <v>12</v>
       </c>
     </row>
@@ -3349,7 +3347,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -3459,7 +3457,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -3485,16 +3483,16 @@
       <c r="A8" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3502,13 +3500,13 @@
       <c r="A9" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3516,10 +3514,10 @@
       <c r="A11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3530,10 +3528,10 @@
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
@@ -3554,13 +3552,13 @@
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="22" t="s">
+      <c r="D19" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>3</v>
       </c>
       <c r="F19" t="s">
@@ -3568,16 +3566,16 @@
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="23">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="B20" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="24">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
         <v>1</v>
       </c>
       <c r="F20">
@@ -3585,16 +3583,16 @@
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="B21" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
         <v>1</v>
       </c>
       <c r="F21">
@@ -3605,16 +3603,16 @@
       <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="24">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="6">
         <v>0</v>
       </c>
     </row>
@@ -3622,16 +3620,16 @@
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="24">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
         <v>0</v>
       </c>
     </row>
@@ -3648,7 +3646,7 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24" s="6">
         <v>0</v>
       </c>
     </row>
@@ -3686,16 +3684,16 @@
       <c r="A37" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3703,13 +3701,13 @@
       <c r="A38" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3717,10 +3715,10 @@
       <c r="A40" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3734,10 +3732,10 @@
       <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>107</v>
       </c>
       <c r="F41" t="s">
@@ -3755,10 +3753,10 @@
       </c>
     </row>
     <row r="47" spans="3:6">
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="23" t="s">
         <v>107</v>
       </c>
       <c r="E47" t="s">
@@ -3769,16 +3767,16 @@
       </c>
     </row>
     <row r="48" spans="2:6">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="23">
-        <v>2</v>
-      </c>
-      <c r="D48" s="3">
-        <v>1</v>
-      </c>
-      <c r="E48" s="3">
+      <c r="C48" s="24">
+        <v>2</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2">
         <v>1</v>
       </c>
       <c r="F48">
@@ -3786,16 +3784,16 @@
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="2">
-        <v>2</v>
-      </c>
-      <c r="D49" s="3">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3">
+      <c r="C49" s="4">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2">
         <v>1</v>
       </c>
       <c r="F49">
@@ -3803,16 +3801,16 @@
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="3">
-        <v>2</v>
-      </c>
-      <c r="D50" s="2">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3">
+      <c r="C50" s="2">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2">
         <v>1</v>
       </c>
       <c r="F50">
@@ -3820,16 +3818,16 @@
       </c>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="3">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1</v>
-      </c>
-      <c r="E51" s="3">
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
         <v>0</v>
       </c>
       <c r="F51">
@@ -3846,7 +3844,7 @@
       <c r="D52">
         <v>0</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E52" s="6">
         <v>0</v>
       </c>
       <c r="F52">
@@ -3888,12 +3886,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="8.60952380952381" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7387387387387" customWidth="1"/>
-    <col min="3" max="3" width="18.045045045045" customWidth="1"/>
-    <col min="4" max="6" width="26.7837837837838" customWidth="1"/>
-    <col min="7" max="10" width="36.3513513513514" customWidth="1"/>
+    <col min="1" max="1" width="10.7428571428571" customWidth="1"/>
+    <col min="3" max="3" width="18.047619047619" customWidth="1"/>
+    <col min="4" max="6" width="26.7809523809524" customWidth="1"/>
+    <col min="7" max="10" width="36.352380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4088,7 +4086,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -4099,19 +4097,19 @@
       <c r="A3" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4119,44 +4117,44 @@
       <c r="A4" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="3:6">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4203,16 +4201,16 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>2</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
         <v>3</v>
       </c>
     </row>
@@ -4220,16 +4218,16 @@
       <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>2</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
         <v>3</v>
       </c>
     </row>
@@ -4237,16 +4235,16 @@
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="3">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="C20" s="2">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
         <v>2</v>
       </c>
     </row>
@@ -4254,16 +4252,16 @@
       <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="3">
-        <v>3</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>2</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="C21" s="2">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2">
         <v>2</v>
       </c>
     </row>
@@ -4271,16 +4269,16 @@
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>4</v>
       </c>
-      <c r="D22" s="3">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3">
-        <v>3</v>
-      </c>
-      <c r="F22" s="3">
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2">
         <v>2</v>
       </c>
     </row>
@@ -4288,16 +4286,16 @@
       <c r="B23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>5</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>4</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>4</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="3">
         <v>3</v>
       </c>
     </row>
@@ -4316,13 +4314,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="15.045045045045" customWidth="1"/>
+    <col min="6" max="6" width="15.047619047619" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.8108108108108" customWidth="1"/>
-    <col min="9" max="9" width="18.0990990990991" customWidth="1"/>
+    <col min="8" max="8" width="13.8095238095238" customWidth="1"/>
+    <col min="9" max="9" width="18.0952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -4330,82 +4328,82 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="15.3" spans="2:12">
+    <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="20">
+      <c r="L3" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.3" spans="2:12">
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="19">
-        <v>2</v>
-      </c>
-      <c r="L4" s="20" t="s">
+    <row r="4" ht="15.75" spans="2:12">
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="20">
+        <v>2</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" ht="15.3" spans="2:9">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="I5" s="19">
+    <row r="5" ht="15.75" spans="2:9">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10">
+        <v>2</v>
+      </c>
+      <c r="I5" s="20">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.3" spans="2:9">
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9">
-        <v>3</v>
-      </c>
-      <c r="I6" s="19">
+    <row r="6" ht="15.75" spans="2:9">
+      <c r="B6" s="9"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10">
+        <v>3</v>
+      </c>
+      <c r="I6" s="20">
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="15.3" spans="2:9">
-      <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9">
+    <row r="7" ht="15.75" spans="2:9">
+      <c r="B7" s="9"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="10">
         <v>4</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="20">
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="15.3" spans="2:9">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13">
+    <row r="8" ht="15.75" spans="2:9">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14">
         <v>5</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="20">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.3" spans="2:2">
+    <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="11" ht="15.3" spans="2:9">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
+    <row r="11" ht="15.75" spans="2:9">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="H11" t="s">
         <v>134</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="20">
         <v>10</v>
       </c>
     </row>
@@ -4413,7 +4411,7 @@
       <c r="H12" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="20">
         <v>11</v>
       </c>
     </row>
@@ -4421,7 +4419,7 @@
       <c r="H13" t="s">
         <v>136</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="20">
         <v>11</v>
       </c>
     </row>
@@ -4429,7 +4427,7 @@
       <c r="H14" t="s">
         <v>137</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="20">
         <v>10</v>
       </c>
     </row>
@@ -4437,7 +4435,7 @@
       <c r="H15">
         <v>5</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="20">
         <v>10</v>
       </c>
     </row>
@@ -4445,7 +4443,7 @@
       <c r="H16" t="s">
         <v>138</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="18">
         <v>12</v>
       </c>
     </row>
@@ -4453,7 +4451,7 @@
       <c r="H17" t="s">
         <v>139</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="18">
         <v>12</v>
       </c>
     </row>
@@ -4461,32 +4459,32 @@
       <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.3"/>
-    <row r="22" customFormat="1" ht="15.3" spans="1:5">
+      <c r="B20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75"/>
+    <row r="22" customFormat="1" ht="15.75" spans="1:5">
       <c r="A22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="18">
-        <v>1</v>
-      </c>
-      <c r="D22" s="19" t="s">
+      <c r="B22" s="19">
+        <v>1</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" ht="15.3"/>
-    <row r="24" customFormat="1" ht="15.3" spans="1:7">
+      <c r="E22" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75"/>
+    <row r="24" customFormat="1" ht="15.75" spans="1:7">
       <c r="A24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="16">
+      <c r="B24" s="15"/>
+      <c r="C24" s="17">
         <v>2</v>
       </c>
       <c r="E24" t="s">
@@ -4495,7 +4493,7 @@
       <c r="F24" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="20">
         <v>4</v>
       </c>
     </row>
@@ -4506,7 +4504,7 @@
       <c r="F25" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="18">
         <v>5</v>
       </c>
       <c r="L25" t="s">
@@ -4516,21 +4514,21 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" ht="15.3" spans="12:13">
+    <row r="26" ht="15.75" spans="12:13">
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="M26" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" ht="15.3" spans="1:13">
+      <c r="M26" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:13">
       <c r="A27" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17">
         <v>3</v>
       </c>
       <c r="F27" t="s">
@@ -4539,13 +4537,13 @@
       <c r="G27" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="20">
         <v>7</v>
       </c>
       <c r="L27">
         <v>2</v>
       </c>
-      <c r="M27" s="19">
+      <c r="M27" s="20">
         <v>5</v>
       </c>
     </row>
@@ -4556,13 +4554,13 @@
       <c r="G28" t="s">
         <v>75</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="20">
         <v>7</v>
       </c>
       <c r="L28">
         <v>3</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M28" s="20">
         <v>7</v>
       </c>
     </row>
@@ -4573,13 +4571,13 @@
       <c r="G29" t="s">
         <v>142</v>
       </c>
-      <c r="H29" s="17">
+      <c r="H29" s="18">
         <v>7</v>
       </c>
       <c r="L29">
         <v>4</v>
       </c>
-      <c r="M29" s="19">
+      <c r="M29" s="20">
         <v>8</v>
       </c>
     </row>
@@ -4587,19 +4585,19 @@
       <c r="L30">
         <v>5</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="20">
         <v>10</v>
       </c>
     </row>
-    <row r="31" ht="15.3"/>
-    <row r="32" ht="15.3" spans="1:9">
+    <row r="31" ht="15.75"/>
+    <row r="32" ht="15.75" spans="1:9">
       <c r="A32" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16">
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17">
         <v>4</v>
       </c>
       <c r="G32" t="s">
@@ -4608,7 +4606,7 @@
       <c r="H32" t="s">
         <v>80</v>
       </c>
-      <c r="I32" s="19">
+      <c r="I32" s="20">
         <v>9</v>
       </c>
     </row>
@@ -4619,7 +4617,7 @@
       <c r="H33" t="s">
         <v>83</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33" s="18">
         <v>10</v>
       </c>
     </row>
@@ -4630,7 +4628,7 @@
       <c r="H34" t="s">
         <v>85</v>
       </c>
-      <c r="I34" s="19">
+      <c r="I34" s="20">
         <v>9</v>
       </c>
     </row>
@@ -4641,20 +4639,20 @@
       <c r="H35" t="s">
         <v>143</v>
       </c>
-      <c r="I35" s="19">
+      <c r="I35" s="20">
         <v>8</v>
       </c>
     </row>
-    <row r="37" ht="15.3"/>
-    <row r="38" ht="15.3" spans="1:10">
+    <row r="37" ht="15.75"/>
+    <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="16">
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="17">
         <v>5</v>
       </c>
       <c r="H38" t="s">
@@ -4663,7 +4661,7 @@
       <c r="I38" t="s">
         <v>145</v>
       </c>
-      <c r="J38" s="19">
+      <c r="J38" s="20">
         <v>12</v>
       </c>
     </row>
@@ -4674,7 +4672,7 @@
       <c r="I39" t="s">
         <v>146</v>
       </c>
-      <c r="J39" s="19">
+      <c r="J39" s="20">
         <v>12</v>
       </c>
     </row>
@@ -4685,7 +4683,7 @@
       <c r="I40" t="s">
         <v>148</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="18">
         <v>12</v>
       </c>
     </row>
@@ -4696,7 +4694,7 @@
       <c r="I41" t="s">
         <v>150</v>
       </c>
-      <c r="J41" s="19">
+      <c r="J41" s="20">
         <v>10</v>
       </c>
     </row>
@@ -4707,7 +4705,7 @@
       <c r="I42" t="s">
         <v>152</v>
       </c>
-      <c r="J42" s="19">
+      <c r="J42" s="20">
         <v>10</v>
       </c>
     </row>
@@ -4722,15 +4720,15 @@
   <sheetPr/>
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.4324324324324" customWidth="1"/>
-    <col min="2" max="2" width="15.2882882882883" customWidth="1"/>
-    <col min="12" max="12" width="12.7117117117117" customWidth="1"/>
+    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -4772,19 +4770,19 @@
       <c r="L15" t="s">
         <v>156</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="2">
         <v>4</v>
       </c>
-      <c r="N15" s="2">
-        <v>2</v>
-      </c>
-      <c r="O15" s="2">
+      <c r="N15" s="4">
+        <v>2</v>
+      </c>
+      <c r="O15" s="4">
         <v>10</v>
       </c>
-      <c r="P15" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2">
+      <c r="P15" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="4">
         <v>2</v>
       </c>
       <c r="R15" t="s">
@@ -4795,19 +4793,19 @@
       <c r="L16" t="s">
         <v>158</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="2">
         <v>12</v>
       </c>
-      <c r="N16" s="2">
-        <v>1</v>
-      </c>
-      <c r="O16" s="2">
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4">
         <v>4</v>
       </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2">
+      <c r="P16" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="4">
         <v>2</v>
       </c>
       <c r="R16" t="s">
@@ -4906,7 +4904,7 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="6">
         <v>0</v>
       </c>
       <c r="K29">
@@ -4944,49 +4942,49 @@
       <c r="C30" s="2">
         <v>0</v>
       </c>
-      <c r="D30" s="3">
-        <v>0</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3">
-        <v>0</v>
-      </c>
-      <c r="J30" s="3">
-        <v>0</v>
-      </c>
-      <c r="K30" s="3">
-        <v>0</v>
-      </c>
-      <c r="L30" s="3">
-        <v>0</v>
-      </c>
-      <c r="M30" s="3">
-        <v>0</v>
-      </c>
-      <c r="N30" s="3">
-        <v>0</v>
-      </c>
-      <c r="O30" s="4">
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2">
+        <v>0</v>
+      </c>
+      <c r="O30" s="3">
         <v>4</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P30" s="2">
         <v>4</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q30" s="2">
         <v>4</v>
       </c>
-      <c r="R30" s="3">
+      <c r="R30" s="2">
         <v>4</v>
       </c>
     </row>
@@ -4997,52 +4995,52 @@
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" s="3">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3">
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
         <v>2</v>
       </c>
       <c r="E31" s="2">
         <v>2</v>
       </c>
-      <c r="F31" s="3">
-        <v>2</v>
-      </c>
-      <c r="G31" s="3">
-        <v>2</v>
-      </c>
-      <c r="H31" s="3">
-        <v>2</v>
-      </c>
-      <c r="I31" s="3">
-        <v>2</v>
-      </c>
-      <c r="J31" s="3">
-        <v>2</v>
-      </c>
-      <c r="K31" s="3">
-        <v>2</v>
-      </c>
-      <c r="L31" s="3">
-        <v>2</v>
-      </c>
-      <c r="M31" s="3">
-        <v>2</v>
-      </c>
-      <c r="N31" s="3">
-        <v>2</v>
-      </c>
-      <c r="O31" s="3">
+      <c r="F31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
+      <c r="K31" s="4">
+        <v>2</v>
+      </c>
+      <c r="L31" s="2">
+        <v>2</v>
+      </c>
+      <c r="M31" s="2">
+        <v>2</v>
+      </c>
+      <c r="N31" s="2">
+        <v>2</v>
+      </c>
+      <c r="O31" s="2">
         <v>4</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P31" s="3">
         <v>6</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31" s="2">
         <v>6</v>
       </c>
-      <c r="R31" s="3">
+      <c r="R31" s="2">
         <v>6</v>
       </c>
     </row>
@@ -5053,52 +5051,52 @@
       <c r="B32">
         <v>3</v>
       </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3">
-        <v>2</v>
-      </c>
-      <c r="F32" s="3">
-        <v>2</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2">
         <v>10</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <v>12</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <v>12</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>12</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="2">
         <v>12</v>
       </c>
-      <c r="L32" s="3">
+      <c r="L32" s="2">
         <v>12</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="2">
         <v>12</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="2">
         <v>12</v>
       </c>
-      <c r="O32" s="2">
+      <c r="O32" s="4">
         <v>12</v>
       </c>
-      <c r="P32" s="3">
+      <c r="P32" s="2">
         <v>12</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="Q32" s="2">
         <v>12</v>
       </c>
-      <c r="R32" s="3">
+      <c r="R32" s="2">
         <v>12</v>
       </c>
     </row>
@@ -5109,52 +5107,52 @@
       <c r="B33">
         <v>4</v>
       </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>2</v>
-      </c>
-      <c r="E33" s="3">
-        <v>2</v>
-      </c>
-      <c r="F33" s="3">
-        <v>2</v>
-      </c>
-      <c r="G33" s="3">
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2</v>
+      </c>
+      <c r="G33" s="2">
         <v>10</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>12</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <v>13</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <v>13</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="2">
         <v>13</v>
       </c>
-      <c r="L33" s="3">
+      <c r="L33" s="2">
         <v>13</v>
       </c>
-      <c r="M33" s="3">
+      <c r="M33" s="2">
         <v>13</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="2">
         <v>13</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="2">
         <v>13</v>
       </c>
-      <c r="P33" s="2">
+      <c r="P33" s="4">
         <v>13</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="Q33" s="2">
         <v>13</v>
       </c>
-      <c r="R33" s="3">
+      <c r="R33" s="2">
         <v>13</v>
       </c>
     </row>
@@ -5165,52 +5163,52 @@
       <c r="B34">
         <v>5</v>
       </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>2</v>
-      </c>
-      <c r="E34" s="3">
-        <v>2</v>
-      </c>
-      <c r="F34" s="4">
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
+      <c r="F34" s="3">
         <v>4</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="2">
         <v>10</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>12</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="2">
         <v>13</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <v>14</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="3">
         <v>15</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L34" s="2">
         <v>15</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34" s="2">
         <v>15</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="2">
         <v>15</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34" s="2">
         <v>15</v>
       </c>
-      <c r="P34" s="3">
+      <c r="P34" s="2">
         <v>15</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="Q34" s="2">
         <v>15</v>
       </c>
-      <c r="R34" s="6">
+      <c r="R34" s="7">
         <v>15</v>
       </c>
     </row>
@@ -5220,12 +5218,12 @@
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="40" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="40" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solved Max Product Subarray problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" activeTab="8"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="206">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -294,16 +294,25 @@
     <t>HouseRobber</t>
   </si>
   <si>
-    <t>MAX(nums[1],dp[0])</t>
-  </si>
-  <si>
-    <t>MAX(nums[2]+dp[0],dp[1])</t>
-  </si>
-  <si>
-    <t>MAX(nums[3]+dp[1],dp[2])</t>
-  </si>
-  <si>
-    <t>MAX(nums[4]+dp[2],dp[3])</t>
+    <t>nums = [2,7,9,3,1]</t>
+  </si>
+  <si>
+    <t>2,9</t>
+  </si>
+  <si>
+    <t>3+dp[1]</t>
+  </si>
+  <si>
+    <t>nums[i]+dp[i-2]</t>
+  </si>
+  <si>
+    <t>9+dp[0]</t>
+  </si>
+  <si>
+    <t>dp[i-1]</t>
+  </si>
+  <si>
+    <t>nums[4]+dp[2]</t>
   </si>
   <si>
     <t>n</t>
@@ -357,55 +366,106 @@
     <t>CoinChange</t>
   </si>
   <si>
-    <t>dp init</t>
-  </si>
-  <si>
-    <t>dp formula</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[1-1])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[2-1],1+dp[2-2])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[3-1],1+dp[3-2])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[4-1],1+dp[4-2])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[5-1],1+dp[5-2],1+dp[5-5])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[6-1],1+dp[6-2],1+dp[6-5])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[7-1],1+dp[7-2],1+dp[7-5])</t>
-  </si>
-  <si>
-    <t>min(12,1+dp[8-1],1+dp[8-2],1+dp[8-5])</t>
-  </si>
-  <si>
-    <t>dp final</t>
-  </si>
-  <si>
-    <t>dp[1] + dp[2]</t>
-  </si>
-  <si>
-    <t>coins</t>
-  </si>
-  <si>
-    <t>amount=&gt;</t>
-  </si>
-  <si>
-    <t>1+dp[3-1],1+dp[3-2]</t>
-  </si>
-  <si>
-    <t>1+dp[3],1+dp[2]</t>
-  </si>
-  <si>
-    <t>3,3,1</t>
+    <t>coins = [1,2,5], amount = 11</t>
+  </si>
+  <si>
+    <t>dp[11]</t>
+  </si>
+  <si>
+    <t>1+dp[11-1]</t>
+  </si>
+  <si>
+    <t>1+dp[11-2]</t>
+  </si>
+  <si>
+    <t>1+dp[11-5]</t>
+  </si>
+  <si>
+    <t>1+dp[3-1]</t>
+  </si>
+  <si>
+    <t>1+dp[amount-coin]</t>
+  </si>
+  <si>
+    <t>1+dp[3-2]</t>
+  </si>
+  <si>
+    <t>1+dp[4-1]</t>
+  </si>
+  <si>
+    <t>1+dp[4-2]</t>
+  </si>
+  <si>
+    <t>dp[5]</t>
+  </si>
+  <si>
+    <t>1+dp[5-1]</t>
+  </si>
+  <si>
+    <t>dp[6]</t>
+  </si>
+  <si>
+    <t>1+dp[6-1]</t>
+  </si>
+  <si>
+    <t>dp[7]</t>
+  </si>
+  <si>
+    <t>1+dp[7-1]</t>
+  </si>
+  <si>
+    <t>1+dp[5-2]</t>
+  </si>
+  <si>
+    <t>1+dp[6-2]</t>
+  </si>
+  <si>
+    <t>1+dp[7-2]</t>
+  </si>
+  <si>
+    <t>1+dp[5-5]</t>
+  </si>
+  <si>
+    <t>1+dp[6-5]</t>
+  </si>
+  <si>
+    <t>1+dp[7-5]</t>
+  </si>
+  <si>
+    <t>dp[8]</t>
+  </si>
+  <si>
+    <t>1+dp[8-1]</t>
+  </si>
+  <si>
+    <t>dp[9]</t>
+  </si>
+  <si>
+    <t>1+dp[9-1]</t>
+  </si>
+  <si>
+    <t>dp[10]</t>
+  </si>
+  <si>
+    <t>1+dp[10-1]</t>
+  </si>
+  <si>
+    <t>1+dp[8-2]</t>
+  </si>
+  <si>
+    <t>1+dp[9-2]</t>
+  </si>
+  <si>
+    <t>1+dp[10-2]</t>
+  </si>
+  <si>
+    <t>1+dp[8-5]</t>
+  </si>
+  <si>
+    <t>1+dp[9-5]</t>
+  </si>
+  <si>
+    <t>1+dp[10-5]</t>
   </si>
   <si>
     <t>word1</t>
@@ -466,9 +526,6 @@
   </si>
   <si>
     <t>price[4]+dp[0]</t>
-  </si>
-  <si>
-    <t>dp[5]</t>
   </si>
   <si>
     <t>price[1]+dp[4]</t>
@@ -590,11 +647,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -646,27 +703,15 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -682,16 +727,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,7 +790,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -720,32 +811,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -759,32 +833,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -805,6 +862,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -817,109 +892,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -937,7 +910,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -949,25 +994,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -979,13 +1012,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1257,6 +1314,65 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1280,7 +1396,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1299,69 +1415,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1379,134 +1436,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1534,8 +1591,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1557,6 +1615,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1971,10 +2033,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J148"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="I160" sqref="I160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2196,7 +2258,7 @@
       <c r="I22">
         <v>7</v>
       </c>
-      <c r="J22" s="30" t="s">
+      <c r="J22" s="31" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2228,7 +2290,7 @@
       <c r="I23" s="5">
         <v>18</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="31" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2242,7 +2304,7 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="25">
         <v>4</v>
       </c>
       <c r="E25">
@@ -2490,28 +2552,28 @@
       <c r="A53" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E53" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F53" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="29" t="s">
+      <c r="G53" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H53" s="29" t="s">
+      <c r="H53" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="29" t="s">
+      <c r="I53" s="30" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2519,7 +2581,7 @@
       <c r="A55" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="26" t="b">
+      <c r="B55" s="25" t="b">
         <v>1</v>
       </c>
       <c r="C55" t="b">
@@ -2567,30 +2629,30 @@
     </row>
     <row r="66" ht="15.75"/>
     <row r="67" ht="15.75" spans="7:7">
-      <c r="G67" s="31"/>
+      <c r="G67" s="32"/>
     </row>
     <row r="68" ht="15.75" spans="6:7">
-      <c r="F68" s="32"/>
-      <c r="G68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="34"/>
     </row>
     <row r="69" ht="15.75" spans="5:7">
-      <c r="E69" s="32"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" ht="15.75" spans="4:7">
-      <c r="D70" s="32"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" ht="15.75" spans="2:7">
-      <c r="B71" s="35"/>
+      <c r="B71" s="36"/>
       <c r="C71" s="15"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="38"/>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
@@ -2619,7 +2681,7 @@
       <c r="A74" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="26">
+      <c r="B74" s="25">
         <v>8</v>
       </c>
       <c r="C74">
@@ -2659,30 +2721,30 @@
     </row>
     <row r="79" ht="15.75"/>
     <row r="80" ht="15.75" spans="7:7">
-      <c r="G80" s="31"/>
+      <c r="G80" s="32"/>
     </row>
     <row r="81" ht="15.75" spans="6:7">
-      <c r="F81" s="32"/>
-      <c r="G81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="34"/>
     </row>
     <row r="82" ht="15.75" spans="5:7">
-      <c r="E82" s="32"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="34"/>
     </row>
     <row r="83" ht="15.75" spans="4:7">
-      <c r="D83" s="32"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="34"/>
     </row>
     <row r="84" ht="15.75" spans="2:7">
-      <c r="B84" s="35"/>
+      <c r="B84" s="36"/>
       <c r="C84" s="15"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
-      <c r="G84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="38"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
@@ -2711,7 +2773,7 @@
       <c r="A87" t="s">
         <v>41</v>
       </c>
-      <c r="B87" s="26">
+      <c r="B87" s="25">
         <v>13</v>
       </c>
       <c r="C87">
@@ -2776,13 +2838,13 @@
       <c r="B96" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="38">
+      <c r="C96" s="39">
         <v>4</v>
       </c>
-      <c r="D96" s="39">
-        <v>3</v>
-      </c>
-      <c r="E96" s="39">
+      <c r="D96" s="40">
+        <v>3</v>
+      </c>
+      <c r="E96" s="40">
         <v>3</v>
       </c>
       <c r="F96" s="5">
@@ -2797,7 +2859,7 @@
       <c r="I96" s="5">
         <v>1</v>
       </c>
-      <c r="J96" s="40">
+      <c r="J96" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2805,13 +2867,13 @@
       <c r="B97" t="s">
         <v>51</v>
       </c>
-      <c r="C97" s="39">
+      <c r="C97" s="40">
         <v>4</v>
       </c>
-      <c r="D97" s="39">
-        <v>3</v>
-      </c>
-      <c r="E97" s="39">
+      <c r="D97" s="40">
+        <v>3</v>
+      </c>
+      <c r="E97" s="40">
         <v>3</v>
       </c>
       <c r="F97" s="5">
@@ -2826,7 +2888,7 @@
       <c r="I97" s="5">
         <v>1</v>
       </c>
-      <c r="J97" s="40">
+      <c r="J97" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2834,13 +2896,13 @@
       <c r="B98" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="39">
+      <c r="C98" s="40">
         <v>4</v>
       </c>
-      <c r="D98" s="39">
-        <v>3</v>
-      </c>
-      <c r="E98" s="39">
+      <c r="D98" s="40">
+        <v>3</v>
+      </c>
+      <c r="E98" s="40">
         <v>3</v>
       </c>
       <c r="F98" s="5">
@@ -2855,7 +2917,7 @@
       <c r="I98" s="5">
         <v>1</v>
       </c>
-      <c r="J98" s="40">
+      <c r="J98" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2884,7 +2946,7 @@
       <c r="I99" s="5">
         <v>1</v>
       </c>
-      <c r="J99" s="40">
+      <c r="J99" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2913,7 +2975,7 @@
       <c r="I100" s="5">
         <v>1</v>
       </c>
-      <c r="J100" s="40">
+      <c r="J100" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2942,7 +3004,7 @@
       <c r="I101" s="5">
         <v>1</v>
       </c>
-      <c r="J101" s="40">
+      <c r="J101" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2950,28 +3012,28 @@
       <c r="B102" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="40">
-        <v>0</v>
-      </c>
-      <c r="D102" s="40">
-        <v>0</v>
-      </c>
-      <c r="E102" s="40">
-        <v>0</v>
-      </c>
-      <c r="F102" s="40">
-        <v>0</v>
-      </c>
-      <c r="G102" s="40">
-        <v>0</v>
-      </c>
-      <c r="H102" s="40">
-        <v>0</v>
-      </c>
-      <c r="I102" s="40">
-        <v>0</v>
-      </c>
-      <c r="J102" s="40">
+      <c r="C102" s="41">
+        <v>0</v>
+      </c>
+      <c r="D102" s="41">
+        <v>0</v>
+      </c>
+      <c r="E102" s="41">
+        <v>0</v>
+      </c>
+      <c r="F102" s="41">
+        <v>0</v>
+      </c>
+      <c r="G102" s="41">
+        <v>0</v>
+      </c>
+      <c r="H102" s="41">
+        <v>0</v>
+      </c>
+      <c r="I102" s="41">
+        <v>0</v>
+      </c>
+      <c r="J102" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2991,13 +3053,13 @@
       </c>
     </row>
     <row r="111" spans="7:7">
-      <c r="G111" s="41"/>
+      <c r="G111" s="42"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>57</v>
       </c>
-      <c r="B112" s="39">
+      <c r="B112" s="40">
         <v>1</v>
       </c>
       <c r="C112" s="5">
@@ -3092,7 +3154,7 @@
       <c r="A118" t="s">
         <v>60</v>
       </c>
-      <c r="B118" s="39">
+      <c r="B118" s="40">
         <v>1</v>
       </c>
       <c r="D118" t="s">
@@ -3101,7 +3163,7 @@
       <c r="E118" t="s">
         <v>62</v>
       </c>
-      <c r="F118" s="26">
+      <c r="F118" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3114,7 +3176,7 @@
       <c r="A121" t="s">
         <v>64</v>
       </c>
-      <c r="B121" s="39">
+      <c r="B121" s="40">
         <v>1</v>
       </c>
       <c r="C121" s="5">
@@ -3129,7 +3191,7 @@
       <c r="G121">
         <v>2</v>
       </c>
-      <c r="H121" s="26">
+      <c r="H121" s="25">
         <v>5</v>
       </c>
     </row>
@@ -3154,7 +3216,7 @@
       <c r="A124" t="s">
         <v>70</v>
       </c>
-      <c r="B124" s="39">
+      <c r="B124" s="40">
         <v>1</v>
       </c>
       <c r="C124" s="5">
@@ -3172,7 +3234,7 @@
       <c r="H124">
         <v>6</v>
       </c>
-      <c r="I124" s="26">
+      <c r="I124" s="25">
         <v>8</v>
       </c>
     </row>
@@ -3211,7 +3273,7 @@
       <c r="A128" t="s">
         <v>78</v>
       </c>
-      <c r="B128" s="39">
+      <c r="B128" s="40">
         <v>1</v>
       </c>
       <c r="C128" s="5">
@@ -3232,7 +3294,7 @@
       <c r="I128">
         <v>9</v>
       </c>
-      <c r="J128" s="26">
+      <c r="J128" s="25">
         <v>10</v>
       </c>
     </row>
@@ -3286,101 +3348,188 @@
         <v>88</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" customFormat="1" spans="1:1">
       <c r="A139" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
-      <c r="A141" t="s">
+    <row r="140" customFormat="1"/>
+    <row r="141" customFormat="1" spans="1:1">
+      <c r="A141" s="43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="142" customFormat="1"/>
+    <row r="143" customFormat="1" spans="1:6">
+      <c r="A143" t="s">
         <v>12</v>
       </c>
-      <c r="B141">
-        <v>0</v>
-      </c>
-      <c r="C141">
-        <v>1</v>
-      </c>
-      <c r="D141">
-        <v>2</v>
-      </c>
-      <c r="E141">
-        <v>3</v>
-      </c>
-      <c r="F141">
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+      <c r="E143">
+        <v>3</v>
+      </c>
+      <c r="F143">
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
-      <c r="A142" t="s">
+    <row r="144" customFormat="1" spans="1:6">
+      <c r="A144" t="s">
         <v>13</v>
       </c>
-      <c r="B142" s="5">
-        <v>2</v>
-      </c>
-      <c r="C142" s="5">
+      <c r="B144" s="44">
+        <v>2</v>
+      </c>
+      <c r="C144" s="44">
         <v>7</v>
       </c>
-      <c r="D142" s="5">
+      <c r="D144" s="44">
         <v>9</v>
       </c>
-      <c r="E142" s="5">
-        <v>3</v>
-      </c>
-      <c r="F142" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" t="s">
+      <c r="E144" s="44">
+        <v>3</v>
+      </c>
+      <c r="F144" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" customFormat="1"/>
+    <row r="146" customFormat="1" spans="1:4">
+      <c r="A146" t="s">
         <v>59</v>
       </c>
-      <c r="B144">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4">
-      <c r="A145" t="s">
+      <c r="B146" s="45">
+        <v>2</v>
+      </c>
+      <c r="C146"/>
+      <c r="D146" s="46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" customFormat="1"/>
+    <row r="148" customFormat="1" spans="1:5">
+      <c r="A148" t="s">
         <v>60</v>
       </c>
-      <c r="B145" t="s">
-        <v>90</v>
-      </c>
-      <c r="D145">
+      <c r="B148" s="45">
+        <v>2</v>
+      </c>
+      <c r="C148" s="45">
         <v>7</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="A146" t="s">
+      <c r="D148"/>
+      <c r="E148" s="46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" customFormat="1"/>
+    <row r="150" customFormat="1" spans="1:7">
+      <c r="A150" t="s">
         <v>64</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B150" s="45">
+        <v>2</v>
+      </c>
+      <c r="C150" s="45">
+        <v>7</v>
+      </c>
+      <c r="D150" s="45">
+        <v>9</v>
+      </c>
+      <c r="E150"/>
+      <c r="F150" t="s">
         <v>91</v>
       </c>
-      <c r="D146">
+      <c r="G150" s="46">
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
-      <c r="A147" t="s">
+    <row r="151" customFormat="1" spans="6:7">
+      <c r="F151">
+        <v>7</v>
+      </c>
+      <c r="G151">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" customFormat="1"/>
+    <row r="153" spans="1:10">
+      <c r="A153" t="s">
         <v>70</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B153" s="45">
+        <v>2</v>
+      </c>
+      <c r="C153" s="45">
+        <v>7</v>
+      </c>
+      <c r="D153" s="45">
+        <v>9</v>
+      </c>
+      <c r="E153" s="45">
+        <v>3</v>
+      </c>
+      <c r="G153" t="s">
         <v>92</v>
       </c>
-      <c r="D147">
+      <c r="H153">
+        <v>10</v>
+      </c>
+      <c r="J153" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="154" spans="7:10">
+      <c r="G154" t="s">
+        <v>94</v>
+      </c>
+      <c r="H154" s="46">
         <v>11</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="A148" t="s">
+      <c r="J154" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="155" customFormat="1"/>
+    <row r="156" spans="1:10">
+      <c r="A156" t="s">
         <v>78</v>
       </c>
-      <c r="B148" t="s">
-        <v>93</v>
-      </c>
-      <c r="D148" s="26">
+      <c r="B156" s="45">
+        <v>2</v>
+      </c>
+      <c r="C156" s="45">
+        <v>7</v>
+      </c>
+      <c r="D156" s="45">
+        <v>9</v>
+      </c>
+      <c r="E156" s="45">
+        <v>3</v>
+      </c>
+      <c r="F156" s="45">
+        <v>1</v>
+      </c>
+      <c r="H156" t="s">
+        <v>96</v>
+      </c>
+      <c r="J156" s="46">
         <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="8:10">
+      <c r="H157" t="s">
+        <v>70</v>
+      </c>
+      <c r="J157">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3402,7 +3551,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -3443,51 +3592,51 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="28">
-        <v>0</v>
-      </c>
-      <c r="C2" s="28">
-        <v>1</v>
-      </c>
-      <c r="D2" s="28">
+        <v>98</v>
+      </c>
+      <c r="B2" s="29">
+        <v>0</v>
+      </c>
+      <c r="C2" s="29">
+        <v>1</v>
+      </c>
+      <c r="D2" s="29">
         <f t="shared" ref="D2:M2" si="0">C2+B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="29">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="29">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="29">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="29">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J2" s="28">
+      <c r="J2" s="29">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K2" s="28">
+      <c r="K2" s="29">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L2" s="28">
+      <c r="L2" s="29">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="M2" s="28">
+      <c r="M2" s="29">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
@@ -3517,22 +3666,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -3549,7 +3698,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3563,18 +3712,18 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="27" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -3594,22 +3743,22 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="26" t="s">
+      <c r="D19" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F19" t="s">
@@ -3617,10 +3766,10 @@
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="27">
+      <c r="B20" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28">
         <v>2</v>
       </c>
       <c r="D20" s="7">
@@ -3634,7 +3783,7 @@
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="5">
@@ -3703,7 +3852,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -3723,17 +3872,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>51</v>
@@ -3745,18 +3894,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -3764,18 +3913,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -3787,7 +3936,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -3795,20 +3944,20 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="3:6">
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="26" t="s">
-        <v>107</v>
+      <c r="D47" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -3818,10 +3967,10 @@
       </c>
     </row>
     <row r="48" spans="2:6">
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="27">
+      <c r="C48" s="28">
         <v>2</v>
       </c>
       <c r="D48" s="5">
@@ -3835,7 +3984,7 @@
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C49" s="7">
@@ -3852,7 +4001,7 @@
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="5">
@@ -3869,8 +4018,8 @@
       </c>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="26" t="s">
-        <v>107</v>
+      <c r="B51" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="C51" s="5">
         <v>1</v>
@@ -3904,7 +4053,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -3916,7 +4065,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -3931,261 +4080,376 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60952380952381" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7428571428571" customWidth="1"/>
-    <col min="2" max="2" width="13.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="18.047619047619" customWidth="1"/>
-    <col min="4" max="6" width="26.7809523809524" customWidth="1"/>
-    <col min="7" max="10" width="36.352380952381" customWidth="1"/>
+    <col min="10" max="10" width="10.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G5" s="5">
         <v>5</v>
       </c>
-      <c r="H3">
+      <c r="H5" s="5">
         <v>6</v>
       </c>
-      <c r="I3">
+      <c r="I5" s="5">
         <v>7</v>
       </c>
-      <c r="J3">
+      <c r="J5" s="5">
         <v>8</v>
       </c>
-      <c r="K3">
+      <c r="K5" s="5">
         <v>9</v>
       </c>
-      <c r="L3">
+      <c r="L5" s="5">
         <v>10</v>
       </c>
-      <c r="M3">
+      <c r="M5" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>12</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>12</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
-      <c r="L4">
-        <v>12</v>
-      </c>
-      <c r="M4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="25">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J9" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="25">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K11" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" spans="5:6">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="13:13">
+      <c r="M13" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="F14" t="s">
         <v>119</v>
       </c>
-      <c r="J5" t="s">
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="M14" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13">
+      <c r="F15" t="s">
         <v>121</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="5:5">
-      <c r="E8" t="s">
+      <c r="G15" s="25">
+        <v>2</v>
+      </c>
+      <c r="M15" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:9">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="G17" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="I17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" spans="7:9">
+      <c r="G18" t="s">
         <v>123</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" t="s">
+      <c r="I18" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15">
+      <c r="B20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="5">
+        <v>3</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="5">
+        <v>3</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="K21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="6">
+        <v>2</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="K22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="5">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="5">
         <v>4</v>
       </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8">
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" t="s">
-        <v>126</v>
-      </c>
-      <c r="H17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" t="s">
-        <v>68</v>
+      <c r="I24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="K24" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G25" s="5">
+        <v>3</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K25" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="6">
+        <v>3</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K26" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -4212,7 +4476,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -4232,7 +4496,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>28</v>
@@ -4277,27 +4541,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -4447,7 +4711,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="L3" s="24">
         <v>5</v>
@@ -4461,7 +4725,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -4508,7 +4772,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -4518,7 +4782,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="H11" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="I11" s="23">
         <v>10</v>
@@ -4526,7 +4790,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="I12" s="23">
         <v>11</v>
@@ -4534,7 +4798,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="I13" s="23">
         <v>11</v>
@@ -4542,7 +4806,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="I14" s="23">
         <v>10</v>
@@ -4558,7 +4822,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="I16" s="21">
         <v>12</v>
@@ -4566,7 +4830,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="I17" s="21">
         <v>12</v>
@@ -4619,7 +4883,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="G25" s="21">
         <v>5</v>
@@ -4628,7 +4892,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -4686,7 +4950,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="H29" s="21">
         <v>7</v>
@@ -4754,7 +5018,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="I35" s="23">
         <v>8</v>
@@ -4763,7 +5027,7 @@
     <row r="37" ht="15.75"/>
     <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -4773,10 +5037,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="I38" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="J38" s="23">
         <v>12</v>
@@ -4784,10 +5048,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="I39" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="J39" s="23">
         <v>12</v>
@@ -4795,10 +5059,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="I40" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="J40" s="21">
         <v>12</v>
@@ -4806,10 +5070,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="I41" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="J41" s="23">
         <v>10</v>
@@ -4817,10 +5081,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="I42" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="J42" s="23">
         <v>10</v>
@@ -4850,17 +5114,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -4885,7 +5149,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="M15" s="5">
         <v>4</v>
@@ -4903,12 +5167,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="M16" s="5">
         <v>12</v>
@@ -4926,12 +5190,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
@@ -4939,10 +5203,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -4995,7 +5259,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5051,7 +5315,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -5107,7 +5371,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -5163,7 +5427,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -5219,7 +5483,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -5275,7 +5539,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -5331,17 +5595,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="42" t="s">
-        <v>174</v>
+      <c r="A38" s="47" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="42" t="s">
-        <v>175</v>
+      <c r="A39" s="47" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -5364,7 +5628,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -5413,40 +5677,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="F6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="G6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="J6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="K6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="L6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="M6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="N6" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5457,7 +5721,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5468,7 +5732,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5479,7 +5743,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5490,7 +5754,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -5504,7 +5768,7 @@
   <sheetPr/>
   <dimension ref="A3:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -5517,7 +5781,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -5552,7 +5816,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -5584,10 +5848,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -5627,15 +5891,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -5645,7 +5909,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started Longest Palindromic Substring problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="240">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -313,6 +313,108 @@
   </si>
   <si>
     <t>nums[4]+dp[2]</t>
+  </si>
+  <si>
+    <t>MaxProductSubarray</t>
+  </si>
+  <si>
+    <t>2,3,-2,4</t>
+  </si>
+  <si>
+    <t>result=max(result, currentMax)</t>
+  </si>
+  <si>
+    <t>currMax</t>
+  </si>
+  <si>
+    <t>currMin</t>
+  </si>
+  <si>
+    <t>tmp1 = currMax*num</t>
+  </si>
+  <si>
+    <t>1*2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currMax=max(tmp1, tmp2, num) </t>
+  </si>
+  <si>
+    <t>max(2,4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tmp2 = currMin*num </t>
+  </si>
+  <si>
+    <t>currMin=min(tmp1,tmp2,num)</t>
+  </si>
+  <si>
+    <t>tmp1=2*3</t>
+  </si>
+  <si>
+    <t>currMax=max(6,6,3)</t>
+  </si>
+  <si>
+    <t>max(4,6)</t>
+  </si>
+  <si>
+    <t>tmp2=2*3</t>
+  </si>
+  <si>
+    <t>currMin=min(6,6,3)</t>
+  </si>
+  <si>
+    <t>tmp1=6*-2</t>
+  </si>
+  <si>
+    <t>currMax=max(-12,-6,-2)</t>
+  </si>
+  <si>
+    <t>max(6,-2)</t>
+  </si>
+  <si>
+    <t>tmp2=3*-2</t>
+  </si>
+  <si>
+    <t>currMin=min(-12,-6,-2)</t>
+  </si>
+  <si>
+    <t>tmp1=-2*4</t>
+  </si>
+  <si>
+    <t>currMax=max(-8,-48,4)</t>
+  </si>
+  <si>
+    <t>max(6,4)</t>
+  </si>
+  <si>
+    <t>tmp2=-12*4</t>
+  </si>
+  <si>
+    <t>currMin=min(-8,-48,4)</t>
+  </si>
+  <si>
+    <t>tmp1=-2*-4</t>
+  </si>
+  <si>
+    <t>currMax=max(8,48,-4)</t>
+  </si>
+  <si>
+    <t>max(6,48)</t>
+  </si>
+  <si>
+    <t>tmp2=-12*-4</t>
+  </si>
+  <si>
+    <t>currMin=min(8,48,-4)</t>
+  </si>
+  <si>
+    <t>Longest Palindromic Substring</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
   <si>
     <t>n</t>
@@ -647,11 +749,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -703,6 +805,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -712,10 +843,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -727,9 +858,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -744,30 +883,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,45 +904,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -833,6 +927,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -841,7 +943,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -862,7 +964,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -874,13 +982,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -892,43 +1126,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -940,109 +1138,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1320,59 +1422,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1388,6 +1440,26 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1415,10 +1487,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1436,134 +1538,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1615,10 +1717,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2033,17 +2136,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:Z195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="I160" sqref="I160"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="J197" sqref="J197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.0095238095238" customWidth="1"/>
     <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
-    <col min="4" max="4" width="15.3714285714286" customWidth="1"/>
+    <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="12.7047619047619" customWidth="1"/>
     <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
     <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
@@ -3353,13 +3456,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="140" customFormat="1"/>
     <row r="141" customFormat="1" spans="1:1">
-      <c r="A141" s="43" t="s">
+      <c r="A141" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="142" customFormat="1"/>
     <row r="143" customFormat="1" spans="1:6">
       <c r="A143" t="s">
         <v>12</v>
@@ -3384,70 +3485,64 @@
       <c r="A144" t="s">
         <v>13</v>
       </c>
-      <c r="B144" s="44">
-        <v>2</v>
-      </c>
-      <c r="C144" s="44">
+      <c r="B144" s="5">
+        <v>2</v>
+      </c>
+      <c r="C144" s="5">
         <v>7</v>
       </c>
-      <c r="D144" s="44">
+      <c r="D144" s="5">
         <v>9</v>
       </c>
-      <c r="E144" s="44">
-        <v>3</v>
-      </c>
-      <c r="F144" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" customFormat="1"/>
+      <c r="E144" s="5">
+        <v>3</v>
+      </c>
+      <c r="F144" s="5">
+        <v>1</v>
+      </c>
+    </row>
     <row r="146" customFormat="1" spans="1:4">
       <c r="A146" t="s">
         <v>59</v>
       </c>
-      <c r="B146" s="45">
-        <v>2</v>
-      </c>
-      <c r="C146"/>
-      <c r="D146" s="46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="147" customFormat="1"/>
+      <c r="B146" s="7">
+        <v>2</v>
+      </c>
+      <c r="D146" s="25">
+        <v>2</v>
+      </c>
+    </row>
     <row r="148" customFormat="1" spans="1:5">
       <c r="A148" t="s">
         <v>60</v>
       </c>
-      <c r="B148" s="45">
-        <v>2</v>
-      </c>
-      <c r="C148" s="45">
+      <c r="B148" s="7">
+        <v>2</v>
+      </c>
+      <c r="C148" s="7">
         <v>7</v>
       </c>
-      <c r="D148"/>
-      <c r="E148" s="46">
+      <c r="E148" s="25">
         <v>7</v>
       </c>
     </row>
-    <row r="149" customFormat="1"/>
     <row r="150" customFormat="1" spans="1:7">
       <c r="A150" t="s">
         <v>64</v>
       </c>
-      <c r="B150" s="45">
-        <v>2</v>
-      </c>
-      <c r="C150" s="45">
+      <c r="B150" s="7">
+        <v>2</v>
+      </c>
+      <c r="C150" s="7">
         <v>7</v>
       </c>
-      <c r="D150" s="45">
+      <c r="D150" s="7">
         <v>9</v>
       </c>
-      <c r="E150"/>
       <c r="F150" t="s">
         <v>91</v>
       </c>
-      <c r="G150" s="46">
+      <c r="G150" s="25">
         <v>11</v>
       </c>
     </row>
@@ -3459,21 +3554,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" customFormat="1"/>
     <row r="153" spans="1:10">
       <c r="A153" t="s">
         <v>70</v>
       </c>
-      <c r="B153" s="45">
-        <v>2</v>
-      </c>
-      <c r="C153" s="45">
+      <c r="B153" s="7">
+        <v>2</v>
+      </c>
+      <c r="C153" s="7">
         <v>7</v>
       </c>
-      <c r="D153" s="45">
+      <c r="D153" s="7">
         <v>9</v>
       </c>
-      <c r="E153" s="45">
+      <c r="E153" s="7">
         <v>3</v>
       </c>
       <c r="G153" t="s">
@@ -3490,37 +3584,36 @@
       <c r="G154" t="s">
         <v>94</v>
       </c>
-      <c r="H154" s="46">
+      <c r="H154" s="25">
         <v>11</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="155" customFormat="1"/>
     <row r="156" spans="1:10">
       <c r="A156" t="s">
         <v>78</v>
       </c>
-      <c r="B156" s="45">
-        <v>2</v>
-      </c>
-      <c r="C156" s="45">
+      <c r="B156" s="7">
+        <v>2</v>
+      </c>
+      <c r="C156" s="7">
         <v>7</v>
       </c>
-      <c r="D156" s="45">
+      <c r="D156" s="7">
         <v>9</v>
       </c>
-      <c r="E156" s="45">
-        <v>3</v>
-      </c>
-      <c r="F156" s="45">
+      <c r="E156" s="7">
+        <v>3</v>
+      </c>
+      <c r="F156" s="7">
         <v>1</v>
       </c>
       <c r="H156" t="s">
         <v>96</v>
       </c>
-      <c r="J156" s="46">
+      <c r="J156" s="25">
         <v>12</v>
       </c>
     </row>
@@ -3530,6 +3623,419 @@
       </c>
       <c r="J157">
         <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>12</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>2</v>
+      </c>
+      <c r="E166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>13</v>
+      </c>
+      <c r="B167" s="5">
+        <v>2</v>
+      </c>
+      <c r="C167" s="5">
+        <v>3</v>
+      </c>
+      <c r="D167" s="5">
+        <v>-2</v>
+      </c>
+      <c r="E167" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5">
+      <c r="B168" s="43">
+        <v>2</v>
+      </c>
+      <c r="C168" s="43">
+        <v>3</v>
+      </c>
+      <c r="D168" s="43">
+        <v>-2</v>
+      </c>
+      <c r="E168" s="25">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5">
+      <c r="B169" s="43"/>
+      <c r="C169" s="43"/>
+      <c r="D169" s="43"/>
+      <c r="E169" s="43"/>
+    </row>
+    <row r="170" spans="1:8">
+      <c r="A170" t="s">
+        <v>41</v>
+      </c>
+      <c r="B170" s="26">
+        <v>4</v>
+      </c>
+      <c r="C170" s="26">
+        <v>6</v>
+      </c>
+      <c r="D170" s="26">
+        <v>6</v>
+      </c>
+      <c r="E170" s="5">
+        <v>6</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="171" spans="8:14">
+      <c r="H171" s="44">
+        <v>6</v>
+      </c>
+      <c r="M171" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14">
+      <c r="A172" t="s">
+        <v>100</v>
+      </c>
+      <c r="B172">
+        <v>2</v>
+      </c>
+      <c r="C172">
+        <v>6</v>
+      </c>
+      <c r="D172">
+        <v>-2</v>
+      </c>
+      <c r="M172" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>101</v>
+      </c>
+      <c r="B173">
+        <v>2</v>
+      </c>
+      <c r="C173">
+        <v>3</v>
+      </c>
+      <c r="D173">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13">
+      <c r="A175" t="s">
+        <v>59</v>
+      </c>
+      <c r="B175" s="7">
+        <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>102</v>
+      </c>
+      <c r="E175" t="s">
+        <v>103</v>
+      </c>
+      <c r="F175" t="s">
+        <v>104</v>
+      </c>
+      <c r="I175">
+        <v>2</v>
+      </c>
+      <c r="K175" t="s">
+        <v>105</v>
+      </c>
+      <c r="M175" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="4:9">
+      <c r="D176" t="s">
+        <v>106</v>
+      </c>
+      <c r="E176" t="s">
+        <v>103</v>
+      </c>
+      <c r="F176" t="s">
+        <v>107</v>
+      </c>
+      <c r="I176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:26">
+      <c r="A178" t="s">
+        <v>60</v>
+      </c>
+      <c r="B178" s="7">
+        <v>2</v>
+      </c>
+      <c r="C178" s="7">
+        <v>3</v>
+      </c>
+      <c r="E178" t="s">
+        <v>108</v>
+      </c>
+      <c r="F178">
+        <v>6</v>
+      </c>
+      <c r="H178" t="s">
+        <v>109</v>
+      </c>
+      <c r="J178">
+        <v>6</v>
+      </c>
+      <c r="L178" t="s">
+        <v>110</v>
+      </c>
+      <c r="N178" s="25">
+        <v>6</v>
+      </c>
+      <c r="Z178" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="5:10">
+      <c r="E179" t="s">
+        <v>111</v>
+      </c>
+      <c r="F179">
+        <v>6</v>
+      </c>
+      <c r="H179" t="s">
+        <v>112</v>
+      </c>
+      <c r="J179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16">
+      <c r="A181" t="s">
+        <v>64</v>
+      </c>
+      <c r="B181" s="7">
+        <v>2</v>
+      </c>
+      <c r="C181" s="7">
+        <v>3</v>
+      </c>
+      <c r="D181" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F181" t="s">
+        <v>113</v>
+      </c>
+      <c r="G181">
+        <v>-12</v>
+      </c>
+      <c r="I181" t="s">
+        <v>114</v>
+      </c>
+      <c r="L181">
+        <v>-2</v>
+      </c>
+      <c r="N181" t="s">
+        <v>115</v>
+      </c>
+      <c r="P181" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="6:12">
+      <c r="F182" t="s">
+        <v>116</v>
+      </c>
+      <c r="G182">
+        <v>-6</v>
+      </c>
+      <c r="I182" t="s">
+        <v>117</v>
+      </c>
+      <c r="L182">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17">
+      <c r="A184" t="s">
+        <v>70</v>
+      </c>
+      <c r="B184" s="7">
+        <v>2</v>
+      </c>
+      <c r="C184" s="7">
+        <v>3</v>
+      </c>
+      <c r="D184" s="7">
+        <v>-2</v>
+      </c>
+      <c r="E184" s="7">
+        <v>4</v>
+      </c>
+      <c r="G184" t="s">
+        <v>118</v>
+      </c>
+      <c r="H184">
+        <v>-8</v>
+      </c>
+      <c r="J184" t="s">
+        <v>119</v>
+      </c>
+      <c r="M184">
+        <v>4</v>
+      </c>
+      <c r="O184" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q184" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185" spans="7:13">
+      <c r="G185" t="s">
+        <v>121</v>
+      </c>
+      <c r="H185">
+        <v>-48</v>
+      </c>
+      <c r="J185" t="s">
+        <v>122</v>
+      </c>
+      <c r="M185">
+        <v>-48</v>
+      </c>
+    </row>
+    <row r="187" spans="2:17">
+      <c r="B187" s="7">
+        <v>2</v>
+      </c>
+      <c r="C187" s="7">
+        <v>3</v>
+      </c>
+      <c r="D187" s="7">
+        <v>-2</v>
+      </c>
+      <c r="E187" s="28">
+        <v>-4</v>
+      </c>
+      <c r="G187" t="s">
+        <v>123</v>
+      </c>
+      <c r="H187">
+        <v>8</v>
+      </c>
+      <c r="J187" t="s">
+        <v>124</v>
+      </c>
+      <c r="M187">
+        <v>48</v>
+      </c>
+      <c r="O187" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q187" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="188" spans="7:13">
+      <c r="G188" t="s">
+        <v>126</v>
+      </c>
+      <c r="H188">
+        <v>48</v>
+      </c>
+      <c r="J188" t="s">
+        <v>127</v>
+      </c>
+      <c r="M188">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10">
+      <c r="A194" t="s">
+        <v>12</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="E194">
+        <v>3</v>
+      </c>
+      <c r="F194">
+        <v>4</v>
+      </c>
+      <c r="I194" t="s">
+        <v>129</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10">
+      <c r="A195" t="s">
+        <v>33</v>
+      </c>
+      <c r="B195" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D195" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E195" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F195" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I195" t="s">
+        <v>130</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3551,7 +4057,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -3592,7 +4098,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B2" s="29">
         <v>0</v>
@@ -3666,22 +4172,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -3698,7 +4204,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -3712,7 +4218,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
@@ -3723,7 +4229,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -3743,12 +4249,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -3852,7 +4358,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -3872,17 +4378,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>51</v>
@@ -3894,18 +4400,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -3913,18 +4419,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -3936,7 +4442,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -3944,12 +4450,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -3957,7 +4463,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -4019,7 +4525,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="25" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="C51" s="5">
         <v>1</v>
@@ -4053,7 +4559,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -4065,7 +4571,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -4093,12 +4599,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4191,10 +4697,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -4209,7 +4715,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -4229,7 +4735,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="K11" s="25">
         <v>3</v>
@@ -4256,13 +4762,13 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="F14" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="M14" s="26">
         <v>2</v>
@@ -4270,7 +4776,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="G15" s="25">
         <v>2</v>
@@ -4288,7 +4794,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -4296,7 +4802,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="I18" s="25">
         <v>2</v>
@@ -4304,28 +4810,28 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="G20" s="5">
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="K20" s="5">
         <v>3</v>
@@ -4334,21 +4840,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="G21" s="5">
         <v>3</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="K21" s="5">
         <v>2</v>
@@ -4357,21 +4863,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="G22" s="6">
         <v>2</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="K22" s="6">
         <v>2</v>
@@ -4379,28 +4885,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="C24" s="5">
         <v>3</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="G24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="K24" s="5">
         <v>4</v>
@@ -4409,21 +4915,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="G25" s="5">
         <v>3</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="K25" s="5">
         <v>4</v>
@@ -4432,21 +4938,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="G26" s="6">
         <v>3</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="K26" s="6">
         <v>2</v>
@@ -4476,7 +4982,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -4496,7 +5002,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>28</v>
@@ -4541,27 +5047,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -4711,7 +5217,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="L3" s="24">
         <v>5</v>
@@ -4725,7 +5231,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -4772,7 +5278,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -4782,7 +5288,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="H11" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="I11" s="23">
         <v>10</v>
@@ -4790,7 +5296,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="I12" s="23">
         <v>11</v>
@@ -4798,7 +5304,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="I13" s="23">
         <v>11</v>
@@ -4806,7 +5312,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="I14" s="23">
         <v>10</v>
@@ -4822,7 +5328,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="I16" s="21">
         <v>12</v>
@@ -4830,7 +5336,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="I17" s="21">
         <v>12</v>
@@ -4883,7 +5389,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="G25" s="21">
         <v>5</v>
@@ -4892,7 +5398,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -4950,7 +5456,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="H29" s="21">
         <v>7</v>
@@ -5018,7 +5524,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="I35" s="23">
         <v>8</v>
@@ -5027,7 +5533,7 @@
     <row r="37" ht="15.75"/>
     <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -5037,10 +5543,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="I38" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="J38" s="23">
         <v>12</v>
@@ -5048,10 +5554,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="I39" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="J39" s="23">
         <v>12</v>
@@ -5059,10 +5565,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="I40" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="J40" s="21">
         <v>12</v>
@@ -5070,10 +5576,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="I41" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="J41" s="23">
         <v>10</v>
@@ -5081,10 +5587,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="I42" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="J42" s="23">
         <v>10</v>
@@ -5114,17 +5620,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -5149,7 +5655,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="M15" s="5">
         <v>4</v>
@@ -5167,12 +5673,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="M16" s="5">
         <v>12</v>
@@ -5190,12 +5696,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
@@ -5203,10 +5709,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5259,7 +5765,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5315,7 +5821,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>221</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -5371,7 +5877,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>188</v>
+        <v>222</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -5427,7 +5933,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -5483,7 +5989,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -5539,7 +6045,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -5595,17 +6101,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="47" t="s">
-        <v>193</v>
+      <c r="A38" s="46" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="47" t="s">
-        <v>194</v>
+      <c r="A39" s="46" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -5628,7 +6134,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -5677,40 +6183,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="E6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="F6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="G6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="H6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="I6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="J6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="K6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="L6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="M6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="N6" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5721,7 +6227,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5732,7 +6238,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5743,7 +6249,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5754,7 +6260,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>196</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5781,7 +6287,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -5816,7 +6322,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>199</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -5848,10 +6354,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -5891,15 +6397,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>202</v>
+        <v>236</v>
       </c>
       <c r="E12" t="s">
-        <v>203</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -5909,7 +6415,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solved longest palindromic substring
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView windowWidth="27428" windowHeight="11734"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="248">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -411,10 +411,34 @@
     <t>Longest Palindromic Substring</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
+    <t>odd length</t>
+  </si>
+  <si>
+    <t>i=2</t>
+  </si>
+  <si>
+    <t>2-(3-1)/2</t>
+  </si>
+  <si>
+    <t>b or a</t>
+  </si>
+  <si>
+    <t>bab</t>
+  </si>
+  <si>
+    <t>bab or aba</t>
+  </si>
+  <si>
+    <t>2+3/2</t>
+  </si>
+  <si>
+    <t>even length</t>
+  </si>
+  <si>
+    <t>c or b</t>
+  </si>
+  <si>
+    <t>bb</t>
   </si>
   <si>
     <t>n</t>
@@ -749,10 +773,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="26">
@@ -813,22 +837,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -837,22 +860,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -868,7 +875,76 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -876,14 +952,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,52 +967,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -964,7 +988,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,13 +1126,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,79 +1156,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,73 +1168,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1420,11 +1444,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1467,8 +1506,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1502,31 +1541,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1541,131 +1565,131 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1719,6 +1743,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1814,8 +1841,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="929005" y="770255"/>
-          <a:ext cx="4342130" cy="2425700"/>
+          <a:off x="963930" y="747395"/>
+          <a:ext cx="4586605" cy="2357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1861,8 +1888,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1584325" y="723265"/>
-          <a:ext cx="4304030" cy="3704590"/>
+          <a:off x="1647190" y="706120"/>
+          <a:ext cx="4572000" cy="3590290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2136,20 +2163,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z195"/>
+  <dimension ref="A1:Z224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="J197" sqref="J197"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
-    <col min="2" max="2" width="23.0095238095238" customWidth="1"/>
-    <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
-    <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="12.7047619047619" customWidth="1"/>
-    <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
-    <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
+    <col min="2" max="2" width="23.009009009009" customWidth="1"/>
+    <col min="3" max="3" width="8.52252252252252" customWidth="1"/>
+    <col min="4" max="4" width="27.5675675675676" customWidth="1"/>
+    <col min="5" max="5" width="12.7027027027027" customWidth="1"/>
+    <col min="6" max="7" width="12.3153153153153" customWidth="1"/>
+    <col min="8" max="8" width="13.1261261261261" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -2730,26 +2757,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" ht="15.75"/>
-    <row r="67" ht="15.75" spans="7:7">
+    <row r="66" ht="15.3"/>
+    <row r="67" ht="15.3" spans="7:7">
       <c r="G67" s="32"/>
     </row>
-    <row r="68" ht="15.75" spans="6:7">
+    <row r="68" ht="15.3" spans="6:7">
       <c r="F68" s="33"/>
       <c r="G68" s="34"/>
     </row>
-    <row r="69" ht="15.75" spans="5:7">
+    <row r="69" ht="15.3" spans="5:7">
       <c r="E69" s="33"/>
       <c r="F69" s="35"/>
       <c r="G69" s="34"/>
     </row>
-    <row r="70" ht="15.75" spans="4:7">
+    <row r="70" ht="15.3" spans="4:7">
       <c r="D70" s="33"/>
       <c r="E70" s="35"/>
       <c r="F70" s="35"/>
       <c r="G70" s="34"/>
     </row>
-    <row r="71" ht="15.75" spans="2:7">
+    <row r="71" ht="15.3" spans="2:7">
       <c r="B71" s="36"/>
       <c r="C71" s="15"/>
       <c r="D71" s="37"/>
@@ -2822,26 +2849,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" ht="15.75"/>
-    <row r="80" ht="15.75" spans="7:7">
+    <row r="79" ht="15.3"/>
+    <row r="80" ht="15.3" spans="7:7">
       <c r="G80" s="32"/>
     </row>
-    <row r="81" ht="15.75" spans="6:7">
+    <row r="81" ht="15.3" spans="6:7">
       <c r="F81" s="33"/>
       <c r="G81" s="34"/>
     </row>
-    <row r="82" ht="15.75" spans="5:7">
+    <row r="82" ht="15.3" spans="5:7">
       <c r="E82" s="33"/>
       <c r="F82" s="35"/>
       <c r="G82" s="34"/>
     </row>
-    <row r="83" ht="15.75" spans="4:7">
+    <row r="83" ht="15.3" spans="4:7">
       <c r="D83" s="33"/>
       <c r="E83" s="35"/>
       <c r="F83" s="35"/>
       <c r="G83" s="34"/>
     </row>
-    <row r="84" ht="15.75" spans="2:7">
+    <row r="84" ht="15.3" spans="2:7">
       <c r="B84" s="36"/>
       <c r="C84" s="15"/>
       <c r="D84" s="37"/>
@@ -3986,56 +4013,320 @@
         <v>128</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
-      <c r="A194" t="s">
+    <row r="194" spans="1:1">
+      <c r="A194" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" t="s">
         <v>12</v>
       </c>
-      <c r="B194">
-        <v>0</v>
-      </c>
-      <c r="C194">
-        <v>1</v>
-      </c>
-      <c r="D194">
-        <v>2</v>
-      </c>
-      <c r="E194">
-        <v>3</v>
-      </c>
-      <c r="F194">
-        <v>4</v>
-      </c>
-      <c r="I194" t="s">
-        <v>129</v>
-      </c>
-      <c r="J194">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:10">
-      <c r="A195" t="s">
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="E195">
+        <v>3</v>
+      </c>
+      <c r="F195">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9">
+      <c r="A196" t="s">
         <v>33</v>
       </c>
-      <c r="B195" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C195" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D195" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E195" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="F195" s="45" t="s">
+      <c r="B196" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D196" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E196" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F196" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I195" t="s">
+      <c r="I196" t="s">
         <v>130</v>
       </c>
-      <c r="J195">
-        <v>0</v>
+    </row>
+    <row r="197" spans="9:10">
+      <c r="I197" t="s">
+        <v>131</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10">
+      <c r="A198" t="s">
+        <v>41</v>
+      </c>
+      <c r="B198" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C198" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D198" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="E198" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="F198" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="I198" t="s">
+        <v>135</v>
+      </c>
+      <c r="J198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="2:6">
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <v>3</v>
+      </c>
+      <c r="E199">
+        <v>3</v>
+      </c>
+      <c r="F199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" t="s">
+        <v>59</v>
+      </c>
+      <c r="B201" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D201" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" t="s">
+        <v>60</v>
+      </c>
+      <c r="B203" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E203" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" t="s">
+        <v>64</v>
+      </c>
+      <c r="B205" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C205" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D205" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F205" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
+      <c r="A207" t="s">
+        <v>70</v>
+      </c>
+      <c r="B207" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D207" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E207" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="G207" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8">
+      <c r="A209" t="s">
+        <v>78</v>
+      </c>
+      <c r="B209" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D209" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E209" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F209" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H209" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" t="s">
+        <v>12</v>
+      </c>
+      <c r="B212">
+        <v>0</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212">
+        <v>2</v>
+      </c>
+      <c r="E212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" t="s">
+        <v>33</v>
+      </c>
+      <c r="B213" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C213" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D213" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E213" s="45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" t="s">
+        <v>41</v>
+      </c>
+      <c r="B215" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C215" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D215" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E215" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="216" customFormat="1" spans="2:5">
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216">
+        <v>2</v>
+      </c>
+      <c r="E216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" t="s">
+        <v>59</v>
+      </c>
+      <c r="B218" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D218" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" t="s">
+        <v>60</v>
+      </c>
+      <c r="B220" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C220" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E220" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" t="s">
+        <v>64</v>
+      </c>
+      <c r="B222" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C222" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D222" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F222" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7">
+      <c r="A224" t="s">
+        <v>70</v>
+      </c>
+      <c r="B224" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C224" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D224" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E224" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G224" s="25" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4053,11 +4344,11 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -4098,7 +4389,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="B2" s="29">
         <v>0</v>
@@ -4163,7 +4454,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -4172,22 +4463,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -4204,7 +4495,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -4218,7 +4509,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
@@ -4229,7 +4520,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -4249,12 +4540,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -4358,7 +4649,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -4378,17 +4669,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>51</v>
@@ -4400,18 +4691,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -4419,18 +4710,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -4442,7 +4733,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -4450,12 +4741,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -4463,7 +4754,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -4525,7 +4816,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="25" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C51" s="5">
         <v>1</v>
@@ -4559,7 +4850,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -4571,7 +4862,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -4592,19 +4883,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="10" max="10" width="10.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="10.1441441441441" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4697,10 +4988,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -4715,7 +5006,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -4735,7 +5026,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="K11" s="25">
         <v>3</v>
@@ -4762,13 +5053,13 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="F14" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="M14" s="26">
         <v>2</v>
@@ -4776,7 +5067,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="G15" s="25">
         <v>2</v>
@@ -4794,7 +5085,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="G17" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -4802,7 +5093,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="I18" s="25">
         <v>2</v>
@@ -4810,28 +5101,28 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="G20" s="5">
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="K20" s="5">
         <v>3</v>
@@ -4840,21 +5131,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="G21" s="5">
         <v>3</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K21" s="5">
         <v>2</v>
@@ -4863,21 +5154,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="G22" s="6">
         <v>2</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="K22" s="6">
         <v>2</v>
@@ -4885,28 +5176,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C24" s="5">
         <v>3</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="G24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="K24" s="5">
         <v>4</v>
@@ -4915,21 +5206,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="G25" s="5">
         <v>3</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="K25" s="5">
         <v>4</v>
@@ -4938,21 +5229,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="G26" s="6">
         <v>3</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="K26" s="6">
         <v>2</v>
@@ -4973,7 +5264,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -4982,7 +5273,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -5002,7 +5293,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>28</v>
@@ -5047,27 +5338,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -5201,13 +5492,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
     <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="15.047619047619" customWidth="1"/>
+    <col min="6" max="6" width="15.045045045045" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.8095238095238" customWidth="1"/>
-    <col min="9" max="9" width="18.0952380952381" customWidth="1"/>
+    <col min="8" max="8" width="13.8108108108108" customWidth="1"/>
+    <col min="9" max="9" width="18.0990990990991" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -5215,15 +5506,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="2:12">
+    <row r="3" ht="15.3" spans="2:12">
       <c r="B3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="L3" s="24">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="2:12">
+    <row r="4" ht="15.3" spans="2:12">
       <c r="B4" s="11">
         <v>1</v>
       </c>
@@ -5231,10 +5522,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="2:9">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" ht="15.3" spans="2:9">
       <c r="B5" s="12"/>
       <c r="C5" s="13">
         <v>2</v>
@@ -5243,7 +5534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="2:9">
+    <row r="6" ht="15.3" spans="2:9">
       <c r="B6" s="12"/>
       <c r="C6" s="14"/>
       <c r="D6" s="13">
@@ -5253,7 +5544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="2:9">
+    <row r="7" ht="15.3" spans="2:9">
       <c r="B7" s="12"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -5264,7 +5555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="2:9">
+    <row r="8" ht="15.3" spans="2:9">
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -5276,19 +5567,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="2:2">
+    <row r="10" customFormat="1" ht="15.3" spans="2:2">
       <c r="B10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" spans="2:9">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" ht="15.3" spans="2:9">
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="I11" s="23">
         <v>10</v>
@@ -5296,7 +5587,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="I12" s="23">
         <v>11</v>
@@ -5304,7 +5595,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="I13" s="23">
         <v>11</v>
@@ -5312,7 +5603,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="I14" s="23">
         <v>10</v>
@@ -5328,7 +5619,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="I16" s="21">
         <v>12</v>
@@ -5336,7 +5627,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="I17" s="21">
         <v>12</v>
@@ -5350,8 +5641,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.75"/>
-    <row r="22" customFormat="1" ht="15.75" spans="1:5">
+    <row r="21" ht="15.3"/>
+    <row r="22" customFormat="1" ht="15.3" spans="1:5">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -5365,8 +5656,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="15.75"/>
-    <row r="24" customFormat="1" ht="15.75" spans="1:7">
+    <row r="23" ht="15.3"/>
+    <row r="24" customFormat="1" ht="15.3" spans="1:7">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -5389,7 +5680,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="G25" s="21">
         <v>5</v>
@@ -5398,10 +5689,10 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" spans="12:13">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" ht="15.3" spans="12:13">
       <c r="L26">
         <v>1</v>
       </c>
@@ -5409,7 +5700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:13">
+    <row r="27" ht="15.3" spans="1:13">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -5456,7 +5747,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="H29" s="21">
         <v>7</v>
@@ -5476,8 +5767,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" ht="15.75"/>
-    <row r="32" ht="15.75" spans="1:9">
+    <row r="31" ht="15.3"/>
+    <row r="32" ht="15.3" spans="1:9">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -5524,16 +5815,16 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="I35" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="37" ht="15.75"/>
-    <row r="38" ht="15.75" spans="1:10">
+    <row r="37" ht="15.3"/>
+    <row r="38" ht="15.3" spans="1:10">
       <c r="A38" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -5543,10 +5834,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="I38" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="J38" s="23">
         <v>12</v>
@@ -5554,10 +5845,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="I39" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="J39" s="23">
         <v>12</v>
@@ -5565,10 +5856,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="I40" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="J40" s="21">
         <v>12</v>
@@ -5576,10 +5867,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="I41" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="J41" s="23">
         <v>10</v>
@@ -5587,10 +5878,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I42" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="J42" s="23">
         <v>10</v>
@@ -5611,26 +5902,26 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
-    <col min="12" max="12" width="12.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="16.4324324324324" customWidth="1"/>
+    <col min="2" max="2" width="15.2882882882883" customWidth="1"/>
+    <col min="12" max="12" width="12.7117117117117" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -5655,7 +5946,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="M15" s="5">
         <v>4</v>
@@ -5673,12 +5964,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="M16" s="5">
         <v>12</v>
@@ -5696,12 +5987,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
@@ -5709,10 +6000,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5765,7 +6056,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -5821,7 +6112,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -5877,7 +6168,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -5933,7 +6224,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -5989,7 +6280,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -6045,7 +6336,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -6101,17 +6392,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="46" t="s">
-        <v>227</v>
+      <c r="A38" s="47" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="46" t="s">
-        <v>228</v>
+      <c r="A39" s="47" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -6130,11 +6421,11 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60952380952381" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.55"/>
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -6183,40 +6474,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="E6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="F6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="G6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="H6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="I6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="J6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="K6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="L6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="M6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="N6" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6227,7 +6518,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6238,7 +6529,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -6249,7 +6540,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -6260,7 +6551,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -6278,7 +6569,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
@@ -6287,7 +6578,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -6322,7 +6613,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -6354,10 +6645,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -6397,15 +6688,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -6415,7 +6706,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed youtube for longest palindromic substring
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27428" windowHeight="11734"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="253">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -411,13 +411,10 @@
     <t>Longest Palindromic Substring</t>
   </si>
   <si>
-    <t>odd length</t>
-  </si>
-  <si>
-    <t>i=2</t>
-  </si>
-  <si>
-    <t>2-(3-1)/2</t>
+    <t>even length=expand from center with 2 chars as center</t>
+  </si>
+  <si>
+    <t>odd length=expand from center with 1 char as center</t>
   </si>
   <si>
     <t>b or a</t>
@@ -426,19 +423,37 @@
     <t>bab</t>
   </si>
   <si>
-    <t>bab or aba</t>
-  </si>
-  <si>
-    <t>2+3/2</t>
-  </si>
-  <si>
-    <t>even length</t>
-  </si>
-  <si>
-    <t>c or b</t>
-  </si>
-  <si>
-    <t>bb</t>
+    <t>aba or bab</t>
+  </si>
+  <si>
+    <t>L=i</t>
+  </si>
+  <si>
+    <t>i=1</t>
+  </si>
+  <si>
+    <t>R=i</t>
+  </si>
+  <si>
+    <t>R=i+1</t>
+  </si>
+  <si>
+    <t>s[L]==s[R]</t>
+  </si>
+  <si>
+    <t>len=3</t>
+  </si>
+  <si>
+    <t>L=i-1</t>
+  </si>
+  <si>
+    <t>L=2</t>
+  </si>
+  <si>
+    <t>aba</t>
+  </si>
+  <si>
+    <t>R=2</t>
   </si>
   <si>
     <t>n</t>
@@ -773,11 +788,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -830,36 +845,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -875,45 +861,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -927,9 +875,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -937,6 +891,22 @@
     <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -952,7 +922,52 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,7 +982,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -988,7 +1003,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,37 +1039,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,13 +1057,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1066,13 +1081,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1084,25 +1099,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,13 +1129,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,19 +1147,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,7 +1177,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1463,7 +1478,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1487,27 +1502,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1541,16 +1536,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1562,134 +1577,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1746,7 +1761,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
@@ -1841,8 +1858,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="963930" y="747395"/>
-          <a:ext cx="4586605" cy="2357120"/>
+          <a:off x="929005" y="770255"/>
+          <a:ext cx="4342130" cy="2425700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1888,8 +1905,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1647190" y="706120"/>
-          <a:ext cx="4572000" cy="3590290"/>
+          <a:off x="1584325" y="723265"/>
+          <a:ext cx="4304030" cy="3704590"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2163,20 +2180,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z224"/>
+  <dimension ref="A1:Z211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.009009009009" customWidth="1"/>
-    <col min="3" max="3" width="8.52252252252252" customWidth="1"/>
-    <col min="4" max="4" width="27.5675675675676" customWidth="1"/>
-    <col min="5" max="5" width="12.7027027027027" customWidth="1"/>
-    <col min="6" max="7" width="12.3153153153153" customWidth="1"/>
-    <col min="8" max="8" width="13.1261261261261" customWidth="1"/>
+    <col min="2" max="2" width="23.0095238095238" customWidth="1"/>
+    <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
+    <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="12.7047619047619" customWidth="1"/>
+    <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
+    <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -2757,26 +2774,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" ht="15.3"/>
-    <row r="67" ht="15.3" spans="7:7">
+    <row r="66" ht="15.75"/>
+    <row r="67" ht="15.75" spans="7:7">
       <c r="G67" s="32"/>
     </row>
-    <row r="68" ht="15.3" spans="6:7">
+    <row r="68" ht="15.75" spans="6:7">
       <c r="F68" s="33"/>
       <c r="G68" s="34"/>
     </row>
-    <row r="69" ht="15.3" spans="5:7">
+    <row r="69" ht="15.75" spans="5:7">
       <c r="E69" s="33"/>
       <c r="F69" s="35"/>
       <c r="G69" s="34"/>
     </row>
-    <row r="70" ht="15.3" spans="4:7">
+    <row r="70" ht="15.75" spans="4:7">
       <c r="D70" s="33"/>
       <c r="E70" s="35"/>
       <c r="F70" s="35"/>
       <c r="G70" s="34"/>
     </row>
-    <row r="71" ht="15.3" spans="2:7">
+    <row r="71" ht="15.75" spans="2:7">
       <c r="B71" s="36"/>
       <c r="C71" s="15"/>
       <c r="D71" s="37"/>
@@ -2849,26 +2866,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" ht="15.3"/>
-    <row r="80" ht="15.3" spans="7:7">
+    <row r="79" ht="15.75"/>
+    <row r="80" ht="15.75" spans="7:7">
       <c r="G80" s="32"/>
     </row>
-    <row r="81" ht="15.3" spans="6:7">
+    <row r="81" ht="15.75" spans="6:7">
       <c r="F81" s="33"/>
       <c r="G81" s="34"/>
     </row>
-    <row r="82" ht="15.3" spans="5:7">
+    <row r="82" ht="15.75" spans="5:7">
       <c r="E82" s="33"/>
       <c r="F82" s="35"/>
       <c r="G82" s="34"/>
     </row>
-    <row r="83" ht="15.3" spans="4:7">
+    <row r="83" ht="15.75" spans="4:7">
       <c r="D83" s="33"/>
       <c r="E83" s="35"/>
       <c r="F83" s="35"/>
       <c r="G83" s="34"/>
     </row>
-    <row r="84" ht="15.3" spans="2:7">
+    <row r="84" ht="15.75" spans="2:7">
       <c r="B84" s="36"/>
       <c r="C84" s="15"/>
       <c r="D84" s="37"/>
@@ -4013,320 +4030,236 @@
         <v>128</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
-      <c r="A194" s="1" t="s">
+    <row r="194" spans="1:6">
+      <c r="A194" t="s">
+        <v>12</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="E194">
+        <v>3</v>
+      </c>
+      <c r="F194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9">
+      <c r="A195" t="s">
+        <v>33</v>
+      </c>
+      <c r="B195" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D195" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E195" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F195" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I195" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
-      <c r="A195" t="s">
-        <v>12</v>
-      </c>
-      <c r="B195">
-        <v>0</v>
-      </c>
-      <c r="C195">
-        <v>1</v>
-      </c>
-      <c r="D195">
-        <v>2</v>
-      </c>
-      <c r="E195">
-        <v>3</v>
-      </c>
-      <c r="F195">
+    <row r="196" spans="9:9">
+      <c r="I196" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" t="s">
+        <v>41</v>
+      </c>
+      <c r="B197" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D197" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E197" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="F197" s="47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="198" spans="8:13">
+      <c r="H198">
+        <v>0</v>
+      </c>
+      <c r="I198">
+        <v>1</v>
+      </c>
+      <c r="J198">
+        <v>2</v>
+      </c>
+      <c r="K198">
+        <v>3</v>
+      </c>
+      <c r="L198">
         <v>4</v>
       </c>
-    </row>
-    <row r="196" spans="1:9">
-      <c r="A196" t="s">
-        <v>33</v>
-      </c>
-      <c r="B196" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C196" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D196" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E196" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="F196" s="45" t="s">
+      <c r="M198">
         <v>5</v>
       </c>
-      <c r="I196" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="197" spans="9:10">
-      <c r="I197" t="s">
+    </row>
+    <row r="199" spans="1:13">
+      <c r="A199" t="s">
+        <v>59</v>
+      </c>
+      <c r="B199" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199"/>
+      <c r="D199" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E199"/>
+      <c r="F199"/>
+      <c r="H199" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I199" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="J199" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="K199" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="L199" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="M199" s="45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" t="s">
+        <v>60</v>
+      </c>
+      <c r="B201" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D201"/>
+      <c r="E201" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="J197">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10">
-      <c r="A198" t="s">
-        <v>41</v>
-      </c>
-      <c r="B198" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C198" s="46" t="s">
+    </row>
+    <row r="203" spans="1:10">
+      <c r="A203" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D203" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E203"/>
+      <c r="F203" t="s">
+        <v>134</v>
+      </c>
+      <c r="G203" t="s">
+        <v>135</v>
+      </c>
+      <c r="J203" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D198" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="E198" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="F198" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="I198" t="s">
-        <v>135</v>
-      </c>
-      <c r="J198">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="199" spans="2:6">
-      <c r="B199">
-        <v>1</v>
-      </c>
-      <c r="C199">
-        <v>1</v>
-      </c>
-      <c r="D199">
-        <v>3</v>
-      </c>
-      <c r="E199">
-        <v>3</v>
-      </c>
-      <c r="F199">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4">
-      <c r="A201" t="s">
-        <v>59</v>
-      </c>
-      <c r="B201" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D201" s="25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5">
-      <c r="A203" t="s">
-        <v>60</v>
-      </c>
-      <c r="B203" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C203" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="E203" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6">
-      <c r="A205" t="s">
-        <v>64</v>
-      </c>
-      <c r="B205" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C205" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D205" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="F205" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7">
+    </row>
+    <row r="204" spans="6:9">
+      <c r="F204" t="s">
+        <v>136</v>
+      </c>
+      <c r="G204" t="s">
+        <v>137</v>
+      </c>
+      <c r="H204" t="s">
+        <v>138</v>
+      </c>
+      <c r="I204" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="205" spans="7:7">
+      <c r="G205" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8">
       <c r="A207" t="s">
         <v>70</v>
       </c>
-      <c r="B207" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C207" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D207" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E207" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="G207" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8">
-      <c r="A209" t="s">
+      <c r="B207" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D207" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E207" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="G207" t="s">
+        <v>95</v>
+      </c>
+      <c r="H207" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9">
+      <c r="A210" t="s">
         <v>78</v>
       </c>
-      <c r="B209" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C209" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D209" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E209" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="F209" s="45" t="s">
+      <c r="B210" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D210" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E210" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F210" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H209" s="25" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1">
-      <c r="A211" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5">
-      <c r="A212" t="s">
-        <v>12</v>
-      </c>
-      <c r="B212">
-        <v>0</v>
-      </c>
-      <c r="C212">
-        <v>1</v>
-      </c>
-      <c r="D212">
-        <v>2</v>
-      </c>
-      <c r="E212">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5">
-      <c r="A213" t="s">
-        <v>33</v>
-      </c>
-      <c r="B213" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C213" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D213" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E213" s="45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5">
-      <c r="A215" t="s">
-        <v>41</v>
-      </c>
-      <c r="B215" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C215" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D215" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="E215" s="45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="216" customFormat="1" spans="2:5">
-      <c r="B216">
-        <v>1</v>
-      </c>
-      <c r="C216">
-        <v>1</v>
-      </c>
-      <c r="D216">
-        <v>2</v>
-      </c>
-      <c r="E216">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4">
-      <c r="A218" t="s">
-        <v>59</v>
-      </c>
-      <c r="B218" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D218" s="25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5">
-      <c r="A220" t="s">
-        <v>60</v>
-      </c>
-      <c r="B220" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C220" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E220" s="25" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222" t="s">
-        <v>64</v>
-      </c>
-      <c r="B222" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C222" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D222" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="F222" s="25" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="224" spans="1:7">
-      <c r="A224" t="s">
-        <v>70</v>
-      </c>
-      <c r="B224" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C224" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D224" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="E224" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="G224" s="25" t="s">
-        <v>138</v>
+      <c r="H210" t="s">
+        <v>141</v>
+      </c>
+      <c r="I210" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="211" spans="8:8">
+      <c r="H211" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -4344,11 +4277,11 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -4389,7 +4322,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B2" s="29">
         <v>0</v>
@@ -4454,7 +4387,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -4463,22 +4396,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -4495,7 +4428,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -4509,7 +4442,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
@@ -4520,7 +4453,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -4540,12 +4473,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -4649,7 +4582,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -4669,17 +4602,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>51</v>
@@ -4691,18 +4624,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -4710,18 +4643,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -4733,7 +4666,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -4741,12 +4674,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -4754,7 +4687,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -4816,7 +4749,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="25" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C51" s="5">
         <v>1</v>
@@ -4850,7 +4783,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -4862,7 +4795,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -4883,19 +4816,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="10" max="10" width="10.1441441441441" customWidth="1"/>
+    <col min="10" max="10" width="10.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4988,10 +4921,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -5006,7 +4939,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -5026,7 +4959,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="K11" s="25">
         <v>3</v>
@@ -5053,13 +4986,13 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="F14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="M14" s="26">
         <v>2</v>
@@ -5067,7 +5000,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="G15" s="25">
         <v>2</v>
@@ -5085,7 +5018,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="G17" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -5093,7 +5026,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I18" s="25">
         <v>2</v>
@@ -5101,28 +5034,28 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="G20" s="5">
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="K20" s="5">
         <v>3</v>
@@ -5131,21 +5064,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="G21" s="5">
         <v>3</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="K21" s="5">
         <v>2</v>
@@ -5154,21 +5087,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G22" s="6">
         <v>2</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="K22" s="6">
         <v>2</v>
@@ -5176,28 +5109,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C24" s="5">
         <v>3</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="G24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="K24" s="5">
         <v>4</v>
@@ -5206,21 +5139,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="G25" s="5">
         <v>3</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="K25" s="5">
         <v>4</v>
@@ -5229,21 +5162,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G26" s="6">
         <v>3</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="K26" s="6">
         <v>2</v>
@@ -5264,7 +5197,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -5273,7 +5206,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -5293,7 +5226,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>28</v>
@@ -5338,27 +5271,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -5492,13 +5425,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="15.045045045045" customWidth="1"/>
+    <col min="6" max="6" width="15.047619047619" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.8108108108108" customWidth="1"/>
-    <col min="9" max="9" width="18.0990990990991" customWidth="1"/>
+    <col min="8" max="8" width="13.8095238095238" customWidth="1"/>
+    <col min="9" max="9" width="18.0952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -5506,15 +5439,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="15.3" spans="2:12">
+    <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="L3" s="24">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.3" spans="2:12">
+    <row r="4" ht="15.75" spans="2:12">
       <c r="B4" s="11">
         <v>1</v>
       </c>
@@ -5522,10 +5455,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" ht="15.3" spans="2:9">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="2:9">
       <c r="B5" s="12"/>
       <c r="C5" s="13">
         <v>2</v>
@@ -5534,7 +5467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.3" spans="2:9">
+    <row r="6" ht="15.75" spans="2:9">
       <c r="B6" s="12"/>
       <c r="C6" s="14"/>
       <c r="D6" s="13">
@@ -5544,7 +5477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="15.3" spans="2:9">
+    <row r="7" ht="15.75" spans="2:9">
       <c r="B7" s="12"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -5555,7 +5488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="15.3" spans="2:9">
+    <row r="8" ht="15.75" spans="2:9">
       <c r="B8" s="15"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
@@ -5567,19 +5500,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.3" spans="2:2">
+    <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" ht="15.3" spans="2:9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" spans="2:9">
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="H11" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="I11" s="23">
         <v>10</v>
@@ -5587,7 +5520,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="I12" s="23">
         <v>11</v>
@@ -5595,7 +5528,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="I13" s="23">
         <v>11</v>
@@ -5603,7 +5536,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="I14" s="23">
         <v>10</v>
@@ -5619,7 +5552,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="I16" s="21">
         <v>12</v>
@@ -5627,7 +5560,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="I17" s="21">
         <v>12</v>
@@ -5641,8 +5574,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.3"/>
-    <row r="22" customFormat="1" ht="15.3" spans="1:5">
+    <row r="21" ht="15.75"/>
+    <row r="22" customFormat="1" ht="15.75" spans="1:5">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -5656,8 +5589,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="15.3"/>
-    <row r="24" customFormat="1" ht="15.3" spans="1:7">
+    <row r="23" ht="15.75"/>
+    <row r="24" customFormat="1" ht="15.75" spans="1:7">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -5680,7 +5613,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G25" s="21">
         <v>5</v>
@@ -5689,10 +5622,10 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" ht="15.3" spans="12:13">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" spans="12:13">
       <c r="L26">
         <v>1</v>
       </c>
@@ -5700,7 +5633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" ht="15.3" spans="1:13">
+    <row r="27" ht="15.75" spans="1:13">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -5747,7 +5680,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="H29" s="21">
         <v>7</v>
@@ -5767,8 +5700,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" ht="15.3"/>
-    <row r="32" ht="15.3" spans="1:9">
+    <row r="31" ht="15.75"/>
+    <row r="32" ht="15.75" spans="1:9">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -5815,16 +5748,16 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="I35" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="37" ht="15.3"/>
-    <row r="38" ht="15.3" spans="1:10">
+    <row r="37" ht="15.75"/>
+    <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -5834,10 +5767,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="I38" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="J38" s="23">
         <v>12</v>
@@ -5845,10 +5778,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="I39" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="J39" s="23">
         <v>12</v>
@@ -5856,10 +5789,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="I40" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="J40" s="21">
         <v>12</v>
@@ -5867,10 +5800,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="I41" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="J41" s="23">
         <v>10</v>
@@ -5878,10 +5811,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="I42" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="J42" s="23">
         <v>10</v>
@@ -5902,26 +5835,26 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.4324324324324" customWidth="1"/>
-    <col min="2" max="2" width="15.2882882882883" customWidth="1"/>
-    <col min="12" max="12" width="12.7117117117117" customWidth="1"/>
+    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
+    <col min="12" max="12" width="12.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -5946,7 +5879,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="M15" s="5">
         <v>4</v>
@@ -5964,12 +5897,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="M16" s="5">
         <v>12</v>
@@ -5987,12 +5920,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
@@ -6000,10 +5933,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -6056,7 +5989,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6112,7 +6045,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -6168,7 +6101,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -6224,7 +6157,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -6280,7 +6213,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -6336,7 +6269,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -6392,17 +6325,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="47" t="s">
-        <v>235</v>
+      <c r="A38" s="49" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="47" t="s">
-        <v>236</v>
+      <c r="A39" s="49" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -6421,11 +6354,11 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="8.60952380952381" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -6474,40 +6407,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="E6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="G6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="H6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="I6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="J6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="K6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="L6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="M6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="N6" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6518,7 +6451,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6529,7 +6462,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -6540,7 +6473,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -6551,7 +6484,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -6569,7 +6502,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
@@ -6578,7 +6511,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -6613,7 +6546,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -6645,10 +6578,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -6688,15 +6621,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E12" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -6706,7 +6639,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added youtube links for partition problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="267">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -454,6 +454,48 @@
   </si>
   <si>
     <t>R=2</t>
+  </si>
+  <si>
+    <t>Partition Equal Subset Sum</t>
+  </si>
+  <si>
+    <t>sum=22</t>
+  </si>
+  <si>
+    <t>target = sum/2</t>
+  </si>
+  <si>
+    <t>HashSet</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,1,5,6</t>
+  </si>
+  <si>
+    <t>0,1,5,6,11,12,16,17</t>
+  </si>
+  <si>
+    <t>0,1,5,6,11,12,16,17,10,21,22</t>
+  </si>
+  <si>
+    <t>5+0</t>
+  </si>
+  <si>
+    <t>5+1</t>
+  </si>
+  <si>
+    <t>11+0</t>
+  </si>
+  <si>
+    <t>11+1</t>
+  </si>
+  <si>
+    <t>11+5</t>
+  </si>
+  <si>
+    <t>11+6</t>
   </si>
   <si>
     <t>n</t>
@@ -788,11 +830,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -844,24 +886,25 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -872,6 +915,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -890,16 +940,69 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,75 +1017,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1003,13 +1045,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,7 +1069,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,13 +1099,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,7 +1117,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,7 +1129,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,13 +1141,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1099,79 +1213,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1498,30 +1540,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1556,16 +1574,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1577,134 +1619,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1761,11 +1803,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2180,10 +2227,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z211"/>
+  <dimension ref="A1:Z244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="D217" sqref="D217"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="E228" sqref="E228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2191,7 +2238,7 @@
     <col min="2" max="2" width="23.0095238095238" customWidth="1"/>
     <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
     <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="12.7047619047619" customWidth="1"/>
+    <col min="5" max="5" width="26.2857142857143" customWidth="1"/>
     <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
     <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
   </cols>
@@ -4082,19 +4129,19 @@
       <c r="A197" t="s">
         <v>41</v>
       </c>
-      <c r="B197" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C197" s="46" t="s">
+      <c r="B197" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D197" s="46" t="s">
+      <c r="D197" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E197" s="46" t="s">
+      <c r="E197" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F197" s="47" t="s">
+      <c r="F197" s="28" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4122,15 +4169,12 @@
       <c r="A199" t="s">
         <v>59</v>
       </c>
-      <c r="B199" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C199"/>
+      <c r="B199" s="46" t="s">
+        <v>3</v>
+      </c>
       <c r="D199" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E199"/>
-      <c r="F199"/>
       <c r="H199" s="45" t="s">
         <v>31</v>
       </c>
@@ -4154,13 +4198,12 @@
       <c r="A201" t="s">
         <v>60</v>
       </c>
-      <c r="B201" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C201" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D201"/>
+      <c r="B201" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="46" t="s">
+        <v>2</v>
+      </c>
       <c r="E201" s="25" t="s">
         <v>131</v>
       </c>
@@ -4169,16 +4212,15 @@
       <c r="A203" t="s">
         <v>64</v>
       </c>
-      <c r="B203" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C203" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D203" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E203"/>
+      <c r="B203" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D203" s="46" t="s">
+        <v>3</v>
+      </c>
       <c r="F203" t="s">
         <v>134</v>
       </c>
@@ -4212,16 +4254,16 @@
       <c r="A207" t="s">
         <v>70</v>
       </c>
-      <c r="B207" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C207" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D207" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E207" s="48" t="s">
+      <c r="B207" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D207" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E207" s="46" t="s">
         <v>2</v>
       </c>
       <c r="G207" t="s">
@@ -4235,19 +4277,19 @@
       <c r="A210" t="s">
         <v>78</v>
       </c>
-      <c r="B210" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C210" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D210" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E210" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F210" s="48" t="s">
+      <c r="B210" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D210" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E210" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F210" s="46" t="s">
         <v>5</v>
       </c>
       <c r="H210" t="s">
@@ -4260,6 +4302,208 @@
     <row r="211" spans="8:8">
       <c r="H211" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" t="s">
+        <v>12</v>
+      </c>
+      <c r="B221">
+        <v>0</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="E221">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" t="s">
+        <v>13</v>
+      </c>
+      <c r="B222" s="47">
+        <v>1</v>
+      </c>
+      <c r="C222" s="47">
+        <v>5</v>
+      </c>
+      <c r="D222" s="47">
+        <v>11</v>
+      </c>
+      <c r="E222" s="47">
+        <v>5</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="223" spans="7:9">
+      <c r="G223" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I223" s="53">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" t="s">
+        <v>147</v>
+      </c>
+      <c r="B225" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C225" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D225" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="E225" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227" t="s">
+        <v>59</v>
+      </c>
+      <c r="B227" s="48">
+        <v>1</v>
+      </c>
+      <c r="D227" s="25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" t="s">
+        <v>60</v>
+      </c>
+      <c r="B229" s="48">
+        <v>1</v>
+      </c>
+      <c r="C229" s="49">
+        <v>5</v>
+      </c>
+      <c r="E229" t="s">
+        <v>152</v>
+      </c>
+      <c r="F229" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="5:6">
+      <c r="E230" t="s">
+        <v>153</v>
+      </c>
+      <c r="F230" s="50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="A232" t="s">
+        <v>64</v>
+      </c>
+      <c r="B232" s="48">
+        <v>1</v>
+      </c>
+      <c r="C232" s="48">
+        <v>5</v>
+      </c>
+      <c r="D232" s="49">
+        <v>11</v>
+      </c>
+      <c r="F232" t="s">
+        <v>154</v>
+      </c>
+      <c r="G232" s="51">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="233" spans="6:7">
+      <c r="F233" t="s">
+        <v>155</v>
+      </c>
+      <c r="G233">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="234" spans="6:7">
+      <c r="F234" t="s">
+        <v>156</v>
+      </c>
+      <c r="G234">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235" spans="6:7">
+      <c r="F235" t="s">
+        <v>157</v>
+      </c>
+      <c r="G235">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
+      <c r="A237" t="s">
+        <v>70</v>
+      </c>
+      <c r="B237" s="48">
+        <v>1</v>
+      </c>
+      <c r="C237" s="48">
+        <v>5</v>
+      </c>
+      <c r="D237" s="48">
+        <v>11</v>
+      </c>
+      <c r="E237" s="49">
+        <v>5</v>
+      </c>
+      <c r="G237" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="238" spans="7:7">
+      <c r="G238">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="239" spans="7:7">
+      <c r="G239" s="52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="7:7">
+      <c r="G240">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="241" spans="7:7">
+      <c r="G241">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="242" spans="7:7">
+      <c r="G242">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="243" spans="7:7">
+      <c r="G243" s="52">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="244" spans="7:7">
+      <c r="G244" s="52">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4281,7 +4525,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -4322,7 +4566,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B2" s="29">
         <v>0</v>
@@ -4396,22 +4640,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>2</v>
@@ -4428,7 +4672,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -4442,7 +4686,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
@@ -4453,7 +4697,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -4473,12 +4717,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -4582,7 +4826,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -4602,17 +4846,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>51</v>
@@ -4624,18 +4868,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -4643,18 +4887,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -4666,7 +4910,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -4674,12 +4918,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -4687,7 +4931,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -4749,7 +4993,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="25" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C51" s="5">
         <v>1</v>
@@ -4783,7 +5027,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -4795,7 +5039,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -4823,12 +5067,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4921,10 +5165,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -4939,7 +5183,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -4959,7 +5203,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="K11" s="25">
         <v>3</v>
@@ -4986,13 +5230,13 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="M14" s="26">
         <v>2</v>
@@ -5000,7 +5244,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="G15" s="25">
         <v>2</v>
@@ -5018,7 +5262,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="G17" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -5026,7 +5270,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="I18" s="25">
         <v>2</v>
@@ -5034,28 +5278,28 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="G20" s="5">
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="K20" s="5">
         <v>3</v>
@@ -5064,21 +5308,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="C21" s="5">
         <v>3</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="G21" s="5">
         <v>3</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="K21" s="5">
         <v>2</v>
@@ -5087,21 +5331,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G22" s="6">
         <v>2</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="K22" s="6">
         <v>2</v>
@@ -5109,28 +5353,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C24" s="5">
         <v>3</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="G24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="K24" s="5">
         <v>4</v>
@@ -5139,21 +5383,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="G25" s="5">
         <v>3</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="K25" s="5">
         <v>4</v>
@@ -5162,21 +5406,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="G26" s="6">
         <v>3</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="K26" s="6">
         <v>2</v>
@@ -5206,7 +5450,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>31</v>
@@ -5226,7 +5470,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>28</v>
@@ -5271,27 +5515,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -5441,7 +5685,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="L3" s="24">
         <v>5</v>
@@ -5455,7 +5699,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -5502,7 +5746,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -5512,7 +5756,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="H11" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="I11" s="23">
         <v>10</v>
@@ -5520,7 +5764,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="I12" s="23">
         <v>11</v>
@@ -5528,7 +5772,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="I13" s="23">
         <v>11</v>
@@ -5536,7 +5780,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="I14" s="23">
         <v>10</v>
@@ -5552,7 +5796,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="I16" s="21">
         <v>12</v>
@@ -5560,7 +5804,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="I17" s="21">
         <v>12</v>
@@ -5613,7 +5857,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="G25" s="21">
         <v>5</v>
@@ -5622,7 +5866,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -5680,7 +5924,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="H29" s="21">
         <v>7</v>
@@ -5748,7 +5992,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
       <c r="I35" s="23">
         <v>8</v>
@@ -5757,7 +6001,7 @@
     <row r="37" ht="15.75"/>
     <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="19"/>
@@ -5767,10 +6011,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="I38" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="J38" s="23">
         <v>12</v>
@@ -5778,10 +6022,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="J39" s="23">
         <v>12</v>
@@ -5789,10 +6033,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="I40" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="J40" s="21">
         <v>12</v>
@@ -5800,10 +6044,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="I41" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="J41" s="23">
         <v>10</v>
@@ -5811,10 +6055,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="I42" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="J42" s="23">
         <v>10</v>
@@ -5844,17 +6088,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -5879,7 +6123,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="M15" s="5">
         <v>4</v>
@@ -5897,12 +6141,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="M16" s="5">
         <v>12</v>
@@ -5920,12 +6164,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="M19" s="8">
         <v>15</v>
@@ -5933,10 +6177,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5989,7 +6233,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -6045,7 +6289,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -6101,7 +6345,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -6157,7 +6401,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -6213,7 +6457,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -6269,7 +6513,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -6325,17 +6569,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="49" t="s">
-        <v>240</v>
+      <c r="A38" s="54" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="49" t="s">
-        <v>241</v>
+      <c r="A39" s="54" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -6358,7 +6602,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -6407,40 +6651,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="D6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="E6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="F6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="G6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="H6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="I6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="J6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="K6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="L6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="M6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="N6" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6451,7 +6695,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6462,7 +6706,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -6473,7 +6717,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -6484,7 +6728,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -6511,7 +6755,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -6546,7 +6790,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -6578,10 +6822,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -6621,15 +6865,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="E12" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -6639,7 +6883,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed Paint House problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" activeTab="9"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="380">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -605,6 +605,51 @@
   </si>
   <si>
     <t>i&lt;=j&lt;k</t>
+  </si>
+  <si>
+    <t>PaintHouse</t>
+  </si>
+  <si>
+    <t>house[i]</t>
+  </si>
+  <si>
+    <t>[14,2,11]</t>
+  </si>
+  <si>
+    <t>[11,14,5]</t>
+  </si>
+  <si>
+    <t>[14,3,10]</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>11+min(2,11)=13</t>
+  </si>
+  <si>
+    <t>14+11=25</t>
+  </si>
+  <si>
+    <t>5+2=7</t>
+  </si>
+  <si>
+    <t>14+7=21</t>
+  </si>
+  <si>
+    <t>3+7=10</t>
+  </si>
+  <si>
+    <t>10+13=23</t>
   </si>
   <si>
     <t>fib(n)</t>
@@ -1125,11 +1170,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1181,8 +1226,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1195,9 +1241,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1206,13 +1274,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1241,24 +1302,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1282,7 +1328,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1290,6 +1336,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1304,28 +1364,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1340,19 +1385,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1364,115 +1433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1490,7 +1451,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1502,25 +1571,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1997,17 +2054,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2036,26 +2098,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2075,35 +2137,30 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2115,134 +2172,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2272,8 +2329,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2336,7 +2391,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2353,7 +2407,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2362,8 +2415,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2778,16 +2836,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z289"/>
+  <dimension ref="A1:Z303"/>
   <sheetViews>
-    <sheetView topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="J288" sqref="J288:P289"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="B305" sqref="B305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.0095238095238" customWidth="1"/>
-    <col min="3" max="3" width="8.52380952380952" customWidth="1"/>
+    <col min="1" max="1" width="12.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="12.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="26.2857142857143" customWidth="1"/>
     <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
@@ -2859,7 +2918,7 @@
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="31">
         <f>IF($B$8=C$7,1+D9,MAX(C9,D8))</f>
         <v>3</v>
       </c>
@@ -3005,7 +3064,7 @@
       <c r="I22">
         <v>7</v>
       </c>
-      <c r="J22" s="55" t="s">
+      <c r="J22" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3037,7 +3096,7 @@
       <c r="I23" s="15">
         <v>18</v>
       </c>
-      <c r="J23" s="55" t="s">
+      <c r="J23" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3051,7 +3110,7 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="28">
+      <c r="D25" s="25">
         <v>4</v>
       </c>
       <c r="E25">
@@ -3254,7 +3313,7 @@
       <c r="E46" s="15">
         <v>4</v>
       </c>
-      <c r="F46" s="33">
+      <c r="F46" s="31">
         <v>3</v>
       </c>
     </row>
@@ -3299,28 +3358,28 @@
       <c r="A53" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="54" t="s">
+      <c r="C53" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="54" t="s">
+      <c r="D53" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="54" t="s">
+      <c r="E53" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="F53" s="54" t="s">
+      <c r="F53" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="54" t="s">
+      <c r="G53" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H53" s="54" t="s">
+      <c r="H53" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="54" t="s">
+      <c r="I53" s="52" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3328,7 +3387,7 @@
       <c r="A55" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="28" t="b">
+      <c r="B55" s="25" t="b">
         <v>1</v>
       </c>
       <c r="C55" t="b">
@@ -3360,7 +3419,7 @@
       <c r="B57" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="29" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3376,30 +3435,30 @@
     </row>
     <row r="66" ht="15.75"/>
     <row r="67" ht="15.75" spans="7:7">
-      <c r="G67" s="56"/>
+      <c r="G67" s="54"/>
     </row>
     <row r="68" ht="15.75" spans="6:7">
-      <c r="F68" s="57"/>
-      <c r="G68" s="58"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="56"/>
     </row>
     <row r="69" ht="15.75" spans="5:7">
-      <c r="E69" s="57"/>
-      <c r="F69" s="59"/>
-      <c r="G69" s="58"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="57"/>
+      <c r="G69" s="56"/>
     </row>
     <row r="70" ht="15.75" spans="4:7">
-      <c r="D70" s="57"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="59"/>
-      <c r="G70" s="58"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="57"/>
+      <c r="F70" s="57"/>
+      <c r="G70" s="56"/>
     </row>
     <row r="71" ht="15.75" spans="2:7">
-      <c r="B71" s="27"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
-      <c r="F71" s="60"/>
-      <c r="G71" s="61"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="59"/>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
@@ -3428,7 +3487,7 @@
       <c r="A74" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="28">
+      <c r="B74" s="25">
         <v>8</v>
       </c>
       <c r="C74">
@@ -3468,30 +3527,30 @@
     </row>
     <row r="79" ht="15.75"/>
     <row r="80" ht="15.75" spans="7:7">
-      <c r="G80" s="56"/>
+      <c r="G80" s="54"/>
     </row>
     <row r="81" ht="15.75" spans="6:7">
-      <c r="F81" s="57"/>
-      <c r="G81" s="58"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="56"/>
     </row>
     <row r="82" ht="15.75" spans="5:7">
-      <c r="E82" s="57"/>
-      <c r="F82" s="59"/>
-      <c r="G82" s="58"/>
+      <c r="E82" s="55"/>
+      <c r="F82" s="57"/>
+      <c r="G82" s="56"/>
     </row>
     <row r="83" ht="15.75" spans="4:7">
-      <c r="D83" s="57"/>
-      <c r="E83" s="59"/>
-      <c r="F83" s="59"/>
-      <c r="G83" s="58"/>
+      <c r="D83" s="55"/>
+      <c r="E83" s="57"/>
+      <c r="F83" s="57"/>
+      <c r="G83" s="56"/>
     </row>
     <row r="84" ht="15.75" spans="2:7">
-      <c r="B84" s="27"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="60"/>
-      <c r="E84" s="60"/>
-      <c r="F84" s="60"/>
-      <c r="G84" s="61"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="58"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="59"/>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
@@ -3520,7 +3579,7 @@
       <c r="A87" t="s">
         <v>41</v>
       </c>
-      <c r="B87" s="28">
+      <c r="B87" s="25">
         <v>13</v>
       </c>
       <c r="C87">
@@ -3585,13 +3644,13 @@
       <c r="B96" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="62">
+      <c r="C96" s="60">
         <v>4</v>
       </c>
-      <c r="D96" s="63">
-        <v>3</v>
-      </c>
-      <c r="E96" s="63">
+      <c r="D96" s="61">
+        <v>3</v>
+      </c>
+      <c r="E96" s="61">
         <v>3</v>
       </c>
       <c r="F96" s="15">
@@ -3614,13 +3673,13 @@
       <c r="B97" t="s">
         <v>51</v>
       </c>
-      <c r="C97" s="63">
+      <c r="C97" s="61">
         <v>4</v>
       </c>
-      <c r="D97" s="63">
-        <v>3</v>
-      </c>
-      <c r="E97" s="63">
+      <c r="D97" s="61">
+        <v>3</v>
+      </c>
+      <c r="E97" s="61">
         <v>3</v>
       </c>
       <c r="F97" s="15">
@@ -3643,13 +3702,13 @@
       <c r="B98" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="63">
+      <c r="C98" s="61">
         <v>4</v>
       </c>
-      <c r="D98" s="63">
-        <v>3</v>
-      </c>
-      <c r="E98" s="63">
+      <c r="D98" s="61">
+        <v>3</v>
+      </c>
+      <c r="E98" s="61">
         <v>3</v>
       </c>
       <c r="F98" s="15">
@@ -3800,13 +3859,13 @@
       </c>
     </row>
     <row r="111" spans="7:7">
-      <c r="G111" s="64"/>
+      <c r="G111" s="62"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>57</v>
       </c>
-      <c r="B112" s="63">
+      <c r="B112" s="61">
         <v>1</v>
       </c>
       <c r="C112" s="15">
@@ -3901,7 +3960,7 @@
       <c r="A118" t="s">
         <v>60</v>
       </c>
-      <c r="B118" s="63">
+      <c r="B118" s="61">
         <v>1</v>
       </c>
       <c r="D118" t="s">
@@ -3910,7 +3969,7 @@
       <c r="E118" t="s">
         <v>62</v>
       </c>
-      <c r="F118" s="28">
+      <c r="F118" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3923,7 +3982,7 @@
       <c r="A121" t="s">
         <v>64</v>
       </c>
-      <c r="B121" s="63">
+      <c r="B121" s="61">
         <v>1</v>
       </c>
       <c r="C121" s="15">
@@ -3938,7 +3997,7 @@
       <c r="G121">
         <v>2</v>
       </c>
-      <c r="H121" s="28">
+      <c r="H121" s="25">
         <v>5</v>
       </c>
     </row>
@@ -3963,7 +4022,7 @@
       <c r="A124" t="s">
         <v>70</v>
       </c>
-      <c r="B124" s="63">
+      <c r="B124" s="61">
         <v>1</v>
       </c>
       <c r="C124" s="15">
@@ -3981,7 +4040,7 @@
       <c r="H124">
         <v>6</v>
       </c>
-      <c r="I124" s="28">
+      <c r="I124" s="25">
         <v>8</v>
       </c>
     </row>
@@ -4020,7 +4079,7 @@
       <c r="A128" t="s">
         <v>78</v>
       </c>
-      <c r="B128" s="63">
+      <c r="B128" s="61">
         <v>1</v>
       </c>
       <c r="C128" s="15">
@@ -4041,7 +4100,7 @@
       <c r="I128">
         <v>9</v>
       </c>
-      <c r="J128" s="28">
+      <c r="J128" s="25">
         <v>10</v>
       </c>
     </row>
@@ -4101,7 +4160,7 @@
       </c>
     </row>
     <row r="141" customFormat="1" spans="1:1">
-      <c r="A141" s="31" t="s">
+      <c r="A141" s="29" t="s">
         <v>90</v>
       </c>
     </row>
@@ -4149,10 +4208,10 @@
       <c r="A146" t="s">
         <v>59</v>
       </c>
-      <c r="B146" s="34">
-        <v>2</v>
-      </c>
-      <c r="D146" s="28">
+      <c r="B146" s="32">
+        <v>2</v>
+      </c>
+      <c r="D146" s="25">
         <v>2</v>
       </c>
     </row>
@@ -4160,13 +4219,13 @@
       <c r="A148" t="s">
         <v>60</v>
       </c>
-      <c r="B148" s="34">
-        <v>2</v>
-      </c>
-      <c r="C148" s="34">
+      <c r="B148" s="32">
+        <v>2</v>
+      </c>
+      <c r="C148" s="32">
         <v>7</v>
       </c>
-      <c r="E148" s="28">
+      <c r="E148" s="25">
         <v>7</v>
       </c>
     </row>
@@ -4174,19 +4233,19 @@
       <c r="A150" t="s">
         <v>64</v>
       </c>
-      <c r="B150" s="34">
-        <v>2</v>
-      </c>
-      <c r="C150" s="34">
+      <c r="B150" s="32">
+        <v>2</v>
+      </c>
+      <c r="C150" s="32">
         <v>7</v>
       </c>
-      <c r="D150" s="34">
+      <c r="D150" s="32">
         <v>9</v>
       </c>
       <c r="F150" t="s">
         <v>91</v>
       </c>
-      <c r="G150" s="28">
+      <c r="G150" s="25">
         <v>11</v>
       </c>
     </row>
@@ -4202,16 +4261,16 @@
       <c r="A153" t="s">
         <v>70</v>
       </c>
-      <c r="B153" s="34">
-        <v>2</v>
-      </c>
-      <c r="C153" s="34">
+      <c r="B153" s="32">
+        <v>2</v>
+      </c>
+      <c r="C153" s="32">
         <v>7</v>
       </c>
-      <c r="D153" s="34">
+      <c r="D153" s="32">
         <v>9</v>
       </c>
-      <c r="E153" s="34">
+      <c r="E153" s="32">
         <v>3</v>
       </c>
       <c r="G153" t="s">
@@ -4228,7 +4287,7 @@
       <c r="G154" t="s">
         <v>94</v>
       </c>
-      <c r="H154" s="28">
+      <c r="H154" s="25">
         <v>11</v>
       </c>
       <c r="J154" s="1" t="s">
@@ -4239,25 +4298,25 @@
       <c r="A156" t="s">
         <v>78</v>
       </c>
-      <c r="B156" s="34">
-        <v>2</v>
-      </c>
-      <c r="C156" s="34">
+      <c r="B156" s="32">
+        <v>2</v>
+      </c>
+      <c r="C156" s="32">
         <v>7</v>
       </c>
-      <c r="D156" s="34">
+      <c r="D156" s="32">
         <v>9</v>
       </c>
-      <c r="E156" s="34">
-        <v>3</v>
-      </c>
-      <c r="F156" s="34">
+      <c r="E156" s="32">
+        <v>3</v>
+      </c>
+      <c r="F156" s="32">
         <v>1</v>
       </c>
       <c r="H156" t="s">
         <v>96</v>
       </c>
-      <c r="J156" s="28">
+      <c r="J156" s="25">
         <v>12</v>
       </c>
     </row>
@@ -4275,7 +4334,7 @@
       </c>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="31" t="s">
+      <c r="A164" s="29" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4314,36 +4373,36 @@
       </c>
     </row>
     <row r="168" spans="2:5">
-      <c r="B168" s="65">
-        <v>2</v>
-      </c>
-      <c r="C168" s="65">
-        <v>3</v>
-      </c>
-      <c r="D168" s="65">
+      <c r="B168" s="63">
+        <v>2</v>
+      </c>
+      <c r="C168" s="63">
+        <v>3</v>
+      </c>
+      <c r="D168" s="63">
         <v>-2</v>
       </c>
-      <c r="E168" s="28">
+      <c r="E168" s="25">
         <v>-4</v>
       </c>
     </row>
     <row r="169" spans="2:5">
-      <c r="B169" s="65"/>
-      <c r="C169" s="65"/>
-      <c r="D169" s="65"/>
-      <c r="E169" s="65"/>
+      <c r="B169" s="63"/>
+      <c r="C169" s="63"/>
+      <c r="D169" s="63"/>
+      <c r="E169" s="63"/>
     </row>
     <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>41</v>
       </c>
-      <c r="B170" s="50">
+      <c r="B170" s="48">
         <v>4</v>
       </c>
-      <c r="C170" s="50">
+      <c r="C170" s="48">
         <v>6</v>
       </c>
-      <c r="D170" s="50">
+      <c r="D170" s="48">
         <v>6</v>
       </c>
       <c r="E170" s="15">
@@ -4354,7 +4413,7 @@
       </c>
     </row>
     <row r="171" spans="8:14">
-      <c r="H171" s="66">
+      <c r="H171" s="64">
         <v>6</v>
       </c>
       <c r="M171" s="1" t="s">
@@ -4402,7 +4461,7 @@
       <c r="A175" t="s">
         <v>59</v>
       </c>
-      <c r="B175" s="34">
+      <c r="B175" s="32">
         <v>2</v>
       </c>
       <c r="D175" t="s">
@@ -4420,7 +4479,7 @@
       <c r="K175" t="s">
         <v>105</v>
       </c>
-      <c r="M175" s="28">
+      <c r="M175" s="25">
         <v>4</v>
       </c>
     </row>
@@ -4442,10 +4501,10 @@
       <c r="A178" t="s">
         <v>60</v>
       </c>
-      <c r="B178" s="34">
-        <v>2</v>
-      </c>
-      <c r="C178" s="34">
+      <c r="B178" s="32">
+        <v>2</v>
+      </c>
+      <c r="C178" s="32">
         <v>3</v>
       </c>
       <c r="E178" t="s">
@@ -4463,10 +4522,10 @@
       <c r="L178" t="s">
         <v>110</v>
       </c>
-      <c r="N178" s="28">
+      <c r="N178" s="25">
         <v>6</v>
       </c>
-      <c r="Z178" s="28">
+      <c r="Z178" s="25">
         <v>4</v>
       </c>
     </row>
@@ -4488,13 +4547,13 @@
       <c r="A181" t="s">
         <v>64</v>
       </c>
-      <c r="B181" s="34">
-        <v>2</v>
-      </c>
-      <c r="C181" s="34">
-        <v>3</v>
-      </c>
-      <c r="D181" s="34">
+      <c r="B181" s="32">
+        <v>2</v>
+      </c>
+      <c r="C181" s="32">
+        <v>3</v>
+      </c>
+      <c r="D181" s="32">
         <v>-2</v>
       </c>
       <c r="F181" t="s">
@@ -4512,7 +4571,7 @@
       <c r="N181" t="s">
         <v>115</v>
       </c>
-      <c r="P181" s="28">
+      <c r="P181" s="25">
         <v>6</v>
       </c>
     </row>
@@ -4534,16 +4593,16 @@
       <c r="A184" t="s">
         <v>70</v>
       </c>
-      <c r="B184" s="34">
-        <v>2</v>
-      </c>
-      <c r="C184" s="34">
-        <v>3</v>
-      </c>
-      <c r="D184" s="34">
+      <c r="B184" s="32">
+        <v>2</v>
+      </c>
+      <c r="C184" s="32">
+        <v>3</v>
+      </c>
+      <c r="D184" s="32">
         <v>-2</v>
       </c>
-      <c r="E184" s="34">
+      <c r="E184" s="32">
         <v>4</v>
       </c>
       <c r="G184" t="s">
@@ -4561,7 +4620,7 @@
       <c r="O184" t="s">
         <v>120</v>
       </c>
-      <c r="Q184" s="28">
+      <c r="Q184" s="25">
         <v>6</v>
       </c>
     </row>
@@ -4580,16 +4639,16 @@
       </c>
     </row>
     <row r="187" spans="2:17">
-      <c r="B187" s="34">
-        <v>2</v>
-      </c>
-      <c r="C187" s="34">
-        <v>3</v>
-      </c>
-      <c r="D187" s="34">
+      <c r="B187" s="32">
+        <v>2</v>
+      </c>
+      <c r="C187" s="32">
+        <v>3</v>
+      </c>
+      <c r="D187" s="32">
         <v>-2</v>
       </c>
-      <c r="E187" s="52">
+      <c r="E187" s="50">
         <v>-4</v>
       </c>
       <c r="G187" t="s">
@@ -4694,7 +4753,7 @@
       <c r="E197" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="F197" s="52" t="s">
+      <c r="F197" s="50" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4722,10 +4781,10 @@
       <c r="A199" t="s">
         <v>59</v>
       </c>
-      <c r="B199" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="D199" s="28" t="s">
+      <c r="B199" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D199" s="25" t="s">
         <v>3</v>
       </c>
       <c r="H199" s="10" t="s">
@@ -4751,13 +4810,13 @@
       <c r="A201" t="s">
         <v>60</v>
       </c>
-      <c r="B201" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C201" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="E201" s="28" t="s">
+      <c r="B201" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E201" s="25" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4765,13 +4824,13 @@
       <c r="A203" t="s">
         <v>64</v>
       </c>
-      <c r="B203" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C203" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="D203" s="67" t="s">
+      <c r="B203" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D203" s="65" t="s">
         <v>3</v>
       </c>
       <c r="F203" t="s">
@@ -4780,7 +4839,7 @@
       <c r="G203" t="s">
         <v>135</v>
       </c>
-      <c r="J203" s="28" t="s">
+      <c r="J203" s="25" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4807,22 +4866,22 @@
       <c r="A207" t="s">
         <v>70</v>
       </c>
-      <c r="B207" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C207" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="D207" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="E207" s="67" t="s">
+      <c r="B207" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D207" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E207" s="65" t="s">
         <v>2</v>
       </c>
       <c r="G207" t="s">
         <v>95</v>
       </c>
-      <c r="H207" s="28" t="s">
+      <c r="H207" s="25" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4830,25 +4889,25 @@
       <c r="A210" t="s">
         <v>78</v>
       </c>
-      <c r="B210" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C210" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="D210" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="E210" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="F210" s="67" t="s">
+      <c r="B210" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D210" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E210" s="65" t="s">
+        <v>2</v>
+      </c>
+      <c r="F210" s="65" t="s">
         <v>5</v>
       </c>
       <c r="H210" t="s">
         <v>141</v>
       </c>
-      <c r="I210" s="28" t="s">
+      <c r="I210" s="25" t="s">
         <v>142</v>
       </c>
     </row>
@@ -4928,10 +4987,10 @@
       <c r="A227" t="s">
         <v>59</v>
       </c>
-      <c r="B227" s="34">
-        <v>1</v>
-      </c>
-      <c r="D227" s="28" t="s">
+      <c r="B227" s="32">
+        <v>1</v>
+      </c>
+      <c r="D227" s="25" t="s">
         <v>148</v>
       </c>
     </row>
@@ -4939,16 +4998,16 @@
       <c r="A229" t="s">
         <v>60</v>
       </c>
-      <c r="B229" s="34">
-        <v>1</v>
-      </c>
-      <c r="C229" s="52">
+      <c r="B229" s="32">
+        <v>1</v>
+      </c>
+      <c r="C229" s="50">
         <v>5</v>
       </c>
       <c r="E229" t="s">
         <v>152</v>
       </c>
-      <c r="F229" s="28">
+      <c r="F229" s="25">
         <v>5</v>
       </c>
     </row>
@@ -4956,7 +5015,7 @@
       <c r="E230" t="s">
         <v>153</v>
       </c>
-      <c r="F230" s="28">
+      <c r="F230" s="25">
         <v>6</v>
       </c>
     </row>
@@ -4964,19 +5023,19 @@
       <c r="A232" t="s">
         <v>64</v>
       </c>
-      <c r="B232" s="34">
-        <v>1</v>
-      </c>
-      <c r="C232" s="34">
+      <c r="B232" s="32">
+        <v>1</v>
+      </c>
+      <c r="C232" s="32">
         <v>5</v>
       </c>
-      <c r="D232" s="52">
+      <c r="D232" s="50">
         <v>11</v>
       </c>
       <c r="F232" t="s">
         <v>154</v>
       </c>
-      <c r="G232" s="68">
+      <c r="G232" s="66">
         <v>11</v>
       </c>
     </row>
@@ -5008,16 +5067,16 @@
       <c r="A237" t="s">
         <v>70</v>
       </c>
-      <c r="B237" s="34">
-        <v>1</v>
-      </c>
-      <c r="C237" s="34">
+      <c r="B237" s="32">
+        <v>1</v>
+      </c>
+      <c r="C237" s="32">
         <v>5</v>
       </c>
-      <c r="D237" s="34">
+      <c r="D237" s="32">
         <v>11</v>
       </c>
-      <c r="E237" s="52">
+      <c r="E237" s="50">
         <v>5</v>
       </c>
       <c r="G237" t="s">
@@ -5068,15 +5127,15 @@
       <c r="A250" s="1"/>
     </row>
     <row r="251" ht="15.75" spans="1:10">
-      <c r="A251" s="69" t="s">
+      <c r="A251" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="B251" s="70" t="s">
+      <c r="B251" s="68" t="s">
         <v>160</v>
       </c>
-      <c r="C251" s="71"/>
-      <c r="D251" s="71"/>
-      <c r="E251" s="72"/>
+      <c r="C251" s="69"/>
+      <c r="D251" s="69"/>
+      <c r="E251" s="70"/>
       <c r="G251" s="1" t="s">
         <v>161</v>
       </c>
@@ -5088,16 +5147,16 @@
       <c r="A252" s="1">
         <v>0</v>
       </c>
-      <c r="B252" s="51">
-        <v>0</v>
-      </c>
-      <c r="C252" s="51">
-        <v>0</v>
-      </c>
-      <c r="D252" s="51">
-        <v>0</v>
-      </c>
-      <c r="E252" s="51">
+      <c r="B252" s="49">
+        <v>0</v>
+      </c>
+      <c r="C252" s="49">
+        <v>0</v>
+      </c>
+      <c r="D252" s="49">
+        <v>0</v>
+      </c>
+      <c r="E252" s="49">
         <v>0</v>
       </c>
       <c r="G252">
@@ -5105,25 +5164,25 @@
       </c>
     </row>
     <row r="253" ht="15.75" spans="1:12">
-      <c r="A253" s="73">
-        <v>1</v>
-      </c>
-      <c r="B253" s="74">
-        <v>0</v>
-      </c>
-      <c r="C253" s="75">
-        <v>0</v>
-      </c>
-      <c r="D253" s="75">
-        <v>0</v>
-      </c>
-      <c r="E253" s="76">
+      <c r="A253" s="22">
+        <v>1</v>
+      </c>
+      <c r="B253" s="71">
+        <v>0</v>
+      </c>
+      <c r="C253" s="72">
+        <v>0</v>
+      </c>
+      <c r="D253" s="72">
+        <v>0</v>
+      </c>
+      <c r="E253" s="73">
         <v>1</v>
       </c>
       <c r="G253">
         <v>1</v>
       </c>
-      <c r="H253" s="77" t="s">
+      <c r="H253" s="74" t="s">
         <v>163</v>
       </c>
       <c r="J253">
@@ -5143,16 +5202,16 @@
       <c r="C254" s="12">
         <v>0</v>
       </c>
-      <c r="D254" s="78">
-        <v>1</v>
-      </c>
-      <c r="E254" s="79">
+      <c r="D254" s="75">
+        <v>1</v>
+      </c>
+      <c r="E254" s="76">
         <v>0</v>
       </c>
       <c r="G254">
         <v>1</v>
       </c>
-      <c r="H254" s="38" t="s">
+      <c r="H254" s="36" t="s">
         <v>165</v>
       </c>
       <c r="J254">
@@ -5166,22 +5225,22 @@
       <c r="A255" s="1">
         <v>3</v>
       </c>
-      <c r="B255" s="80">
-        <v>0</v>
-      </c>
-      <c r="C255" s="81">
-        <v>0</v>
-      </c>
-      <c r="D255" s="82">
-        <v>1</v>
-      </c>
-      <c r="E255" s="83">
+      <c r="B255" s="77">
+        <v>0</v>
+      </c>
+      <c r="C255" s="78">
+        <v>0</v>
+      </c>
+      <c r="D255" s="79">
+        <v>1</v>
+      </c>
+      <c r="E255" s="80">
         <v>1</v>
       </c>
       <c r="G255">
         <v>2</v>
       </c>
-      <c r="H255" s="84" t="s">
+      <c r="H255" s="81" t="s">
         <v>165</v>
       </c>
       <c r="J255">
@@ -5192,25 +5251,25 @@
       </c>
     </row>
     <row r="256" spans="1:12">
-      <c r="A256" s="85">
+      <c r="A256" s="82">
         <v>4</v>
       </c>
       <c r="B256" s="11">
         <v>0</v>
       </c>
-      <c r="C256" s="78">
+      <c r="C256" s="75">
         <v>1</v>
       </c>
       <c r="D256" s="12">
         <v>0</v>
       </c>
-      <c r="E256" s="79">
+      <c r="E256" s="76">
         <v>0</v>
       </c>
       <c r="G256">
         <v>1</v>
       </c>
-      <c r="H256" s="38" t="s">
+      <c r="H256" s="36" t="s">
         <v>168</v>
       </c>
       <c r="J256">
@@ -5221,25 +5280,25 @@
       </c>
     </row>
     <row r="257" spans="1:12">
-      <c r="A257" s="86">
+      <c r="A257" s="83">
         <v>5</v>
       </c>
-      <c r="B257" s="87">
-        <v>0</v>
-      </c>
-      <c r="C257" s="33">
+      <c r="B257" s="84">
+        <v>0</v>
+      </c>
+      <c r="C257" s="31">
         <v>1</v>
       </c>
       <c r="D257" s="15">
         <v>0</v>
       </c>
-      <c r="E257" s="88">
+      <c r="E257" s="85">
         <v>1</v>
       </c>
       <c r="G257">
         <v>2</v>
       </c>
-      <c r="H257" s="89" t="s">
+      <c r="H257" s="86" t="s">
         <v>168</v>
       </c>
       <c r="J257">
@@ -5250,25 +5309,25 @@
       </c>
     </row>
     <row r="258" spans="1:10">
-      <c r="A258" s="86">
+      <c r="A258" s="83">
         <v>6</v>
       </c>
-      <c r="B258" s="87">
-        <v>0</v>
-      </c>
-      <c r="C258" s="33">
-        <v>1</v>
-      </c>
-      <c r="D258" s="33">
-        <v>1</v>
-      </c>
-      <c r="E258" s="90">
+      <c r="B258" s="84">
+        <v>0</v>
+      </c>
+      <c r="C258" s="31">
+        <v>1</v>
+      </c>
+      <c r="D258" s="31">
+        <v>1</v>
+      </c>
+      <c r="E258" s="16">
         <v>0</v>
       </c>
       <c r="G258">
         <v>2</v>
       </c>
-      <c r="H258" s="89" t="s">
+      <c r="H258" s="86" t="s">
         <v>168</v>
       </c>
       <c r="J258">
@@ -5276,25 +5335,25 @@
       </c>
     </row>
     <row r="259" ht="15.75" spans="1:10">
-      <c r="A259" s="91">
+      <c r="A259" s="87">
         <v>7</v>
       </c>
-      <c r="B259" s="92">
-        <v>0</v>
-      </c>
-      <c r="C259" s="93">
-        <v>1</v>
-      </c>
-      <c r="D259" s="93">
-        <v>1</v>
-      </c>
-      <c r="E259" s="94">
+      <c r="B259" s="88">
+        <v>0</v>
+      </c>
+      <c r="C259" s="89">
+        <v>1</v>
+      </c>
+      <c r="D259" s="89">
+        <v>1</v>
+      </c>
+      <c r="E259" s="90">
         <v>1</v>
       </c>
       <c r="G259">
         <v>3</v>
       </c>
-      <c r="H259" s="84" t="s">
+      <c r="H259" s="81" t="s">
         <v>168</v>
       </c>
       <c r="J259">
@@ -5305,7 +5364,7 @@
       <c r="A260" s="23">
         <v>8</v>
       </c>
-      <c r="B260" s="95">
+      <c r="B260" s="91">
         <v>1</v>
       </c>
       <c r="C260" s="12">
@@ -5314,21 +5373,21 @@
       <c r="D260" s="12">
         <v>0</v>
       </c>
-      <c r="E260" s="79">
+      <c r="E260" s="76">
         <v>0</v>
       </c>
       <c r="G260">
         <v>1</v>
       </c>
-      <c r="H260" s="38" t="s">
+      <c r="H260" s="36" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="261" spans="1:8">
-      <c r="A261" s="96">
+      <c r="A261" s="92">
         <v>9</v>
       </c>
-      <c r="B261" s="97">
+      <c r="B261" s="93">
         <v>1</v>
       </c>
       <c r="C261" s="15">
@@ -5337,116 +5396,116 @@
       <c r="D261" s="15">
         <v>0</v>
       </c>
-      <c r="E261" s="88">
+      <c r="E261" s="85">
         <v>1</v>
       </c>
       <c r="G261">
         <v>2</v>
       </c>
-      <c r="H261" s="89" t="s">
+      <c r="H261" s="86" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="262" spans="1:8">
-      <c r="A262" s="96">
+      <c r="A262" s="92">
         <v>10</v>
       </c>
-      <c r="B262" s="97">
+      <c r="B262" s="93">
         <v>1</v>
       </c>
       <c r="C262" s="15">
         <v>0</v>
       </c>
-      <c r="D262" s="33">
-        <v>1</v>
-      </c>
-      <c r="E262" s="90">
+      <c r="D262" s="31">
+        <v>1</v>
+      </c>
+      <c r="E262" s="16">
         <v>0</v>
       </c>
       <c r="G262">
         <v>2</v>
       </c>
-      <c r="H262" s="89" t="s">
+      <c r="H262" s="86" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="263" spans="1:8">
-      <c r="A263" s="96">
+      <c r="A263" s="92">
         <v>11</v>
       </c>
-      <c r="B263" s="97">
+      <c r="B263" s="93">
         <v>1</v>
       </c>
       <c r="C263" s="15">
         <v>0</v>
       </c>
-      <c r="D263" s="33">
-        <v>1</v>
-      </c>
-      <c r="E263" s="33">
-        <v>1</v>
-      </c>
-      <c r="H263" s="89" t="s">
+      <c r="D263" s="31">
+        <v>1</v>
+      </c>
+      <c r="E263" s="31">
+        <v>1</v>
+      </c>
+      <c r="H263" s="86" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="264" spans="1:8">
-      <c r="A264" s="96">
+      <c r="A264" s="92">
         <v>12</v>
       </c>
-      <c r="B264" s="97">
-        <v>1</v>
-      </c>
-      <c r="C264" s="33">
+      <c r="B264" s="93">
+        <v>1</v>
+      </c>
+      <c r="C264" s="31">
         <v>1</v>
       </c>
       <c r="D264" s="15">
         <v>0</v>
       </c>
-      <c r="E264" s="90">
-        <v>0</v>
-      </c>
-      <c r="H264" s="89" t="s">
+      <c r="E264" s="16">
+        <v>0</v>
+      </c>
+      <c r="H264" s="86" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="265" spans="1:8">
-      <c r="A265" s="96">
+      <c r="A265" s="92">
         <v>13</v>
       </c>
-      <c r="B265" s="97">
-        <v>1</v>
-      </c>
-      <c r="C265" s="33">
+      <c r="B265" s="93">
+        <v>1</v>
+      </c>
+      <c r="C265" s="31">
         <v>1</v>
       </c>
       <c r="D265" s="15">
         <v>0</v>
       </c>
-      <c r="E265" s="88">
-        <v>1</v>
-      </c>
-      <c r="H265" s="89" t="s">
+      <c r="E265" s="85">
+        <v>1</v>
+      </c>
+      <c r="H265" s="86" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="266" spans="1:8">
-      <c r="A266" s="96">
+      <c r="A266" s="92">
         <v>14</v>
       </c>
-      <c r="B266" s="97">
-        <v>1</v>
-      </c>
-      <c r="C266" s="33">
-        <v>1</v>
-      </c>
-      <c r="D266" s="33">
-        <v>1</v>
-      </c>
-      <c r="E266" s="90">
-        <v>0</v>
-      </c>
-      <c r="H266" s="89" t="s">
+      <c r="B266" s="93">
+        <v>1</v>
+      </c>
+      <c r="C266" s="31">
+        <v>1</v>
+      </c>
+      <c r="D266" s="31">
+        <v>1</v>
+      </c>
+      <c r="E266" s="16">
+        <v>0</v>
+      </c>
+      <c r="H266" s="86" t="s">
         <v>171</v>
       </c>
     </row>
@@ -5454,19 +5513,19 @@
       <c r="A267" s="26">
         <v>15</v>
       </c>
-      <c r="B267" s="98">
-        <v>1</v>
-      </c>
-      <c r="C267" s="82">
-        <v>1</v>
-      </c>
-      <c r="D267" s="82">
-        <v>1</v>
-      </c>
-      <c r="E267" s="83">
-        <v>1</v>
-      </c>
-      <c r="H267" s="84" t="s">
+      <c r="B267" s="94">
+        <v>1</v>
+      </c>
+      <c r="C267" s="79">
+        <v>1</v>
+      </c>
+      <c r="D267" s="79">
+        <v>1</v>
+      </c>
+      <c r="E267" s="80">
+        <v>1</v>
+      </c>
+      <c r="H267" s="81" t="s">
         <v>171</v>
       </c>
     </row>
@@ -5552,7 +5611,7 @@
       <c r="D280" s="12">
         <v>6000</v>
       </c>
-      <c r="E280" s="99">
+      <c r="E280" s="13">
         <v>18000</v>
       </c>
       <c r="H280" t="s">
@@ -5572,11 +5631,11 @@
       <c r="B281">
         <v>1</v>
       </c>
-      <c r="C281" s="87"/>
+      <c r="C281" s="84"/>
       <c r="D281" s="15">
         <v>0</v>
       </c>
-      <c r="E281" s="90">
+      <c r="E281" s="16">
         <v>24000</v>
       </c>
       <c r="H281" t="s">
@@ -5596,9 +5655,9 @@
       <c r="B282">
         <v>2</v>
       </c>
-      <c r="C282" s="80"/>
-      <c r="D282" s="81"/>
-      <c r="E282" s="100">
+      <c r="C282" s="77"/>
+      <c r="D282" s="78"/>
+      <c r="E282" s="20">
         <v>0</v>
       </c>
     </row>
@@ -5631,7 +5690,7 @@
       <c r="K285" t="s">
         <v>189</v>
       </c>
-      <c r="M285" s="28">
+      <c r="M285" s="25">
         <v>18000</v>
       </c>
     </row>
@@ -5649,19 +5708,113 @@
       <c r="M288" s="24"/>
       <c r="N288" s="24"/>
       <c r="O288" s="24"/>
-      <c r="P288" s="29"/>
+      <c r="P288" s="27"/>
     </row>
     <row r="289" ht="15.75" spans="10:16">
       <c r="J289" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="K289" s="27"/>
-      <c r="L289" s="27"/>
-      <c r="M289" s="27"/>
-      <c r="N289" s="27"/>
-      <c r="O289" s="27"/>
-      <c r="P289" s="30" t="s">
+      <c r="K289" s="19"/>
+      <c r="L289" s="19"/>
+      <c r="M289" s="19"/>
+      <c r="N289" s="19"/>
+      <c r="O289" s="19"/>
+      <c r="P289" s="28" t="s">
         <v>193</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295" s="1"/>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="A296" t="s">
+        <v>12</v>
+      </c>
+      <c r="B296">
+        <v>0</v>
+      </c>
+      <c r="C296">
+        <v>1</v>
+      </c>
+      <c r="D296">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="A297" t="s">
+        <v>195</v>
+      </c>
+      <c r="B297" s="95" t="s">
+        <v>196</v>
+      </c>
+      <c r="C297" s="95" t="s">
+        <v>197</v>
+      </c>
+      <c r="D297" s="95" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4">
+      <c r="B299" s="96" t="s">
+        <v>199</v>
+      </c>
+      <c r="C299" s="97" t="s">
+        <v>200</v>
+      </c>
+      <c r="D299" s="98" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301">
+        <v>0</v>
+      </c>
+      <c r="B301">
+        <v>14</v>
+      </c>
+      <c r="C301" s="99">
+        <v>2</v>
+      </c>
+      <c r="D301">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4">
+      <c r="A302">
+        <v>1</v>
+      </c>
+      <c r="B302" t="s">
+        <v>203</v>
+      </c>
+      <c r="C302" t="s">
+        <v>204</v>
+      </c>
+      <c r="D302" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
+      <c r="A303">
+        <v>2</v>
+      </c>
+      <c r="B303" t="s">
+        <v>206</v>
+      </c>
+      <c r="C303" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D303" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -5678,7 +5831,7 @@
   <sheetPr/>
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -5693,13 +5846,13 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" ht="15.75"/>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -5711,7 +5864,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -5747,39 +5900,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" ht="15.75"/>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="E9" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="E10" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" ht="15.75"/>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -5798,37 +5951,37 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
       <c r="B16" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="C16" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:2">
       <c r="A17" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="B17" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="B18" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="C18" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:1">
       <c r="A20" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -5836,19 +5989,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="F22" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="G22" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -5859,15 +6012,15 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="C23" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -5890,7 +6043,7 @@
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5898,30 +6051,30 @@
         <v>174</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" ht="15.75" spans="3:6">
       <c r="C30" s="10" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" ht="15.75" spans="3:20">
@@ -5948,11 +6101,11 @@
       <c r="Q31" s="24"/>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
-      <c r="T31" s="29"/>
+      <c r="T31" s="27"/>
     </row>
     <row r="32" ht="15.75" spans="1:20">
       <c r="A32" s="10" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -5970,29 +6123,29 @@
         <v>30</v>
       </c>
       <c r="I32" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="J32" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="K32" s="25">
         <v>6</v>
       </c>
       <c r="N32" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="27"/>
-      <c r="T32" s="30" t="s">
-        <v>335</v>
+        <v>349</v>
+      </c>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="28" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="10" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -6008,10 +6161,10 @@
         <v>48</v>
       </c>
       <c r="I33" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="J33" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="K33" s="25">
         <v>24</v>
@@ -6019,7 +6172,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="10" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -6033,10 +6186,10 @@
         <v>36</v>
       </c>
       <c r="I34" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="J34" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="K34" s="25">
         <v>36</v>
@@ -6044,7 +6197,7 @@
     </row>
     <row r="35" ht="15.75" spans="1:6">
       <c r="A35" s="10" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -6063,30 +6216,30 @@
     </row>
     <row r="37" spans="9:13">
       <c r="I37" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="J37" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="K37" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
       <c r="L37" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="M37">
         <v>32</v>
       </c>
     </row>
     <row r="38" spans="10:13">
-      <c r="J38" s="28" t="s">
-        <v>344</v>
+      <c r="J38" s="25" t="s">
+        <v>359</v>
       </c>
       <c r="K38" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="L38" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
       <c r="M38" s="25">
         <v>18</v>
@@ -6094,30 +6247,30 @@
     </row>
     <row r="40" spans="9:13">
       <c r="I40" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="J40" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="K40" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="L40" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="M40">
         <v>54</v>
       </c>
     </row>
     <row r="41" spans="10:13">
-      <c r="J41" s="28" t="s">
-        <v>351</v>
+      <c r="J41" s="25" t="s">
+        <v>366</v>
       </c>
       <c r="K41" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
       <c r="L41" t="s">
-        <v>353</v>
+        <v>368</v>
       </c>
       <c r="M41" s="25">
         <v>48</v>
@@ -6126,21 +6279,21 @@
     <row r="42" ht="15.75"/>
     <row r="43" ht="15.75" spans="9:9">
       <c r="I43" s="22" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
     </row>
     <row r="44" spans="9:13">
       <c r="I44" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="J44" t="s">
-        <v>356</v>
+        <v>371</v>
       </c>
       <c r="K44" t="s">
-        <v>357</v>
+        <v>372</v>
       </c>
       <c r="L44" t="s">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="M44">
         <v>54</v>
@@ -6148,27 +6301,27 @@
     </row>
     <row r="45" spans="10:13">
       <c r="J45" t="s">
-        <v>359</v>
+        <v>374</v>
       </c>
       <c r="K45" t="s">
-        <v>360</v>
+        <v>375</v>
       </c>
       <c r="L45" t="s">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="M45">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="10:13">
-      <c r="J46" s="28" t="s">
-        <v>362</v>
+      <c r="J46" s="25" t="s">
+        <v>377</v>
       </c>
       <c r="K46" t="s">
-        <v>363</v>
+        <v>378</v>
       </c>
       <c r="L46" t="s">
-        <v>364</v>
+        <v>379</v>
       </c>
       <c r="M46" s="25">
         <v>30</v>
@@ -6234,51 +6387,51 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B2" s="53">
-        <v>0</v>
-      </c>
-      <c r="C2" s="53">
-        <v>1</v>
-      </c>
-      <c r="D2" s="53">
+        <v>209</v>
+      </c>
+      <c r="B2" s="51">
+        <v>0</v>
+      </c>
+      <c r="C2" s="51">
+        <v>1</v>
+      </c>
+      <c r="D2" s="51">
         <f t="shared" ref="D2:M2" si="0">C2+B2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="51">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="51">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="51">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H2" s="53">
+      <c r="H2" s="51">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I2" s="53">
+      <c r="I2" s="51">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="J2" s="53">
+      <c r="J2" s="51">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="K2" s="53">
+      <c r="K2" s="51">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L2" s="53">
+      <c r="L2" s="51">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="M2" s="53">
+      <c r="M2" s="51">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
@@ -6308,27 +6461,27 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -6340,32 +6493,32 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="34" t="s">
+      <c r="C9" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="49" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -6385,22 +6538,22 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="28" t="s">
+      <c r="D19" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F19" t="s">
@@ -6408,13 +6561,13 @@
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="52">
-        <v>2</v>
-      </c>
-      <c r="D20" s="34">
+      <c r="B20" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="50">
+        <v>2</v>
+      </c>
+      <c r="D20" s="32">
         <v>2</v>
       </c>
       <c r="E20" s="15">
@@ -6425,7 +6578,7 @@
       </c>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="15">
@@ -6434,7 +6587,7 @@
       <c r="D21" s="15">
         <v>1</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="32">
         <v>1</v>
       </c>
       <c r="F21">
@@ -6454,7 +6607,7 @@
       <c r="E22" s="15">
         <v>0</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="34">
         <v>0</v>
       </c>
     </row>
@@ -6471,7 +6624,7 @@
       <c r="E23" s="15">
         <v>0</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F23" s="34">
         <v>0</v>
       </c>
     </row>
@@ -6488,13 +6641,13 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="36">
+      <c r="F24" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -6514,17 +6667,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>51</v>
@@ -6532,22 +6685,22 @@
       <c r="C37" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="34" t="s">
-        <v>206</v>
+      <c r="E37" s="32" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>199</v>
-      </c>
-      <c r="B38" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="B38" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="34" t="s">
-        <v>206</v>
+      <c r="C38" s="32" t="s">
+        <v>221</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>6</v>
@@ -6555,18 +6708,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -6578,7 +6731,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -6586,20 +6739,20 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
     </row>
     <row r="47" spans="3:6">
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="28" t="s">
-        <v>206</v>
+      <c r="D47" s="25" t="s">
+        <v>221</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -6609,10 +6762,10 @@
       </c>
     </row>
     <row r="48" spans="2:6">
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="52">
+      <c r="C48" s="50">
         <v>2</v>
       </c>
       <c r="D48" s="15">
@@ -6626,10 +6779,10 @@
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="34">
+      <c r="C49" s="32">
         <v>2</v>
       </c>
       <c r="D49" s="15">
@@ -6643,13 +6796,13 @@
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="25" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="15">
         <v>2</v>
       </c>
-      <c r="D50" s="34">
+      <c r="D50" s="32">
         <v>1</v>
       </c>
       <c r="E50" s="15">
@@ -6660,13 +6813,13 @@
       </c>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="28" t="s">
-        <v>206</v>
+      <c r="B51" s="25" t="s">
+        <v>221</v>
       </c>
       <c r="C51" s="15">
         <v>1</v>
       </c>
-      <c r="D51" s="34">
+      <c r="D51" s="32">
         <v>1</v>
       </c>
       <c r="E51" s="15">
@@ -6686,7 +6839,7 @@
       <c r="D52">
         <v>0</v>
       </c>
-      <c r="E52" s="36">
+      <c r="E52" s="34">
         <v>0</v>
       </c>
       <c r="F52">
@@ -6695,7 +6848,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -6707,7 +6860,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -6735,12 +6888,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
-      <c r="A3" s="31" t="s">
-        <v>210</v>
+      <c r="A3" s="29" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -6821,7 +6974,7 @@
       <c r="L7">
         <v>2</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="25">
         <v>3</v>
       </c>
     </row>
@@ -6829,14 +6982,14 @@
       <c r="A9" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="25">
         <v>0</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -6846,12 +6999,12 @@
       <c r="A10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="25">
         <v>1</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="15" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -6861,8 +7014,8 @@
       <c r="A11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="E11" t="s">
         <v>65</v>
       </c>
@@ -6871,9 +7024,9 @@
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="K11" s="28">
+        <v>229</v>
+      </c>
+      <c r="K11" s="25">
         <v>3</v>
       </c>
     </row>
@@ -6881,12 +7034,12 @@
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="13:13">
-      <c r="M13" s="50">
+      <c r="M13" s="48">
         <v>1</v>
       </c>
     </row>
@@ -6894,30 +7047,30 @@
       <c r="A14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
       <c r="F14" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="M14" s="50">
+        <v>231</v>
+      </c>
+      <c r="M14" s="48">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>217</v>
-      </c>
-      <c r="G15" s="28">
-        <v>2</v>
-      </c>
-      <c r="M15" s="50">
+        <v>232</v>
+      </c>
+      <c r="G15" s="25">
+        <v>2</v>
+      </c>
+      <c r="M15" s="48">
         <v>5</v>
       </c>
     </row>
@@ -6925,12 +7078,12 @@
       <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
       <c r="G17" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -6938,36 +7091,36 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>219</v>
-      </c>
-      <c r="I18" s="28">
+        <v>234</v>
+      </c>
+      <c r="I18" s="25">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="15" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="C20" s="15">
         <v>3</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G20" s="15">
         <v>2</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="K20" s="15">
         <v>3</v>
@@ -6976,21 +7129,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="15"/>
       <c r="B21" s="15" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="C21" s="15">
         <v>3</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="G21" s="15">
         <v>3</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="K21" s="15">
         <v>2</v>
@@ -6999,50 +7152,50 @@
     <row r="22" spans="1:11">
       <c r="A22" s="15"/>
       <c r="B22" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="C22" s="33">
+        <v>244</v>
+      </c>
+      <c r="C22" s="31">
         <v>1</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="G22" s="33">
+        <v>245</v>
+      </c>
+      <c r="G22" s="31">
         <v>2</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="K22" s="33">
+        <v>246</v>
+      </c>
+      <c r="K22" s="31">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="15" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="C24" s="15">
         <v>3</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="G24" s="15">
         <v>4</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="K24" s="15">
         <v>4</v>
@@ -7051,21 +7204,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="15"/>
       <c r="B25" s="15" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C25" s="15">
         <v>3</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="G25" s="15">
         <v>3</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="15" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="K25" s="15">
         <v>4</v>
@@ -7074,23 +7227,23 @@
     <row r="26" spans="1:11">
       <c r="A26" s="15"/>
       <c r="B26" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C26" s="33">
+        <v>256</v>
+      </c>
+      <c r="C26" s="31">
         <v>3</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="G26" s="33">
+        <v>257</v>
+      </c>
+      <c r="G26" s="31">
         <v>3</v>
       </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="K26" s="33">
+        <v>258</v>
+      </c>
+      <c r="K26" s="31">
         <v>2</v>
       </c>
     </row>
@@ -7118,7 +7271,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>31</v>
@@ -7138,7 +7291,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>28</v>
@@ -7160,10 +7313,10 @@
       <c r="D6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="31" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7174,36 +7327,36 @@
       <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -7318,7 +7471,7 @@
       <c r="E23" s="15">
         <v>4</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="31">
         <v>3</v>
       </c>
     </row>
@@ -7353,104 +7506,104 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>251</v>
-      </c>
-      <c r="L3" s="49">
+        <v>266</v>
+      </c>
+      <c r="L3" s="47">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="2:12">
-      <c r="B4" s="38">
-        <v>1</v>
-      </c>
-      <c r="I4" s="48">
-        <v>2</v>
-      </c>
-      <c r="L4" s="49" t="s">
-        <v>252</v>
+      <c r="B4" s="36">
+        <v>1</v>
+      </c>
+      <c r="I4" s="46">
+        <v>2</v>
+      </c>
+      <c r="L4" s="47" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
-      <c r="B5" s="39"/>
-      <c r="C5" s="29">
-        <v>2</v>
-      </c>
-      <c r="I5" s="48">
+      <c r="B5" s="37"/>
+      <c r="C5" s="27">
+        <v>2</v>
+      </c>
+      <c r="I5" s="46">
         <v>5</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="2:9">
-      <c r="B6" s="39"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="24"/>
-      <c r="D6" s="29">
-        <v>3</v>
-      </c>
-      <c r="I6" s="48">
+      <c r="D6" s="27">
+        <v>3</v>
+      </c>
+      <c r="I6" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="2:9">
-      <c r="B7" s="39"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="29">
+      <c r="E7" s="27">
         <v>4</v>
       </c>
-      <c r="I7" s="48">
+      <c r="I7" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="2:9">
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42">
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40">
         <v>5</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="45"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="43"/>
       <c r="H11" t="s">
-        <v>254</v>
-      </c>
-      <c r="I11" s="48">
+        <v>269</v>
+      </c>
+      <c r="I11" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>255</v>
-      </c>
-      <c r="I12" s="48">
+        <v>270</v>
+      </c>
+      <c r="I12" s="46">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>256</v>
-      </c>
-      <c r="I13" s="48">
+        <v>271</v>
+      </c>
+      <c r="I13" s="46">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>257</v>
-      </c>
-      <c r="I14" s="48">
+        <v>272</v>
+      </c>
+      <c r="I14" s="46">
         <v>10</v>
       </c>
     </row>
@@ -7458,23 +7611,23 @@
       <c r="H15">
         <v>5</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>258</v>
-      </c>
-      <c r="I16" s="46">
+        <v>273</v>
+      </c>
+      <c r="I16" s="44">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>259</v>
-      </c>
-      <c r="I17" s="46">
+        <v>274</v>
+      </c>
+      <c r="I17" s="44">
         <v>12</v>
       </c>
     </row>
@@ -7482,7 +7635,7 @@
       <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="46">
+      <c r="B20" s="44">
         <v>0</v>
       </c>
     </row>
@@ -7491,13 +7644,13 @@
       <c r="A22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="47">
-        <v>1</v>
-      </c>
-      <c r="D22" s="48" t="s">
+      <c r="B22" s="45">
+        <v>1</v>
+      </c>
+      <c r="D22" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="44">
         <v>2</v>
       </c>
     </row>
@@ -7506,8 +7659,8 @@
       <c r="A24" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="45">
+      <c r="B24" s="41"/>
+      <c r="C24" s="43">
         <v>2</v>
       </c>
       <c r="E24" t="s">
@@ -7516,7 +7669,7 @@
       <c r="F24" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="48">
+      <c r="G24" s="46">
         <v>4</v>
       </c>
     </row>
@@ -7525,23 +7678,23 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>260</v>
-      </c>
-      <c r="G25" s="46">
+        <v>275</v>
+      </c>
+      <c r="G25" s="44">
         <v>5</v>
       </c>
       <c r="L25" t="s">
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="M26" s="48">
+      <c r="M26" s="46">
         <v>2</v>
       </c>
     </row>
@@ -7549,9 +7702,9 @@
       <c r="A27" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45">
+      <c r="B27" s="41"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43">
         <v>3</v>
       </c>
       <c r="F27" t="s">
@@ -7560,13 +7713,13 @@
       <c r="G27" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="48">
+      <c r="H27" s="46">
         <v>7</v>
       </c>
       <c r="L27">
         <v>2</v>
       </c>
-      <c r="M27" s="48">
+      <c r="M27" s="46">
         <v>5</v>
       </c>
     </row>
@@ -7577,13 +7730,13 @@
       <c r="G28" t="s">
         <v>75</v>
       </c>
-      <c r="H28" s="48">
+      <c r="H28" s="46">
         <v>7</v>
       </c>
       <c r="L28">
         <v>3</v>
       </c>
-      <c r="M28" s="48">
+      <c r="M28" s="46">
         <v>7</v>
       </c>
     </row>
@@ -7592,15 +7745,15 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>262</v>
-      </c>
-      <c r="H29" s="46">
+        <v>277</v>
+      </c>
+      <c r="H29" s="44">
         <v>7</v>
       </c>
       <c r="L29">
         <v>4</v>
       </c>
-      <c r="M29" s="48">
+      <c r="M29" s="46">
         <v>8</v>
       </c>
     </row>
@@ -7608,7 +7761,7 @@
       <c r="L30">
         <v>5</v>
       </c>
-      <c r="M30" s="48">
+      <c r="M30" s="46">
         <v>10</v>
       </c>
     </row>
@@ -7617,10 +7770,10 @@
       <c r="A32" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="45">
+      <c r="B32" s="41"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="43">
         <v>4</v>
       </c>
       <c r="G32" t="s">
@@ -7629,7 +7782,7 @@
       <c r="H32" t="s">
         <v>80</v>
       </c>
-      <c r="I32" s="48">
+      <c r="I32" s="46">
         <v>9</v>
       </c>
     </row>
@@ -7640,7 +7793,7 @@
       <c r="H33" t="s">
         <v>83</v>
       </c>
-      <c r="I33" s="46">
+      <c r="I33" s="44">
         <v>10</v>
       </c>
     </row>
@@ -7651,7 +7804,7 @@
       <c r="H34" t="s">
         <v>85</v>
       </c>
-      <c r="I34" s="48">
+      <c r="I34" s="46">
         <v>9</v>
       </c>
     </row>
@@ -7660,75 +7813,75 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>263</v>
-      </c>
-      <c r="I35" s="48">
+        <v>278</v>
+      </c>
+      <c r="I35" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="37" ht="15.75"/>
     <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
-        <v>220</v>
-      </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="45">
+        <v>235</v>
+      </c>
+      <c r="B38" s="41"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="43">
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="I38" t="s">
-        <v>264</v>
-      </c>
-      <c r="J38" s="48">
+        <v>279</v>
+      </c>
+      <c r="J38" s="46">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="I39" t="s">
-        <v>265</v>
-      </c>
-      <c r="J39" s="48">
+        <v>280</v>
+      </c>
+      <c r="J39" s="46">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="I40" t="s">
-        <v>267</v>
-      </c>
-      <c r="J40" s="46">
+        <v>282</v>
+      </c>
+      <c r="J40" s="44">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="I41" t="s">
-        <v>269</v>
-      </c>
-      <c r="J41" s="48">
+        <v>284</v>
+      </c>
+      <c r="J41" s="46">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="I42" t="s">
-        <v>271</v>
-      </c>
-      <c r="J42" s="48">
+        <v>286</v>
+      </c>
+      <c r="J42" s="46">
         <v>10</v>
       </c>
     </row>
@@ -7756,17 +7909,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -7791,64 +7944,64 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="M15" s="15">
         <v>4</v>
       </c>
-      <c r="N15" s="34">
-        <v>2</v>
-      </c>
-      <c r="O15" s="34">
+      <c r="N15" s="32">
+        <v>2</v>
+      </c>
+      <c r="O15" s="32">
         <v>10</v>
       </c>
-      <c r="P15" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="34">
+      <c r="P15" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="32">
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="M16" s="15">
         <v>12</v>
       </c>
-      <c r="N16" s="34">
-        <v>1</v>
-      </c>
-      <c r="O16" s="34">
+      <c r="N16" s="32">
+        <v>1</v>
+      </c>
+      <c r="O16" s="32">
         <v>4</v>
       </c>
-      <c r="P16" s="34">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="34">
+      <c r="P16" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="32">
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>279</v>
-      </c>
-      <c r="M19" s="35">
+        <v>294</v>
+      </c>
+      <c r="M19" s="33">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -7901,7 +8054,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -7927,7 +8080,7 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29" s="36">
+      <c r="J29" s="34">
         <v>0</v>
       </c>
       <c r="K29">
@@ -7957,7 +8110,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -7983,7 +8136,7 @@
       <c r="I30" s="15">
         <v>0</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="32">
         <v>0</v>
       </c>
       <c r="K30" s="15">
@@ -7998,7 +8151,7 @@
       <c r="N30" s="15">
         <v>0</v>
       </c>
-      <c r="O30" s="33">
+      <c r="O30" s="31">
         <v>4</v>
       </c>
       <c r="P30" s="15">
@@ -8013,7 +8166,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8042,7 +8195,7 @@
       <c r="J31" s="15">
         <v>2</v>
       </c>
-      <c r="K31" s="34">
+      <c r="K31" s="32">
         <v>2</v>
       </c>
       <c r="L31" s="15">
@@ -8057,7 +8210,7 @@
       <c r="O31" s="15">
         <v>4</v>
       </c>
-      <c r="P31" s="33">
+      <c r="P31" s="31">
         <v>6</v>
       </c>
       <c r="Q31" s="15">
@@ -8069,7 +8222,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8089,7 +8242,7 @@
       <c r="G32" s="15">
         <v>10</v>
       </c>
-      <c r="H32" s="33">
+      <c r="H32" s="31">
         <v>12</v>
       </c>
       <c r="I32" s="15">
@@ -8110,7 +8263,7 @@
       <c r="N32" s="15">
         <v>12</v>
       </c>
-      <c r="O32" s="34">
+      <c r="O32" s="32">
         <v>12</v>
       </c>
       <c r="P32" s="15">
@@ -8125,7 +8278,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -8148,7 +8301,7 @@
       <c r="H33" s="15">
         <v>12</v>
       </c>
-      <c r="I33" s="33">
+      <c r="I33" s="31">
         <v>13</v>
       </c>
       <c r="J33" s="15">
@@ -8169,7 +8322,7 @@
       <c r="O33" s="15">
         <v>13</v>
       </c>
-      <c r="P33" s="34">
+      <c r="P33" s="32">
         <v>13</v>
       </c>
       <c r="Q33" s="15">
@@ -8181,7 +8334,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -8195,7 +8348,7 @@
       <c r="E34" s="15">
         <v>2</v>
       </c>
-      <c r="F34" s="33">
+      <c r="F34" s="31">
         <v>4</v>
       </c>
       <c r="G34" s="15">
@@ -8210,7 +8363,7 @@
       <c r="J34" s="15">
         <v>14</v>
       </c>
-      <c r="K34" s="33">
+      <c r="K34" s="31">
         <v>15</v>
       </c>
       <c r="L34" s="15">
@@ -8231,23 +8384,23 @@
       <c r="Q34" s="15">
         <v>15</v>
       </c>
-      <c r="R34" s="37">
+      <c r="R34" s="35">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="101" t="s">
-        <v>289</v>
+      <c r="A38" s="100" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="101" t="s">
-        <v>290</v>
+      <c r="A39" s="100" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -8270,11 +8423,11 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="2:2">
-      <c r="B3" s="31"/>
+      <c r="B3" s="29"/>
     </row>
     <row r="5" spans="3:14">
       <c r="C5">
@@ -8319,40 +8472,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="D6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="E6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="F6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="G6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="H6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="I6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="J6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="K6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="L6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="M6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="N6" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8363,7 +8516,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8374,7 +8527,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8385,7 +8538,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -8396,7 +8549,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -8422,8 +8575,8 @@
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="31" t="s">
-        <v>294</v>
+      <c r="A5" s="29" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8458,42 +8611,42 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="30" t="s">
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -8533,15 +8686,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="E12" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -8551,7 +8704,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed pascals triangle videos
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="397">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -652,6 +652,30 @@
     <t>10+13=23</t>
   </si>
   <si>
+    <t>Pascal's Triangle</t>
+  </si>
+  <si>
+    <t>numRows = 5</t>
+  </si>
+  <si>
+    <t>i,j</t>
+  </si>
+  <si>
+    <t>i=0</t>
+  </si>
+  <si>
+    <t>j=1</t>
+  </si>
+  <si>
+    <t>row[n]=row_prev[i]+row_prev[j]</t>
+  </si>
+  <si>
+    <t>i++; j++</t>
+  </si>
+  <si>
+    <t>dp[5]</t>
+  </si>
+  <si>
     <t>fib(n)</t>
   </si>
   <si>
@@ -730,9 +754,6 @@
     <t>1+dp[4-2]</t>
   </si>
   <si>
-    <t>dp[5]</t>
-  </si>
-  <si>
     <t>1+dp[5-1]</t>
   </si>
   <si>
@@ -1109,9 +1130,6 @@
   </si>
   <si>
     <t>(0*1*2)</t>
-  </si>
-  <si>
-    <t>i=0</t>
   </si>
   <si>
     <t>k=0</t>
@@ -1203,13 +1221,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,10 +1284,39 @@
     </font>
     <font>
       <b/>
+      <sz val="9.75"/>
+      <color rgb="FF263238"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1281,9 +1328,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1295,17 +1350,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1327,15 +1373,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1357,31 +1412,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1390,13 +1422,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1442,7 +1467,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1454,7 +1479,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1466,31 +1515,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1514,6 +1545,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1526,13 +1563,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1544,25 +1575,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1580,13 +1605,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1598,25 +1641,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2093,6 +2118,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2104,11 +2144,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2124,6 +2162,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2145,33 +2192,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2193,7 +2218,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2211,134 +2236,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2458,6 +2483,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2872,10 +2905,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z303"/>
+  <dimension ref="A1:Z313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="J288" sqref="J288"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5851,6 +5884,140 @@
       </c>
       <c r="D303" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="307" customFormat="1" spans="1:7">
+      <c r="A307" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B307"/>
+      <c r="C307"/>
+      <c r="D307"/>
+      <c r="E307"/>
+      <c r="F307"/>
+      <c r="G307" s="99" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="308" customFormat="1" ht="15.75"/>
+    <row r="309" customFormat="1" ht="15.75" spans="1:10">
+      <c r="A309" t="s">
+        <v>60</v>
+      </c>
+      <c r="B309"/>
+      <c r="C309">
+        <v>0</v>
+      </c>
+      <c r="D309" s="100">
+        <v>1</v>
+      </c>
+      <c r="E309">
+        <v>0</v>
+      </c>
+      <c r="F309"/>
+      <c r="G309"/>
+      <c r="H309"/>
+      <c r="I309"/>
+      <c r="J309" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="310" customFormat="1" ht="15.75" spans="1:10">
+      <c r="A310" t="s">
+        <v>64</v>
+      </c>
+      <c r="B310"/>
+      <c r="C310">
+        <v>0</v>
+      </c>
+      <c r="D310" s="101">
+        <v>1</v>
+      </c>
+      <c r="E310" s="102">
+        <v>1</v>
+      </c>
+      <c r="F310">
+        <v>0</v>
+      </c>
+      <c r="G310"/>
+      <c r="H310"/>
+      <c r="I310"/>
+      <c r="J310" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="311" ht="15.75" spans="1:11">
+      <c r="A311" t="s">
+        <v>70</v>
+      </c>
+      <c r="C311">
+        <v>0</v>
+      </c>
+      <c r="D311" s="101">
+        <v>1</v>
+      </c>
+      <c r="E311" s="103">
+        <v>2</v>
+      </c>
+      <c r="F311" s="102">
+        <v>1</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+      <c r="J311" t="s">
+        <v>213</v>
+      </c>
+      <c r="K311" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="312" ht="15.75" spans="1:11">
+      <c r="A312" t="s">
+        <v>78</v>
+      </c>
+      <c r="C312">
+        <v>0</v>
+      </c>
+      <c r="D312" s="101">
+        <v>1</v>
+      </c>
+      <c r="E312" s="103">
+        <v>3</v>
+      </c>
+      <c r="F312" s="103">
+        <v>3</v>
+      </c>
+      <c r="G312" s="102">
+        <v>1</v>
+      </c>
+      <c r="H312">
+        <v>0</v>
+      </c>
+      <c r="K312" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="313" customFormat="1" ht="15.75" spans="1:8">
+      <c r="A313" t="s">
+        <v>216</v>
+      </c>
+      <c r="B313"/>
+      <c r="C313"/>
+      <c r="D313" s="104">
+        <v>1</v>
+      </c>
+      <c r="E313" s="105">
+        <v>4</v>
+      </c>
+      <c r="F313" s="105">
+        <v>6</v>
+      </c>
+      <c r="G313" s="105">
+        <v>4</v>
+      </c>
+      <c r="H313" s="106">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5884,13 +6051,13 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" ht="15.75"/>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -5902,7 +6069,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -5938,39 +6105,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" ht="15.75"/>
     <row r="9" customFormat="1" spans="1:5">
       <c r="A9" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="E9" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="E10" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" ht="15.75"/>
     <row r="12" customFormat="1" spans="1:3">
       <c r="A12" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -5989,41 +6156,41 @@
     </row>
     <row r="16" customFormat="1" spans="1:3">
       <c r="A16" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B16" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="C16" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B17" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="F17" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="I17" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="B18" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="F18" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -6031,21 +6198,21 @@
     </row>
     <row r="19" customFormat="1" spans="6:6">
       <c r="F19" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
       <c r="A20" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="C20" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="D20" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="F20" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:9">
@@ -6053,19 +6220,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="F22" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="G22" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -6076,15 +6243,15 @@
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C23" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="3:4">
       <c r="C24" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -6092,7 +6259,7 @@
     </row>
     <row r="27" customFormat="1" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:5">
@@ -6117,34 +6284,34 @@
         <v>174</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31" ht="15.75"/>
     <row r="32" customFormat="1" ht="15.75" spans="3:10">
       <c r="C32" s="10" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>178</v>
@@ -6172,7 +6339,7 @@
     </row>
     <row r="34" customFormat="1" spans="1:10">
       <c r="A34" s="10" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -6190,10 +6357,10 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="I34" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J34" s="24">
         <v>6</v>
@@ -6201,7 +6368,7 @@
     </row>
     <row r="35" customFormat="1" spans="1:10">
       <c r="A35" s="10" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -6217,10 +6384,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="I35" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="J35" s="24">
         <v>24</v>
@@ -6228,7 +6395,7 @@
     </row>
     <row r="36" customFormat="1" spans="1:10">
       <c r="A36" s="10" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -6242,10 +6409,10 @@
         <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="I36" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="J36" s="24">
         <v>36</v>
@@ -6253,7 +6420,7 @@
     </row>
     <row r="37" customFormat="1" ht="15.75" spans="1:6">
       <c r="A37" s="10" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -6275,25 +6442,25 @@
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="D39" t="s">
-        <v>362</v>
+        <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="F39" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="H39" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="I39" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="J39" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="K39">
         <v>32</v>
@@ -6301,13 +6468,13 @@
     </row>
     <row r="40" spans="4:11">
       <c r="D40" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="J40" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="K40" s="24">
         <v>18</v>
@@ -6315,27 +6482,27 @@
     </row>
     <row r="41" customFormat="1" spans="4:4">
       <c r="D41" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
     </row>
     <row r="42" spans="4:11">
       <c r="D42" t="s">
-        <v>362</v>
+        <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="F42" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="H42" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="I42" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="J42" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="K42">
         <v>54</v>
@@ -6343,13 +6510,13 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="J43" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="K43" s="24">
         <v>48</v>
@@ -6358,24 +6525,24 @@
     <row r="44" ht="15.75"/>
     <row r="45" customFormat="1" ht="15.75" spans="7:7">
       <c r="G45" s="11" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="2:10">
       <c r="B46" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="C46" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="G46" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="H46" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="I46" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="J46">
         <v>54</v>
@@ -6383,16 +6550,16 @@
     </row>
     <row r="47" customFormat="1" spans="2:10">
       <c r="B47" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="C47" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="H47" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="I47" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="J47">
         <v>51</v>
@@ -6400,17 +6567,17 @@
     </row>
     <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="23" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="C48" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I48" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="J48" s="24">
         <v>30</v>
@@ -6421,10 +6588,10 @@
         <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -6487,7 +6654,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B2" s="50">
         <v>0</v>
@@ -6561,22 +6728,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>2</v>
@@ -6593,7 +6760,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
@@ -6607,7 +6774,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>2</v>
@@ -6618,7 +6785,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -6638,12 +6805,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -6747,7 +6914,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -6767,17 +6934,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
@@ -6789,18 +6956,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>6</v>
@@ -6808,18 +6975,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -6831,7 +6998,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -6839,12 +7006,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -6852,7 +7019,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -6914,7 +7081,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="24" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C51" s="16">
         <v>1</v>
@@ -6948,7 +7115,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -6960,7 +7127,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -6988,12 +7155,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="25" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -7086,10 +7253,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -7104,7 +7271,7 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -7124,7 +7291,7 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="K11" s="24">
         <v>3</v>
@@ -7151,13 +7318,13 @@
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="F14" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="M14" s="47">
         <v>2</v>
@@ -7165,7 +7332,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="G15" s="24">
         <v>2</v>
@@ -7183,7 +7350,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="G17" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -7191,7 +7358,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="I18" s="24">
         <v>2</v>
@@ -7199,28 +7366,28 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="16" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C20" s="16">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="K20" s="16">
         <v>3</v>
@@ -7229,21 +7396,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C21" s="16">
         <v>3</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="G21" s="16">
         <v>3</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="K21" s="16">
         <v>2</v>
@@ -7252,21 +7419,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="G22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="K22" s="28">
         <v>2</v>
@@ -7274,28 +7441,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="C24" s="16">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="G24" s="16">
         <v>4</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="K24" s="16">
         <v>4</v>
@@ -7304,21 +7471,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C25" s="16">
         <v>3</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="G25" s="16">
         <v>3</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="K25" s="16">
         <v>4</v>
@@ -7327,21 +7494,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C26" s="28">
         <v>3</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="G26" s="28">
         <v>3</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="K26" s="28">
         <v>2</v>
@@ -7371,7 +7538,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>31</v>
@@ -7391,7 +7558,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -7436,27 +7603,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -7606,7 +7773,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="L3" s="46">
         <v>5</v>
@@ -7620,7 +7787,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -7667,7 +7834,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -7677,7 +7844,7 @@
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="H11" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="I11" s="45">
         <v>10</v>
@@ -7685,7 +7852,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="I12" s="45">
         <v>11</v>
@@ -7693,7 +7860,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="I13" s="45">
         <v>11</v>
@@ -7701,7 +7868,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="I14" s="45">
         <v>10</v>
@@ -7717,7 +7884,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="I16" s="43">
         <v>12</v>
@@ -7725,7 +7892,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="I17" s="43">
         <v>12</v>
@@ -7778,7 +7945,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="G25" s="43">
         <v>5</v>
@@ -7787,7 +7954,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -7845,7 +8012,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="H29" s="43">
         <v>7</v>
@@ -7913,7 +8080,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="I35" s="45">
         <v>8</v>
@@ -7922,7 +8089,7 @@
     <row r="37" ht="15.75"/>
     <row r="38" ht="15.75" spans="1:10">
       <c r="A38" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="B38" s="40"/>
       <c r="C38" s="41"/>
@@ -7932,10 +8099,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="I38" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="J38" s="45">
         <v>12</v>
@@ -7943,10 +8110,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="I39" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="J39" s="45">
         <v>12</v>
@@ -7954,10 +8121,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="I40" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="J40" s="43">
         <v>12</v>
@@ -7965,10 +8132,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="I41" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="J41" s="45">
         <v>10</v>
@@ -7976,10 +8143,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="I42" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="J42" s="45">
         <v>10</v>
@@ -8009,17 +8176,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -8044,7 +8211,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="M15" s="16">
         <v>4</v>
@@ -8062,12 +8229,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="M16" s="16">
         <v>12</v>
@@ -8085,12 +8252,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="M19" s="30">
         <v>15</v>
@@ -8098,10 +8265,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -8154,7 +8321,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -8210,7 +8377,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -8266,7 +8433,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8322,7 +8489,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8378,7 +8545,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -8434,7 +8601,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -8490,17 +8657,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="99" t="s">
-        <v>304</v>
+      <c r="A38" s="107" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="99" t="s">
-        <v>305</v>
+      <c r="A39" s="107" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -8523,7 +8690,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -8572,40 +8739,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="E6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="F6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="G6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="H6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="I6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="J6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="K6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="L6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="M6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="N6" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8616,7 +8783,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8627,7 +8794,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8638,7 +8805,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -8649,7 +8816,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -8676,7 +8843,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8711,7 +8878,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -8743,10 +8910,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -8786,15 +8953,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E12" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -8804,7 +8971,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored decode ways problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="409">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -674,6 +674,42 @@
   </si>
   <si>
     <t>dp[5]</t>
+  </si>
+  <si>
+    <t>Decode Ways</t>
+  </si>
+  <si>
+    <t>s="226"</t>
+  </si>
+  <si>
+    <t>dp[i]=dp[i+1]</t>
+  </si>
+  <si>
+    <t>26 together is 1</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>dp[0]=dp[1]</t>
+  </si>
+  <si>
+    <t>dp[0]=dp[0]+dp[0+2]</t>
+  </si>
+  <si>
+    <t>dp[i]=dp[i]+dp[i+2]</t>
+  </si>
+  <si>
+    <t>s="12106"</t>
+  </si>
+  <si>
+    <t>dp[2]+dp[4]</t>
+  </si>
+  <si>
+    <t>dp[1]+dp[3]</t>
+  </si>
+  <si>
+    <t>dp[0]+dp[2]</t>
   </si>
   <si>
     <t>fib(n)</t>
@@ -1221,11 +1257,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1290,29 +1326,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1327,8 +1340,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1339,21 +1361,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1373,9 +1380,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1412,8 +1418,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1422,6 +1450,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1467,25 +1503,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1497,13 +1527,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1521,13 +1545,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1539,7 +1569,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1557,25 +1623,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1587,19 +1641,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1611,37 +1659,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2118,17 +2154,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2147,6 +2183,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2175,16 +2226,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2200,25 +2251,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2236,134 +2272,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2491,6 +2527,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2905,10 +2961,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z313"/>
+  <dimension ref="A1:Z358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
-      <selection activeCell="B316" sqref="B316"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="H338" sqref="H338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -5890,21 +5946,15 @@
       <c r="A307" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B307"/>
-      <c r="C307"/>
-      <c r="D307"/>
-      <c r="E307"/>
-      <c r="F307"/>
       <c r="G307" s="99" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="308" customFormat="1" ht="15.75"/>
+    <row r="308" ht="15.75"/>
     <row r="309" customFormat="1" ht="15.75" spans="1:10">
       <c r="A309" t="s">
         <v>60</v>
       </c>
-      <c r="B309"/>
       <c r="C309">
         <v>0</v>
       </c>
@@ -5914,10 +5964,6 @@
       <c r="E309">
         <v>0</v>
       </c>
-      <c r="F309"/>
-      <c r="G309"/>
-      <c r="H309"/>
-      <c r="I309"/>
       <c r="J309" t="s">
         <v>211</v>
       </c>
@@ -5926,7 +5972,6 @@
       <c r="A310" t="s">
         <v>64</v>
       </c>
-      <c r="B310"/>
       <c r="C310">
         <v>0</v>
       </c>
@@ -5939,9 +5984,6 @@
       <c r="F310">
         <v>0</v>
       </c>
-      <c r="G310"/>
-      <c r="H310"/>
-      <c r="I310"/>
       <c r="J310" t="s">
         <v>212</v>
       </c>
@@ -6002,8 +6044,6 @@
       <c r="A313" t="s">
         <v>216</v>
       </c>
-      <c r="B313"/>
-      <c r="C313"/>
       <c r="D313" s="104">
         <v>1</v>
       </c>
@@ -6018,6 +6058,326 @@
       </c>
       <c r="H313" s="106">
         <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="319" spans="4:4">
+      <c r="D319" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="321" ht="15.75" spans="1:4">
+      <c r="A321" t="s">
+        <v>12</v>
+      </c>
+      <c r="B321">
+        <v>0</v>
+      </c>
+      <c r="C321">
+        <v>1</v>
+      </c>
+      <c r="D321">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" ht="15.75" spans="1:5">
+      <c r="A322" t="s">
+        <v>33</v>
+      </c>
+      <c r="B322" s="107">
+        <v>2</v>
+      </c>
+      <c r="C322" s="108">
+        <v>2</v>
+      </c>
+      <c r="D322" s="109">
+        <v>6</v>
+      </c>
+      <c r="E322" s="50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5">
+      <c r="A324" t="s">
+        <v>41</v>
+      </c>
+      <c r="B324" s="110">
+        <v>3</v>
+      </c>
+      <c r="C324" s="111">
+        <v>2</v>
+      </c>
+      <c r="D324" s="111">
+        <v>1</v>
+      </c>
+      <c r="E324" s="112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4">
+      <c r="A327" t="s">
+        <v>64</v>
+      </c>
+      <c r="B327" s="113">
+        <v>6</v>
+      </c>
+      <c r="D327" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6">
+      <c r="A329" t="s">
+        <v>60</v>
+      </c>
+      <c r="B329" s="113">
+        <v>2</v>
+      </c>
+      <c r="C329" s="113">
+        <v>6</v>
+      </c>
+      <c r="E329" t="s">
+        <v>219</v>
+      </c>
+      <c r="F329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="5:7">
+      <c r="E330" t="s">
+        <v>220</v>
+      </c>
+      <c r="F330" t="s">
+        <v>221</v>
+      </c>
+      <c r="G330" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" ht="15.75" spans="1:8">
+      <c r="A332" t="s">
+        <v>59</v>
+      </c>
+      <c r="B332" s="113">
+        <v>2</v>
+      </c>
+      <c r="C332" s="113">
+        <v>2</v>
+      </c>
+      <c r="D332" s="113">
+        <v>6</v>
+      </c>
+      <c r="F332" t="s">
+        <v>222</v>
+      </c>
+      <c r="H332">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333" spans="6:8">
+      <c r="F333" t="s">
+        <v>223</v>
+      </c>
+      <c r="H333" s="114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="335" spans="6:6">
+      <c r="F335" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="339" spans="4:4">
+      <c r="D339" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="341" ht="15.75" spans="1:6">
+      <c r="A341" t="s">
+        <v>12</v>
+      </c>
+      <c r="B341">
+        <v>0</v>
+      </c>
+      <c r="C341">
+        <v>1</v>
+      </c>
+      <c r="D341">
+        <v>2</v>
+      </c>
+      <c r="E341">
+        <v>3</v>
+      </c>
+      <c r="F341">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="342" ht="15.75" spans="1:6">
+      <c r="A342" t="s">
+        <v>33</v>
+      </c>
+      <c r="B342" s="115">
+        <v>1</v>
+      </c>
+      <c r="C342" s="116">
+        <v>2</v>
+      </c>
+      <c r="D342" s="116">
+        <v>1</v>
+      </c>
+      <c r="E342" s="117">
+        <v>0</v>
+      </c>
+      <c r="F342" s="118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6">
+      <c r="A344" t="s">
+        <v>41</v>
+      </c>
+      <c r="B344" s="110">
+        <v>2</v>
+      </c>
+      <c r="C344" s="111">
+        <v>1</v>
+      </c>
+      <c r="D344" s="111">
+        <v>1</v>
+      </c>
+      <c r="E344" s="111">
+        <v>0</v>
+      </c>
+      <c r="F344" s="111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4">
+      <c r="A347" t="s">
+        <v>78</v>
+      </c>
+      <c r="B347" s="113">
+        <v>6</v>
+      </c>
+      <c r="D347" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5">
+      <c r="A349" t="s">
+        <v>70</v>
+      </c>
+      <c r="B349" s="113">
+        <v>0</v>
+      </c>
+      <c r="C349" s="113">
+        <v>6</v>
+      </c>
+      <c r="E349" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:9">
+      <c r="A351" t="s">
+        <v>64</v>
+      </c>
+      <c r="B351" s="113">
+        <v>1</v>
+      </c>
+      <c r="C351" s="113">
+        <v>0</v>
+      </c>
+      <c r="D351" s="113">
+        <v>6</v>
+      </c>
+      <c r="F351" t="s">
+        <v>219</v>
+      </c>
+      <c r="G351"/>
+      <c r="H351" t="s">
+        <v>70</v>
+      </c>
+      <c r="I351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="6:9">
+      <c r="F352" t="s">
+        <v>224</v>
+      </c>
+      <c r="H352" t="s">
+        <v>226</v>
+      </c>
+      <c r="I352" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" ht="15.75" spans="1:8">
+      <c r="A354" t="s">
+        <v>60</v>
+      </c>
+      <c r="B354" s="119">
+        <v>2</v>
+      </c>
+      <c r="C354" s="119">
+        <v>1</v>
+      </c>
+      <c r="D354" s="120">
+        <v>0</v>
+      </c>
+      <c r="E354" s="121">
+        <v>6</v>
+      </c>
+      <c r="G354" t="s">
+        <v>64</v>
+      </c>
+      <c r="H354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="7:8">
+      <c r="G355" t="s">
+        <v>227</v>
+      </c>
+      <c r="H355" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" ht="15.75" spans="1:9">
+      <c r="A357" t="s">
+        <v>59</v>
+      </c>
+      <c r="B357" s="122">
+        <v>1</v>
+      </c>
+      <c r="C357" s="119">
+        <v>2</v>
+      </c>
+      <c r="D357" s="119">
+        <v>1</v>
+      </c>
+      <c r="E357" s="120">
+        <v>0</v>
+      </c>
+      <c r="F357" s="121">
+        <v>6</v>
+      </c>
+      <c r="H357" t="s">
+        <v>60</v>
+      </c>
+      <c r="I357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="8:9">
+      <c r="H358" t="s">
+        <v>228</v>
+      </c>
+      <c r="I358" s="114">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6051,13 +6411,13 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" ht="15.75"/>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -6069,7 +6429,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -6105,39 +6465,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" ht="15.75"/>
     <row r="9" customFormat="1" spans="1:5">
       <c r="A9" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="E9" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="E10" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" ht="15.75"/>
     <row r="12" customFormat="1" spans="1:3">
       <c r="A12" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -6156,41 +6516,41 @@
     </row>
     <row r="16" customFormat="1" spans="1:3">
       <c r="A16" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="B16" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="C16" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="F17" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="I17" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="B18" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="C18" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="F18" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -6198,21 +6558,21 @@
     </row>
     <row r="19" customFormat="1" spans="6:6">
       <c r="F19" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
       <c r="A20" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="C20" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="D20" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="F20" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:9">
@@ -6220,19 +6580,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="F22" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="G22" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -6243,15 +6603,15 @@
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="C23" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="3:4">
       <c r="C24" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -6259,7 +6619,7 @@
     </row>
     <row r="27" customFormat="1" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:5">
@@ -6284,34 +6644,34 @@
         <v>174</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" ht="15.75"/>
     <row r="32" customFormat="1" ht="15.75" spans="3:10">
       <c r="C32" s="10" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>178</v>
@@ -6339,7 +6699,7 @@
     </row>
     <row r="34" customFormat="1" spans="1:10">
       <c r="A34" s="10" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -6357,10 +6717,10 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="I34" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="J34" s="24">
         <v>6</v>
@@ -6368,7 +6728,7 @@
     </row>
     <row r="35" customFormat="1" spans="1:10">
       <c r="A35" s="10" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -6384,10 +6744,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="I35" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
       <c r="J35" s="24">
         <v>24</v>
@@ -6395,7 +6755,7 @@
     </row>
     <row r="36" customFormat="1" spans="1:10">
       <c r="A36" s="10" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -6409,10 +6769,10 @@
         <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="I36" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="J36" s="24">
         <v>36</v>
@@ -6420,7 +6780,7 @@
     </row>
     <row r="37" customFormat="1" ht="15.75" spans="1:6">
       <c r="A37" s="10" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -6442,25 +6802,25 @@
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="D39" t="s">
         <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="F39" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="H39" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="I39" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="J39" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="K39">
         <v>32</v>
@@ -6468,13 +6828,13 @@
     </row>
     <row r="40" spans="4:11">
       <c r="D40" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="J40" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="K40" s="24">
         <v>18</v>
@@ -6482,7 +6842,7 @@
     </row>
     <row r="41" customFormat="1" spans="4:4">
       <c r="D41" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="42" spans="4:11">
@@ -6490,19 +6850,19 @@
         <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="F42" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="H42" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="I42" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="J42" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="K42">
         <v>54</v>
@@ -6510,13 +6870,13 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="J43" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="K43" s="24">
         <v>48</v>
@@ -6525,24 +6885,24 @@
     <row r="44" ht="15.75"/>
     <row r="45" customFormat="1" ht="15.75" spans="7:7">
       <c r="G45" s="11" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="2:10">
       <c r="B46" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="C46" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="G46" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="H46" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="I46" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="J46">
         <v>54</v>
@@ -6550,16 +6910,16 @@
     </row>
     <row r="47" customFormat="1" spans="2:10">
       <c r="B47" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="C47" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="H47" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="I47" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="J47">
         <v>51</v>
@@ -6567,17 +6927,17 @@
     </row>
     <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="23" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="C48" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="I48" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="J48" s="24">
         <v>30</v>
@@ -6588,10 +6948,10 @@
         <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -6654,7 +7014,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="B2" s="50">
         <v>0</v>
@@ -6728,22 +7088,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>2</v>
@@ -6760,7 +7120,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
@@ -6774,7 +7134,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>2</v>
@@ -6785,7 +7145,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -6805,12 +7165,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -6914,7 +7274,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -6934,17 +7294,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
@@ -6956,18 +7316,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>6</v>
@@ -6975,18 +7335,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -6998,7 +7358,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -7006,12 +7366,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -7019,7 +7379,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -7081,7 +7441,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="24" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="C51" s="16">
         <v>1</v>
@@ -7115,7 +7475,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -7127,7 +7487,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -7155,12 +7515,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="25" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -7253,10 +7613,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -7271,7 +7631,7 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -7291,7 +7651,7 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="K11" s="24">
         <v>3</v>
@@ -7318,13 +7678,13 @@
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="F14" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="M14" s="47">
         <v>2</v>
@@ -7332,7 +7692,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="G15" s="24">
         <v>2</v>
@@ -7350,7 +7710,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="G17" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -7358,7 +7718,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="I18" s="24">
         <v>2</v>
@@ -7369,25 +7729,25 @@
         <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="C20" s="16">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="K20" s="16">
         <v>3</v>
@@ -7396,21 +7756,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="C21" s="16">
         <v>3</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="G21" s="16">
         <v>3</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="K21" s="16">
         <v>2</v>
@@ -7419,21 +7779,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="G22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="K22" s="28">
         <v>2</v>
@@ -7441,28 +7801,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="C24" s="16">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="G24" s="16">
         <v>4</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="K24" s="16">
         <v>4</v>
@@ -7471,21 +7831,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="C25" s="16">
         <v>3</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="G25" s="16">
         <v>3</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="K25" s="16">
         <v>4</v>
@@ -7494,21 +7854,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="C26" s="28">
         <v>3</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="G26" s="28">
         <v>3</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="K26" s="28">
         <v>2</v>
@@ -7538,7 +7898,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>31</v>
@@ -7558,7 +7918,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -7603,27 +7963,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -7773,7 +8133,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="L3" s="46">
         <v>5</v>
@@ -7787,7 +8147,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -7834,7 +8194,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -7844,7 +8204,7 @@
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="H11" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="I11" s="45">
         <v>10</v>
@@ -7852,7 +8212,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="I12" s="45">
         <v>11</v>
@@ -7860,7 +8220,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="I13" s="45">
         <v>11</v>
@@ -7868,7 +8228,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="I14" s="45">
         <v>10</v>
@@ -7884,7 +8244,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="I16" s="43">
         <v>12</v>
@@ -7892,7 +8252,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="I17" s="43">
         <v>12</v>
@@ -7945,7 +8305,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="G25" s="43">
         <v>5</v>
@@ -7954,7 +8314,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -8012,7 +8372,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="H29" s="43">
         <v>7</v>
@@ -8080,7 +8440,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="I35" s="45">
         <v>8</v>
@@ -8099,10 +8459,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="I38" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="J38" s="45">
         <v>12</v>
@@ -8110,10 +8470,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="I39" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="J39" s="45">
         <v>12</v>
@@ -8121,10 +8481,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="I40" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="J40" s="43">
         <v>12</v>
@@ -8132,10 +8492,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="I41" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="J41" s="45">
         <v>10</v>
@@ -8143,10 +8503,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="I42" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="J42" s="45">
         <v>10</v>
@@ -8176,17 +8536,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -8211,7 +8571,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="M15" s="16">
         <v>4</v>
@@ -8229,12 +8589,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="M16" s="16">
         <v>12</v>
@@ -8252,12 +8612,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="M19" s="30">
         <v>15</v>
@@ -8265,10 +8625,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -8321,7 +8681,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -8377,7 +8737,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -8433,7 +8793,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8489,7 +8849,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8545,7 +8905,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -8601,7 +8961,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -8657,17 +9017,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="107" t="s">
-        <v>311</v>
+      <c r="A38" s="123" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="107" t="s">
-        <v>312</v>
+      <c r="A39" s="123" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -8690,7 +9050,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -8739,40 +9099,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="D6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="E6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="F6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="G6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="H6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="I6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="J6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="K6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="L6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="M6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="N6" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8783,7 +9143,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8794,7 +9154,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8805,7 +9165,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -8816,7 +9176,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -8843,7 +9203,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8878,7 +9238,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -8910,10 +9270,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -8953,15 +9313,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="E12" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -8971,7 +9331,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved Count Vowels Permutation
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="422">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -712,6 +712,48 @@
     <t>dp[0]+dp[2]</t>
   </si>
   <si>
+    <t>Unique Paths</t>
+  </si>
+  <si>
+    <t>Input: m = 3, n = 7</t>
+  </si>
+  <si>
+    <t>n=0</t>
+  </si>
+  <si>
+    <t>n=1</t>
+  </si>
+  <si>
+    <t>n=2</t>
+  </si>
+  <si>
+    <t>n=3</t>
+  </si>
+  <si>
+    <t>n=4</t>
+  </si>
+  <si>
+    <t>n=5</t>
+  </si>
+  <si>
+    <t>n=6</t>
+  </si>
+  <si>
+    <t>m=0</t>
+  </si>
+  <si>
+    <t>START 28</t>
+  </si>
+  <si>
+    <t>m=1</t>
+  </si>
+  <si>
+    <t>m=2</t>
+  </si>
+  <si>
+    <t>FINISH 1</t>
+  </si>
+  <si>
     <t>fib(n)</t>
   </si>
   <si>
@@ -944,9 +986,6 @@
   </si>
   <si>
     <t>0-1 Knapsack Problem</t>
-  </si>
-  <si>
-    <t>n=5</t>
   </si>
   <si>
     <t>c=15</t>
@@ -1257,11 +1296,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1326,8 +1365,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1340,9 +1380,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1357,7 +1403,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1372,31 +1418,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1410,14 +1455,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1426,24 +1463,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1464,13 +1496,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1503,49 +1542,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1563,7 +1560,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1575,7 +1608,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1587,7 +1674,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1605,31 +1704,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1641,37 +1716,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2154,6 +2199,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2169,20 +2223,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2198,21 +2249,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2251,10 +2287,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2272,134 +2317,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2527,26 +2572,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2961,10 +3008,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z358"/>
+  <dimension ref="A1:Z371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="H338" sqref="H338"/>
+    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="B374" sqref="B374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6088,13 +6135,13 @@
       <c r="A322" t="s">
         <v>33</v>
       </c>
-      <c r="B322" s="107">
-        <v>2</v>
-      </c>
-      <c r="C322" s="108">
-        <v>2</v>
-      </c>
-      <c r="D322" s="109">
+      <c r="B322" s="70">
+        <v>2</v>
+      </c>
+      <c r="C322" s="71">
+        <v>2</v>
+      </c>
+      <c r="D322" s="107">
         <v>6</v>
       </c>
       <c r="E322" s="50" t="s">
@@ -6105,16 +6152,16 @@
       <c r="A324" t="s">
         <v>41</v>
       </c>
-      <c r="B324" s="110">
-        <v>3</v>
-      </c>
-      <c r="C324" s="111">
-        <v>2</v>
-      </c>
-      <c r="D324" s="111">
-        <v>1</v>
-      </c>
-      <c r="E324" s="112">
+      <c r="B324" s="28">
+        <v>3</v>
+      </c>
+      <c r="C324" s="16">
+        <v>2</v>
+      </c>
+      <c r="D324" s="16">
+        <v>1</v>
+      </c>
+      <c r="E324" s="29">
         <v>1</v>
       </c>
     </row>
@@ -6122,10 +6169,10 @@
       <c r="A327" t="s">
         <v>64</v>
       </c>
-      <c r="B327" s="113">
+      <c r="B327" s="63">
         <v>6</v>
       </c>
-      <c r="D327" s="114">
+      <c r="D327" s="24">
         <v>1</v>
       </c>
     </row>
@@ -6133,10 +6180,10 @@
       <c r="A329" t="s">
         <v>60</v>
       </c>
-      <c r="B329" s="113">
-        <v>2</v>
-      </c>
-      <c r="C329" s="113">
+      <c r="B329" s="63">
+        <v>2</v>
+      </c>
+      <c r="C329" s="63">
         <v>6</v>
       </c>
       <c r="E329" t="s">
@@ -6153,21 +6200,21 @@
       <c r="F330" t="s">
         <v>221</v>
       </c>
-      <c r="G330" s="114">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="332" ht="15.75" spans="1:8">
+      <c r="G330" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8">
       <c r="A332" t="s">
         <v>59</v>
       </c>
-      <c r="B332" s="113">
-        <v>2</v>
-      </c>
-      <c r="C332" s="113">
-        <v>2</v>
-      </c>
-      <c r="D332" s="113">
+      <c r="B332" s="63">
+        <v>2</v>
+      </c>
+      <c r="C332" s="63">
+        <v>2</v>
+      </c>
+      <c r="D332" s="63">
         <v>6</v>
       </c>
       <c r="F332" t="s">
@@ -6181,7 +6228,7 @@
       <c r="F333" t="s">
         <v>223</v>
       </c>
-      <c r="H333" s="114">
+      <c r="H333" s="24">
         <v>3</v>
       </c>
     </row>
@@ -6219,19 +6266,19 @@
       <c r="A342" t="s">
         <v>33</v>
       </c>
-      <c r="B342" s="115">
-        <v>1</v>
-      </c>
-      <c r="C342" s="116">
-        <v>2</v>
-      </c>
-      <c r="D342" s="116">
-        <v>1</v>
-      </c>
-      <c r="E342" s="117">
-        <v>0</v>
-      </c>
-      <c r="F342" s="118">
+      <c r="B342" s="70">
+        <v>1</v>
+      </c>
+      <c r="C342" s="71">
+        <v>2</v>
+      </c>
+      <c r="D342" s="71">
+        <v>1</v>
+      </c>
+      <c r="E342" s="108">
+        <v>0</v>
+      </c>
+      <c r="F342" s="107">
         <v>6</v>
       </c>
     </row>
@@ -6239,19 +6286,19 @@
       <c r="A344" t="s">
         <v>41</v>
       </c>
-      <c r="B344" s="110">
-        <v>2</v>
-      </c>
-      <c r="C344" s="111">
-        <v>1</v>
-      </c>
-      <c r="D344" s="111">
-        <v>1</v>
-      </c>
-      <c r="E344" s="111">
-        <v>0</v>
-      </c>
-      <c r="F344" s="111">
+      <c r="B344" s="28">
+        <v>2</v>
+      </c>
+      <c r="C344" s="16">
+        <v>1</v>
+      </c>
+      <c r="D344" s="16">
+        <v>1</v>
+      </c>
+      <c r="E344" s="16">
+        <v>0</v>
+      </c>
+      <c r="F344" s="16">
         <v>1</v>
       </c>
     </row>
@@ -6259,10 +6306,10 @@
       <c r="A347" t="s">
         <v>78</v>
       </c>
-      <c r="B347" s="113">
+      <c r="B347" s="63">
         <v>6</v>
       </c>
-      <c r="D347" s="114">
+      <c r="D347" s="24">
         <v>1</v>
       </c>
     </row>
@@ -6270,13 +6317,13 @@
       <c r="A349" t="s">
         <v>70</v>
       </c>
-      <c r="B349" s="113">
-        <v>0</v>
-      </c>
-      <c r="C349" s="113">
+      <c r="B349" s="63">
+        <v>0</v>
+      </c>
+      <c r="C349" s="63">
         <v>6</v>
       </c>
-      <c r="E349" s="114">
+      <c r="E349" s="24">
         <v>0</v>
       </c>
     </row>
@@ -6284,19 +6331,18 @@
       <c r="A351" t="s">
         <v>64</v>
       </c>
-      <c r="B351" s="113">
-        <v>1</v>
-      </c>
-      <c r="C351" s="113">
-        <v>0</v>
-      </c>
-      <c r="D351" s="113">
+      <c r="B351" s="63">
+        <v>1</v>
+      </c>
+      <c r="C351" s="63">
+        <v>0</v>
+      </c>
+      <c r="D351" s="63">
         <v>6</v>
       </c>
       <c r="F351" t="s">
         <v>219</v>
       </c>
-      <c r="G351"/>
       <c r="H351" t="s">
         <v>70</v>
       </c>
@@ -6311,24 +6357,25 @@
       <c r="H352" t="s">
         <v>226</v>
       </c>
-      <c r="I352" s="114">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="I352" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" ht="15.75"/>
     <row r="354" ht="15.75" spans="1:8">
       <c r="A354" t="s">
         <v>60</v>
       </c>
-      <c r="B354" s="119">
-        <v>2</v>
-      </c>
-      <c r="C354" s="119">
-        <v>1</v>
-      </c>
-      <c r="D354" s="120">
-        <v>0</v>
-      </c>
-      <c r="E354" s="121">
+      <c r="B354" s="109">
+        <v>2</v>
+      </c>
+      <c r="C354" s="109">
+        <v>1</v>
+      </c>
+      <c r="D354" s="110">
+        <v>0</v>
+      </c>
+      <c r="E354" s="111">
         <v>6</v>
       </c>
       <c r="G354" t="s">
@@ -6342,27 +6389,28 @@
       <c r="G355" t="s">
         <v>227</v>
       </c>
-      <c r="H355" s="114">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="H355" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" ht="15.75"/>
     <row r="357" ht="15.75" spans="1:9">
       <c r="A357" t="s">
         <v>59</v>
       </c>
-      <c r="B357" s="122">
-        <v>1</v>
-      </c>
-      <c r="C357" s="119">
-        <v>2</v>
-      </c>
-      <c r="D357" s="119">
-        <v>1</v>
-      </c>
-      <c r="E357" s="120">
-        <v>0</v>
-      </c>
-      <c r="F357" s="121">
+      <c r="B357" s="112">
+        <v>1</v>
+      </c>
+      <c r="C357" s="109">
+        <v>2</v>
+      </c>
+      <c r="D357" s="109">
+        <v>1</v>
+      </c>
+      <c r="E357" s="110">
+        <v>0</v>
+      </c>
+      <c r="F357" s="111">
         <v>6</v>
       </c>
       <c r="H357" t="s">
@@ -6376,8 +6424,121 @@
       <c r="H358" t="s">
         <v>228</v>
       </c>
-      <c r="I358" s="114">
-        <v>2</v>
+      <c r="I358" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361" customFormat="1"/>
+    <row r="362" customFormat="1"/>
+    <row r="363" customFormat="1"/>
+    <row r="364" customFormat="1"/>
+    <row r="366" spans="1:4">
+      <c r="A366" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="368" ht="15.75" spans="3:9">
+      <c r="C368" t="s">
+        <v>231</v>
+      </c>
+      <c r="D368" t="s">
+        <v>232</v>
+      </c>
+      <c r="E368" t="s">
+        <v>233</v>
+      </c>
+      <c r="F368" t="s">
+        <v>234</v>
+      </c>
+      <c r="G368" t="s">
+        <v>235</v>
+      </c>
+      <c r="H368" t="s">
+        <v>236</v>
+      </c>
+      <c r="I368" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="369" spans="2:9">
+      <c r="B369" t="s">
+        <v>238</v>
+      </c>
+      <c r="C369" s="113" t="s">
+        <v>239</v>
+      </c>
+      <c r="D369" s="114">
+        <v>21</v>
+      </c>
+      <c r="E369" s="115">
+        <v>15</v>
+      </c>
+      <c r="F369" s="114">
+        <v>10</v>
+      </c>
+      <c r="G369" s="115">
+        <v>6</v>
+      </c>
+      <c r="H369" s="114">
+        <v>3</v>
+      </c>
+      <c r="I369" s="122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="2:9">
+      <c r="B370" t="s">
+        <v>240</v>
+      </c>
+      <c r="C370" s="116">
+        <v>7</v>
+      </c>
+      <c r="D370" s="117">
+        <v>6</v>
+      </c>
+      <c r="E370" s="118">
+        <v>5</v>
+      </c>
+      <c r="F370" s="117">
+        <v>4</v>
+      </c>
+      <c r="G370" s="118">
+        <v>3</v>
+      </c>
+      <c r="H370" s="117">
+        <v>2</v>
+      </c>
+      <c r="I370" s="123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" ht="15.75" spans="2:9">
+      <c r="B371" t="s">
+        <v>241</v>
+      </c>
+      <c r="C371" s="119">
+        <v>1</v>
+      </c>
+      <c r="D371" s="120">
+        <v>1</v>
+      </c>
+      <c r="E371" s="121">
+        <v>1</v>
+      </c>
+      <c r="F371" s="120">
+        <v>1</v>
+      </c>
+      <c r="G371" s="121">
+        <v>1</v>
+      </c>
+      <c r="H371" s="120">
+        <v>1</v>
+      </c>
+      <c r="I371" s="124" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -6411,13 +6572,13 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" ht="15.75"/>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -6429,7 +6590,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -6465,39 +6626,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>339</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" ht="15.75"/>
     <row r="9" customFormat="1" spans="1:5">
       <c r="A9" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="E9" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>344</v>
+        <v>357</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="E10" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" ht="15.75"/>
     <row r="12" customFormat="1" spans="1:3">
       <c r="A12" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -6516,41 +6677,41 @@
     </row>
     <row r="16" customFormat="1" spans="1:3">
       <c r="A16" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="B16" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="C16" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>349</v>
+        <v>362</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="F17" t="s">
-        <v>351</v>
+        <v>364</v>
       </c>
       <c r="I17" t="s">
-        <v>352</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" t="s">
-        <v>353</v>
+        <v>366</v>
       </c>
       <c r="B18" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="C18" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
       <c r="F18" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -6558,21 +6719,21 @@
     </row>
     <row r="19" customFormat="1" spans="6:6">
       <c r="F19" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
       <c r="A20" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="C20" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="D20" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="F20" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:9">
@@ -6580,19 +6741,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="F22" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
       <c r="G22" t="s">
-        <v>364</v>
+        <v>377</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -6603,15 +6764,15 @@
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" t="s">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="C23" t="s">
-        <v>366</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="3:4">
       <c r="C24" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -6619,7 +6780,7 @@
     </row>
     <row r="27" customFormat="1" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>368</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:5">
@@ -6644,34 +6805,34 @@
         <v>174</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" ht="15.75"/>
     <row r="32" customFormat="1" ht="15.75" spans="3:10">
       <c r="C32" s="10" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>178</v>
@@ -6699,7 +6860,7 @@
     </row>
     <row r="34" customFormat="1" spans="1:10">
       <c r="A34" s="10" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -6717,10 +6878,10 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
       <c r="I34" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
       <c r="J34" s="24">
         <v>6</v>
@@ -6728,7 +6889,7 @@
     </row>
     <row r="35" customFormat="1" spans="1:10">
       <c r="A35" s="10" t="s">
-        <v>370</v>
+        <v>383</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -6744,10 +6905,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="I35" t="s">
-        <v>377</v>
+        <v>390</v>
       </c>
       <c r="J35" s="24">
         <v>24</v>
@@ -6755,7 +6916,7 @@
     </row>
     <row r="36" customFormat="1" spans="1:10">
       <c r="A36" s="10" t="s">
-        <v>371</v>
+        <v>384</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -6769,10 +6930,10 @@
         <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="I36" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="J36" s="24">
         <v>36</v>
@@ -6780,7 +6941,7 @@
     </row>
     <row r="37" customFormat="1" ht="15.75" spans="1:6">
       <c r="A37" s="10" t="s">
-        <v>372</v>
+        <v>385</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -6802,25 +6963,25 @@
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="D39" t="s">
         <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="F39" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="H39" t="s">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="I39" t="s">
-        <v>383</v>
+        <v>396</v>
       </c>
       <c r="J39" t="s">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="K39">
         <v>32</v>
@@ -6828,13 +6989,13 @@
     </row>
     <row r="40" spans="4:11">
       <c r="D40" t="s">
-        <v>385</v>
+        <v>398</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>386</v>
+        <v>399</v>
       </c>
       <c r="J40" t="s">
-        <v>387</v>
+        <v>400</v>
       </c>
       <c r="K40" s="24">
         <v>18</v>
@@ -6842,7 +7003,7 @@
     </row>
     <row r="41" customFormat="1" spans="4:4">
       <c r="D41" t="s">
-        <v>388</v>
+        <v>401</v>
       </c>
     </row>
     <row r="42" spans="4:11">
@@ -6850,19 +7011,19 @@
         <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="F42" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="H42" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="I42" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="J42" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="K42">
         <v>54</v>
@@ -6870,13 +7031,13 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="J43" t="s">
-        <v>395</v>
+        <v>408</v>
       </c>
       <c r="K43" s="24">
         <v>48</v>
@@ -6885,24 +7046,24 @@
     <row r="44" ht="15.75"/>
     <row r="45" customFormat="1" ht="15.75" spans="7:7">
       <c r="G45" s="11" t="s">
-        <v>396</v>
+        <v>409</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="2:10">
       <c r="B46" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="C46" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="G46" t="s">
-        <v>399</v>
+        <v>412</v>
       </c>
       <c r="H46" t="s">
-        <v>397</v>
+        <v>410</v>
       </c>
       <c r="I46" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
       <c r="J46">
         <v>54</v>
@@ -6910,16 +7071,16 @@
     </row>
     <row r="47" customFormat="1" spans="2:10">
       <c r="B47" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="C47" t="s">
-        <v>402</v>
+        <v>415</v>
       </c>
       <c r="H47" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="I47" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="J47">
         <v>51</v>
@@ -6927,17 +7088,17 @@
     </row>
     <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="23" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="C48" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>404</v>
+        <v>417</v>
       </c>
       <c r="I48" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="J48" s="24">
         <v>30</v>
@@ -6948,10 +7109,10 @@
         <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -7014,7 +7175,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B2" s="50">
         <v>0</v>
@@ -7088,22 +7249,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>2</v>
@@ -7120,7 +7281,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
@@ -7134,7 +7295,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>2</v>
@@ -7145,7 +7306,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -7165,12 +7326,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -7274,7 +7435,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -7294,17 +7455,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
@@ -7316,18 +7477,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>6</v>
@@ -7335,18 +7496,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -7358,7 +7519,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -7366,12 +7527,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -7379,7 +7540,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -7441,7 +7602,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="24" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="C51" s="16">
         <v>1</v>
@@ -7475,7 +7636,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -7487,7 +7648,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -7515,12 +7676,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="25" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -7613,10 +7774,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -7631,7 +7792,7 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -7651,7 +7812,7 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="K11" s="24">
         <v>3</v>
@@ -7678,13 +7839,13 @@
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="F14" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="M14" s="47">
         <v>2</v>
@@ -7692,7 +7853,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="G15" s="24">
         <v>2</v>
@@ -7710,7 +7871,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="G17" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -7718,7 +7879,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="I18" s="24">
         <v>2</v>
@@ -7729,25 +7890,25 @@
         <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="C20" s="16">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="K20" s="16">
         <v>3</v>
@@ -7756,21 +7917,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="C21" s="16">
         <v>3</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="G21" s="16">
         <v>3</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="K21" s="16">
         <v>2</v>
@@ -7779,21 +7940,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="G22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="K22" s="28">
         <v>2</v>
@@ -7801,28 +7962,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
       <c r="C24" s="16">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G24" s="16">
         <v>4</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="K24" s="16">
         <v>4</v>
@@ -7831,21 +7992,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="C25" s="16">
         <v>3</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="G25" s="16">
         <v>3</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="K25" s="16">
         <v>4</v>
@@ -7854,21 +8015,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="C26" s="28">
         <v>3</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="G26" s="28">
         <v>3</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="K26" s="28">
         <v>2</v>
@@ -7898,7 +8059,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>31</v>
@@ -7918,7 +8079,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -7963,27 +8124,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -8133,7 +8294,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="L3" s="46">
         <v>5</v>
@@ -8147,7 +8308,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -8194,7 +8355,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -8204,7 +8365,7 @@
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="H11" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="I11" s="45">
         <v>10</v>
@@ -8212,7 +8373,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="I12" s="45">
         <v>11</v>
@@ -8220,7 +8381,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="I13" s="45">
         <v>11</v>
@@ -8228,7 +8389,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="I14" s="45">
         <v>10</v>
@@ -8244,7 +8405,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="I16" s="43">
         <v>12</v>
@@ -8252,7 +8413,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="I17" s="43">
         <v>12</v>
@@ -8305,7 +8466,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="G25" s="43">
         <v>5</v>
@@ -8314,7 +8475,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -8372,7 +8533,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="H29" s="43">
         <v>7</v>
@@ -8440,7 +8601,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="I35" s="45">
         <v>8</v>
@@ -8459,10 +8620,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="I38" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
       <c r="J38" s="45">
         <v>12</v>
@@ -8470,10 +8631,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="I39" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="J39" s="45">
         <v>12</v>
@@ -8481,10 +8642,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="I40" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="J40" s="43">
         <v>12</v>
@@ -8492,10 +8653,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="I41" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="J41" s="45">
         <v>10</v>
@@ -8503,10 +8664,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="I42" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="J42" s="45">
         <v>10</v>
@@ -8536,17 +8697,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="12:12">
       <c r="L11" t="s">
-        <v>307</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>308</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -8571,7 +8732,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="M15" s="16">
         <v>4</v>
@@ -8589,12 +8750,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="M16" s="16">
         <v>12</v>
@@ -8612,12 +8773,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="M19" s="30">
         <v>15</v>
@@ -8625,10 +8786,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -8681,7 +8842,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -8737,7 +8898,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -8793,7 +8954,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8849,7 +9010,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8905,7 +9066,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -8961,7 +9122,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -9017,17 +9178,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="123" t="s">
-        <v>323</v>
+      <c r="A38" s="125" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="123" t="s">
-        <v>324</v>
+      <c r="A39" s="125" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -9050,7 +9211,7 @@
   <sheetData>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>325</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -9099,40 +9260,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
       <c r="D6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="E6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="F6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="G6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="H6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="I6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="J6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="K6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="L6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="M6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="N6" t="s">
-        <v>327</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -9143,7 +9304,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -9154,7 +9315,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -9165,7 +9326,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -9176,7 +9337,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>326</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -9203,7 +9364,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -9238,7 +9399,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -9270,10 +9431,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -9313,15 +9474,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="E12" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>334</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -9331,7 +9492,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added README for Target Sum problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView windowWidth="27428" windowHeight="11734"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="445">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -775,6 +775,60 @@
   </si>
   <si>
     <t>Count Vowels Permutation</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>a-&gt;e = "ae"</t>
+  </si>
+  <si>
+    <t>e-&gt;a = "ea"</t>
+  </si>
+  <si>
+    <t>i-&gt;a = "ia"</t>
+  </si>
+  <si>
+    <t>o-&gt;i = "oi"</t>
+  </si>
+  <si>
+    <t>u-&gt;a = "ua"</t>
+  </si>
+  <si>
+    <t>e-&gt;i = "ei"</t>
+  </si>
+  <si>
+    <t>i-&gt;e = "ie"</t>
+  </si>
+  <si>
+    <t>o-&gt;u = "ou"</t>
+  </si>
+  <si>
+    <t>i-&gt;o = "io"</t>
+  </si>
+  <si>
+    <t>i-&gt;u = "iu"</t>
+  </si>
+  <si>
+    <t>ending with char (down)</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>a2 = e1+i1+u1</t>
+  </si>
+  <si>
+    <t>e2 = a1+i1</t>
+  </si>
+  <si>
+    <t>i2 = e1+o1</t>
+  </si>
+  <si>
+    <t>o2 = i1</t>
+  </si>
+  <si>
+    <t>u2 = i2+o2</t>
   </si>
   <si>
     <t>fib(n)</t>
@@ -1310,11 +1364,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1380,6 +1434,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1388,22 +1450,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1421,14 +1484,6 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1479,14 +1534,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -1494,16 +1541,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1518,6 +1565,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1562,6 +1616,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1574,7 +1646,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1586,7 +1658,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1598,25 +1718,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,61 +1736,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1694,7 +1748,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1706,7 +1772,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1724,24 +1790,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -2213,26 +2267,108 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2285,41 +2421,39 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2331,31 +2465,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="48" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2364,101 +2498,101 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2604,13 +2738,25 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2703,8 +2849,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="929005" y="770255"/>
-          <a:ext cx="4342130" cy="2425700"/>
+          <a:off x="963930" y="747395"/>
+          <a:ext cx="4586605" cy="2357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2750,8 +2896,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1584325" y="723265"/>
-          <a:ext cx="4304030" cy="3704590"/>
+          <a:off x="1647190" y="706120"/>
+          <a:ext cx="4572000" cy="3590290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3025,23 +3171,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z398"/>
+  <dimension ref="A1:Z413"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="A400" sqref="A400"/>
+      <selection activeCell="A398" sqref="A398"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="12.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="12.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="26.2857142857143" customWidth="1"/>
-    <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
-    <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
-    <col min="9" max="9" width="16.2857142857143" customWidth="1"/>
-    <col min="11" max="11" width="13.7428571428571" customWidth="1"/>
+    <col min="1" max="1" width="24.7837837837838" customWidth="1"/>
+    <col min="2" max="2" width="19.1441441441441" customWidth="1"/>
+    <col min="3" max="3" width="12.5675675675676" customWidth="1"/>
+    <col min="4" max="4" width="27.5675675675676" customWidth="1"/>
+    <col min="5" max="5" width="26.2882882882883" customWidth="1"/>
+    <col min="6" max="7" width="12.3153153153153" customWidth="1"/>
+    <col min="8" max="8" width="13.1261261261261" customWidth="1"/>
+    <col min="9" max="9" width="16.2882882882883" customWidth="1"/>
+    <col min="11" max="11" width="13.7387387387387" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -3622,26 +3768,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" ht="15.75"/>
-    <row r="67" ht="15.75" spans="7:7">
+    <row r="66" ht="15.3"/>
+    <row r="67" ht="15.3" spans="7:7">
       <c r="G67" s="53"/>
     </row>
-    <row r="68" ht="15.75" spans="6:7">
+    <row r="68" ht="15.3" spans="6:7">
       <c r="F68" s="54"/>
       <c r="G68" s="55"/>
     </row>
-    <row r="69" ht="15.75" spans="5:7">
+    <row r="69" ht="15.3" spans="5:7">
       <c r="E69" s="54"/>
       <c r="F69" s="56"/>
       <c r="G69" s="55"/>
     </row>
-    <row r="70" ht="15.75" spans="4:7">
+    <row r="70" ht="15.3" spans="4:7">
       <c r="D70" s="54"/>
       <c r="E70" s="56"/>
       <c r="F70" s="56"/>
       <c r="G70" s="55"/>
     </row>
-    <row r="71" ht="15.75" spans="2:7">
+    <row r="71" ht="15.3" spans="2:7">
       <c r="B71" s="20"/>
       <c r="C71" s="37"/>
       <c r="D71" s="57"/>
@@ -3714,26 +3860,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" ht="15.75"/>
-    <row r="80" ht="15.75" spans="7:7">
+    <row r="79" ht="15.3"/>
+    <row r="80" ht="15.3" spans="7:7">
       <c r="G80" s="53"/>
     </row>
-    <row r="81" ht="15.75" spans="6:7">
+    <row r="81" ht="15.3" spans="6:7">
       <c r="F81" s="54"/>
       <c r="G81" s="55"/>
     </row>
-    <row r="82" ht="15.75" spans="5:7">
+    <row r="82" ht="15.3" spans="5:7">
       <c r="E82" s="54"/>
       <c r="F82" s="56"/>
       <c r="G82" s="55"/>
     </row>
-    <row r="83" ht="15.75" spans="4:7">
+    <row r="83" ht="15.3" spans="4:7">
       <c r="D83" s="54"/>
       <c r="E83" s="56"/>
       <c r="F83" s="56"/>
       <c r="G83" s="55"/>
     </row>
-    <row r="84" ht="15.75" spans="2:7">
+    <row r="84" ht="15.3" spans="2:7">
       <c r="B84" s="20"/>
       <c r="C84" s="37"/>
       <c r="D84" s="57"/>
@@ -5312,10 +5458,10 @@
         <v>158</v>
       </c>
     </row>
-    <row r="250" ht="15.75" spans="1:1">
+    <row r="250" ht="15.3" spans="1:1">
       <c r="A250" s="1"/>
     </row>
-    <row r="251" ht="15.75" spans="1:10">
+    <row r="251" ht="15.3" spans="1:10">
       <c r="A251" s="66" t="s">
         <v>159</v>
       </c>
@@ -5332,7 +5478,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="252" ht="15.75" spans="1:7">
+    <row r="252" ht="15.3" spans="1:7">
       <c r="A252" s="1">
         <v>0</v>
       </c>
@@ -5352,7 +5498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" ht="15.75" spans="1:12">
+    <row r="253" ht="15.3" spans="1:12">
       <c r="A253" s="11">
         <v>1</v>
       </c>
@@ -5410,7 +5556,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="255" ht="15.75" spans="1:12">
+    <row r="255" ht="15.3" spans="1:12">
       <c r="A255" s="1">
         <v>3</v>
       </c>
@@ -5523,7 +5669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" ht="15.75" spans="1:10">
+    <row r="259" ht="15.3" spans="1:10">
       <c r="A259" s="86">
         <v>7</v>
       </c>
@@ -5698,7 +5844,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="267" ht="15.75" spans="1:8">
+    <row r="267" ht="15.3" spans="1:8">
       <c r="A267" s="94">
         <v>15</v>
       </c>
@@ -5773,7 +5919,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="279" ht="15.75" spans="3:7">
+    <row r="279" ht="15.3" spans="3:7">
       <c r="C279">
         <v>0</v>
       </c>
@@ -5837,7 +5983,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="282" ht="15.75" spans="1:5">
+    <row r="282" ht="15.3" spans="1:5">
       <c r="A282" s="10" t="s">
         <v>177</v>
       </c>
@@ -5883,7 +6029,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="287" ht="15.75" spans="8:8">
+    <row r="287" ht="15.3" spans="8:8">
       <c r="H287" s="1" t="s">
         <v>190</v>
       </c>
@@ -5899,7 +6045,7 @@
       <c r="O288" s="36"/>
       <c r="P288" s="35"/>
     </row>
-    <row r="289" ht="15.75" spans="10:16">
+    <row r="289" ht="15.3" spans="10:16">
       <c r="J289" s="94" t="s">
         <v>192</v>
       </c>
@@ -6014,8 +6160,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="308" ht="15.75"/>
-    <row r="309" customFormat="1" ht="15.75" spans="1:10">
+    <row r="308" ht="15.3"/>
+    <row r="309" customFormat="1" ht="15.3" spans="1:10">
       <c r="A309" t="s">
         <v>60</v>
       </c>
@@ -6032,7 +6178,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="310" customFormat="1" ht="15.75" spans="1:10">
+    <row r="310" customFormat="1" ht="15.3" spans="1:10">
       <c r="A310" t="s">
         <v>64</v>
       </c>
@@ -6052,7 +6198,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="311" ht="15.75" spans="1:11">
+    <row r="311" ht="15.3" spans="1:11">
       <c r="A311" t="s">
         <v>70</v>
       </c>
@@ -6078,7 +6224,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="312" ht="15.75" spans="1:11">
+    <row r="312" ht="15.3" spans="1:11">
       <c r="A312" t="s">
         <v>78</v>
       </c>
@@ -6104,7 +6250,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="313" customFormat="1" ht="15.75" spans="1:8">
+    <row r="313" customFormat="1" ht="15.3" spans="1:8">
       <c r="A313" t="s">
         <v>216</v>
       </c>
@@ -6134,7 +6280,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="321" ht="15.75" spans="1:4">
+    <row r="321" ht="15.3" spans="1:4">
       <c r="A321" t="s">
         <v>12</v>
       </c>
@@ -6148,7 +6294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" ht="15.75" spans="1:5">
+    <row r="322" ht="15.3" spans="1:5">
       <c r="A322" t="s">
         <v>33</v>
       </c>
@@ -6259,7 +6405,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="341" ht="15.75" spans="1:6">
+    <row r="341" ht="15.3" spans="1:6">
       <c r="A341" t="s">
         <v>12</v>
       </c>
@@ -6279,7 +6425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" ht="15.75" spans="1:6">
+    <row r="342" ht="15.3" spans="1:6">
       <c r="A342" t="s">
         <v>33</v>
       </c>
@@ -6378,8 +6524,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" ht="15.75"/>
-    <row r="354" ht="15.75" spans="1:8">
+    <row r="353" ht="15.3"/>
+    <row r="354" ht="15.3" spans="1:8">
       <c r="A354" t="s">
         <v>60</v>
       </c>
@@ -6410,8 +6556,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" ht="15.75"/>
-    <row r="357" ht="15.75" spans="1:9">
+    <row r="356" ht="15.3"/>
+    <row r="357" ht="15.3" spans="1:9">
       <c r="A357" t="s">
         <v>59</v>
       </c>
@@ -6453,7 +6599,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="368" ht="15.75" spans="3:9">
+    <row r="368" ht="15.3" spans="3:9">
       <c r="C368" t="s">
         <v>231</v>
       </c>
@@ -6524,11 +6670,11 @@
       <c r="H370" s="16">
         <v>2</v>
       </c>
-      <c r="I370" s="126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="371" ht="15.75" spans="2:9">
+      <c r="I370" s="125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" ht="15.3" spans="2:9">
       <c r="B371" t="s">
         <v>241</v>
       </c>
@@ -6559,6 +6705,7 @@
         <v>243</v>
       </c>
     </row>
+    <row r="381" ht="15.3"/>
     <row r="382" spans="2:4">
       <c r="B382" s="117">
         <v>1</v>
@@ -6574,26 +6721,27 @@
       <c r="B383" s="120">
         <v>1</v>
       </c>
-      <c r="C383" s="121">
+      <c r="C383" s="47">
         <v>5</v>
       </c>
-      <c r="D383" s="122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="384" ht="15.75" spans="2:4">
-      <c r="B384" s="123">
+      <c r="D383" s="121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" ht="15.3" spans="2:4">
+      <c r="B384" s="122">
         <v>4</v>
       </c>
-      <c r="C384" s="124">
-        <v>2</v>
-      </c>
-      <c r="D384" s="125">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="C384" s="123">
+        <v>2</v>
+      </c>
+      <c r="D384" s="124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" ht="15.3"/>
     <row r="387" spans="2:6">
-      <c r="B387" s="127">
+      <c r="B387" s="126">
         <v>7</v>
       </c>
       <c r="C387" s="118">
@@ -6613,24 +6761,24 @@
       <c r="B388" s="120">
         <v>8</v>
       </c>
-      <c r="C388" s="121">
+      <c r="C388" s="47">
         <v>7</v>
       </c>
-      <c r="D388" s="122">
+      <c r="D388" s="121">
         <v>2</v>
       </c>
       <c r="E388" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="389" ht="15.75" spans="2:5">
-      <c r="B389" s="123" t="s">
+    <row r="389" ht="15.3" spans="2:5">
+      <c r="B389" s="122" t="s">
         <v>246</v>
       </c>
-      <c r="C389" s="124" t="s">
+      <c r="C389" s="123" t="s">
         <v>247</v>
       </c>
-      <c r="D389" s="125" t="s">
+      <c r="D389" s="124" t="s">
         <v>248</v>
       </c>
       <c r="E389" t="s">
@@ -6654,6 +6802,165 @@
     <row r="398" spans="1:1">
       <c r="A398" s="1" t="s">
         <v>250</v>
+      </c>
+    </row>
+    <row r="400" spans="1:8">
+      <c r="A400" t="s">
+        <v>232</v>
+      </c>
+      <c r="B400" s="127" t="s">
+        <v>2</v>
+      </c>
+      <c r="C400" s="127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D400" s="127" t="s">
+        <v>12</v>
+      </c>
+      <c r="E400" s="127" t="s">
+        <v>29</v>
+      </c>
+      <c r="F400" s="127" t="s">
+        <v>251</v>
+      </c>
+      <c r="H400" s="128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="401" spans="1:8">
+      <c r="A401" t="s">
+        <v>233</v>
+      </c>
+      <c r="B401" s="129" t="s">
+        <v>252</v>
+      </c>
+      <c r="C401" s="130" t="s">
+        <v>253</v>
+      </c>
+      <c r="D401" s="130" t="s">
+        <v>254</v>
+      </c>
+      <c r="E401" s="130" t="s">
+        <v>255</v>
+      </c>
+      <c r="F401" s="131" t="s">
+        <v>256</v>
+      </c>
+      <c r="H401" s="128">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="402" spans="2:6">
+      <c r="B402" s="132"/>
+      <c r="C402" t="s">
+        <v>257</v>
+      </c>
+      <c r="D402" t="s">
+        <v>258</v>
+      </c>
+      <c r="E402" t="s">
+        <v>259</v>
+      </c>
+      <c r="F402" s="133"/>
+    </row>
+    <row r="403" spans="2:6">
+      <c r="B403" s="132"/>
+      <c r="D403" t="s">
+        <v>260</v>
+      </c>
+      <c r="F403" s="133"/>
+    </row>
+    <row r="404" spans="2:6">
+      <c r="B404" s="134"/>
+      <c r="C404" s="135"/>
+      <c r="D404" s="135" t="s">
+        <v>261</v>
+      </c>
+      <c r="E404" s="135"/>
+      <c r="F404" s="136"/>
+    </row>
+    <row r="408" spans="1:4">
+      <c r="A408" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4">
+      <c r="A409" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="B409" s="127">
+        <v>1</v>
+      </c>
+      <c r="C409" s="127">
+        <v>3</v>
+      </c>
+      <c r="D409" s="137" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4">
+      <c r="A410" s="137" t="s">
+        <v>6</v>
+      </c>
+      <c r="B410" s="127">
+        <v>1</v>
+      </c>
+      <c r="C410" s="127">
+        <v>2</v>
+      </c>
+      <c r="D410" s="137" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4">
+      <c r="A411" s="137" t="s">
+        <v>12</v>
+      </c>
+      <c r="B411" s="127">
+        <v>1</v>
+      </c>
+      <c r="C411" s="127">
+        <v>2</v>
+      </c>
+      <c r="D411" s="137" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4">
+      <c r="A412" s="137" t="s">
+        <v>29</v>
+      </c>
+      <c r="B412" s="127">
+        <v>1</v>
+      </c>
+      <c r="C412" s="127">
+        <v>1</v>
+      </c>
+      <c r="D412" s="137" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4">
+      <c r="A413" s="137" t="s">
+        <v>251</v>
+      </c>
+      <c r="B413" s="127">
+        <v>1</v>
+      </c>
+      <c r="C413" s="127">
+        <v>2</v>
+      </c>
+      <c r="D413" s="137" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -6674,7 +6981,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -6719,7 +7026,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="B2" s="50">
         <v>0</v>
@@ -6784,7 +7091,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -6793,22 +7100,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>2</v>
@@ -6825,7 +7132,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
@@ -6839,7 +7146,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>2</v>
@@ -6850,7 +7157,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -6870,12 +7177,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -6979,7 +7286,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -6999,17 +7306,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
@@ -7021,18 +7328,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>6</v>
@@ -7040,18 +7347,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -7063,7 +7370,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -7071,12 +7378,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -7084,7 +7391,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -7146,7 +7453,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="24" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="C51" s="16">
         <v>1</v>
@@ -7180,7 +7487,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -7192,7 +7499,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -7213,19 +7520,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="10" max="10" width="10.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="10.1441441441441" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="25" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -7318,10 +7625,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -7336,7 +7643,7 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -7356,7 +7663,7 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="K11" s="24">
         <v>3</v>
@@ -7383,13 +7690,13 @@
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="F14" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="M14" s="47">
         <v>2</v>
@@ -7397,7 +7704,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="G15" s="24">
         <v>2</v>
@@ -7415,7 +7722,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="G17" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -7423,7 +7730,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="I18" s="24">
         <v>2</v>
@@ -7434,25 +7741,25 @@
         <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="C20" s="16">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="K20" s="16">
         <v>3</v>
@@ -7461,21 +7768,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="C21" s="16">
         <v>3</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="G21" s="16">
         <v>3</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="K21" s="16">
         <v>2</v>
@@ -7484,21 +7791,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="G22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="K22" s="28">
         <v>2</v>
@@ -7506,28 +7813,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="C24" s="16">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="G24" s="16">
         <v>4</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="K24" s="16">
         <v>4</v>
@@ -7536,21 +7843,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="C25" s="16">
         <v>3</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="G25" s="16">
         <v>3</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="K25" s="16">
         <v>4</v>
@@ -7559,21 +7866,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="C26" s="28">
         <v>3</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="G26" s="28">
         <v>3</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="K26" s="28">
         <v>2</v>
@@ -7594,7 +7901,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -7603,7 +7910,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>31</v>
@@ -7623,7 +7930,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -7668,27 +7975,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -7822,13 +8129,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
     <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="15.047619047619" customWidth="1"/>
+    <col min="6" max="6" width="15.045045045045" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.8095238095238" customWidth="1"/>
-    <col min="9" max="9" width="18.0952380952381" customWidth="1"/>
+    <col min="8" max="8" width="13.8108108108108" customWidth="1"/>
+    <col min="9" max="9" width="18.0990990990991" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -7836,15 +8143,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="2:12">
+    <row r="3" ht="15.3" spans="2:12">
       <c r="B3" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="L3" s="46">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="2:12">
+    <row r="4" ht="15.3" spans="2:12">
       <c r="B4" s="33">
         <v>1</v>
       </c>
@@ -7852,10 +8159,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="2:9">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" ht="15.3" spans="2:9">
       <c r="B5" s="34"/>
       <c r="C5" s="35">
         <v>2</v>
@@ -7864,7 +8171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="2:9">
+    <row r="6" ht="15.3" spans="2:9">
       <c r="B6" s="34"/>
       <c r="C6" s="36"/>
       <c r="D6" s="35">
@@ -7874,7 +8181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="2:9">
+    <row r="7" ht="15.3" spans="2:9">
       <c r="B7" s="34"/>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -7885,7 +8192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="2:9">
+    <row r="8" ht="15.3" spans="2:9">
       <c r="B8" s="37"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7897,19 +8204,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="2:2">
+    <row r="10" customFormat="1" ht="15.3" spans="2:2">
       <c r="B10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" spans="2:9">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" ht="15.3" spans="2:9">
       <c r="B11" s="40"/>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="H11" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="I11" s="45">
         <v>10</v>
@@ -7917,7 +8224,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="I12" s="45">
         <v>11</v>
@@ -7925,7 +8232,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="I13" s="45">
         <v>11</v>
@@ -7933,7 +8240,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="I14" s="45">
         <v>10</v>
@@ -7949,7 +8256,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="I16" s="43">
         <v>12</v>
@@ -7957,7 +8264,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="I17" s="43">
         <v>12</v>
@@ -7971,8 +8278,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.75"/>
-    <row r="22" customFormat="1" ht="15.75" spans="1:5">
+    <row r="21" ht="15.3"/>
+    <row r="22" customFormat="1" ht="15.3" spans="1:5">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -7986,8 +8293,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="15.75"/>
-    <row r="24" customFormat="1" ht="15.75" spans="1:7">
+    <row r="23" ht="15.3"/>
+    <row r="24" customFormat="1" ht="15.3" spans="1:7">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -8010,7 +8317,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="G25" s="43">
         <v>5</v>
@@ -8019,10 +8326,10 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" spans="12:13">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" ht="15.3" spans="12:13">
       <c r="L26">
         <v>1</v>
       </c>
@@ -8030,7 +8337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:13">
+    <row r="27" ht="15.3" spans="1:13">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -8077,7 +8384,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="H29" s="43">
         <v>7</v>
@@ -8097,8 +8404,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" ht="15.75"/>
-    <row r="32" ht="15.75" spans="1:9">
+    <row r="31" ht="15.3"/>
+    <row r="32" ht="15.3" spans="1:9">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -8145,14 +8452,14 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>319</v>
+        <v>337</v>
       </c>
       <c r="I35" s="45">
         <v>8</v>
       </c>
     </row>
-    <row r="37" ht="15.75"/>
-    <row r="38" ht="15.75" spans="1:10">
+    <row r="37" ht="15.3"/>
+    <row r="38" ht="15.3" spans="1:10">
       <c r="A38" t="s">
         <v>216</v>
       </c>
@@ -8164,10 +8471,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="I38" t="s">
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="J38" s="45">
         <v>12</v>
@@ -8175,10 +8482,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="I39" t="s">
-        <v>321</v>
+        <v>339</v>
       </c>
       <c r="J39" s="45">
         <v>12</v>
@@ -8186,10 +8493,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>322</v>
+        <v>340</v>
       </c>
       <c r="I40" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="J40" s="43">
         <v>12</v>
@@ -8197,10 +8504,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="I41" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="J41" s="45">
         <v>10</v>
@@ -8208,10 +8515,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="I42" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="J42" s="45">
         <v>10</v>
@@ -8232,16 +8539,16 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
-    <col min="12" max="12" width="12.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="16.4324324324324" customWidth="1"/>
+    <col min="2" max="2" width="15.2882882882883" customWidth="1"/>
+    <col min="12" max="12" width="12.7117117117117" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" spans="12:12">
@@ -8251,7 +8558,7 @@
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>329</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -8276,7 +8583,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="M15" s="16">
         <v>4</v>
@@ -8294,12 +8601,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>331</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>332</v>
+        <v>350</v>
       </c>
       <c r="M16" s="16">
         <v>12</v>
@@ -8317,12 +8624,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>333</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="M19" s="30">
         <v>15</v>
@@ -8330,10 +8637,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>336</v>
+        <v>354</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -8386,7 +8693,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -8442,7 +8749,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>338</v>
+        <v>356</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -8498,7 +8805,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>339</v>
+        <v>357</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8554,7 +8861,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8610,7 +8917,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -8666,7 +8973,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -8722,17 +9029,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>343</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="128" t="s">
-        <v>344</v>
+      <c r="A38" s="138" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="128" t="s">
-        <v>345</v>
+      <c r="A39" s="138" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -8751,7 +9058,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
@@ -8760,7 +9067,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8795,7 +9102,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>347</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -8827,10 +9134,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>349</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -8870,15 +9177,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>350</v>
+        <v>368</v>
       </c>
       <c r="E12" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>352</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -8888,7 +9195,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>353</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -8906,26 +9213,26 @@
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="9.57142857142857" customWidth="1"/>
+    <col min="1" max="1" width="9.56756756756757" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="22.352380952381" customWidth="1"/>
-    <col min="6" max="6" width="10.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="10.5047619047619" customWidth="1"/>
-    <col min="9" max="9" width="12.5714285714286" customWidth="1"/>
-    <col min="10" max="10" width="11.4952380952381" customWidth="1"/>
+    <col min="3" max="3" width="22.3513513513514" customWidth="1"/>
+    <col min="6" max="6" width="10.8558558558559" customWidth="1"/>
+    <col min="8" max="8" width="10.5045045045045" customWidth="1"/>
+    <col min="9" max="9" width="12.5675675675676" customWidth="1"/>
+    <col min="10" max="10" width="11.4954954954955" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75"/>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" ht="15.3"/>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -8937,7 +9244,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -8946,7 +9253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="2:8">
+    <row r="4" customFormat="1" ht="15.3" spans="2:8">
       <c r="B4" s="5">
         <v>4</v>
       </c>
@@ -8963,7 +9270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="7:8">
+    <row r="5" customFormat="1" ht="15.3" spans="7:8">
       <c r="G5" s="5">
         <v>11</v>
       </c>
@@ -8973,39 +9280,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" ht="15.3"/>
     <row r="9" customFormat="1" spans="1:5">
       <c r="A9" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="E9" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="10" customFormat="1" ht="15.75" spans="2:5">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" ht="15.3" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>362</v>
+        <v>380</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>363</v>
+        <v>381</v>
       </c>
       <c r="E10" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" ht="15.3"/>
     <row r="12" customFormat="1" spans="1:3">
       <c r="A12" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -9014,7 +9321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="2:3">
+    <row r="13" customFormat="1" ht="15.3" spans="2:3">
       <c r="B13" s="5">
         <v>139</v>
       </c>
@@ -9024,41 +9331,41 @@
     </row>
     <row r="16" customFormat="1" spans="1:3">
       <c r="A16" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
       <c r="B16" t="s">
-        <v>366</v>
+        <v>384</v>
       </c>
       <c r="C16" t="s">
-        <v>366</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
       <c r="B17" t="s">
-        <v>368</v>
+        <v>386</v>
       </c>
       <c r="F17" t="s">
-        <v>369</v>
+        <v>387</v>
       </c>
       <c r="I17" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="B18" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="C18" t="s">
-        <v>373</v>
+        <v>391</v>
       </c>
       <c r="F18" t="s">
-        <v>374</v>
+        <v>392</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -9066,21 +9373,21 @@
     </row>
     <row r="19" customFormat="1" spans="6:6">
       <c r="F19" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>394</v>
       </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="D20" t="s">
-        <v>378</v>
+        <v>396</v>
       </c>
       <c r="F20" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:9">
@@ -9088,19 +9395,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>381</v>
+        <v>399</v>
       </c>
       <c r="F22" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="G22" t="s">
-        <v>382</v>
+        <v>400</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -9111,15 +9418,15 @@
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" t="s">
-        <v>383</v>
+        <v>401</v>
       </c>
       <c r="C23" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="3:4">
       <c r="C24" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -9127,7 +9434,7 @@
     </row>
     <row r="27" customFormat="1" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:5">
@@ -9152,34 +9459,34 @@
         <v>174</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75"/>
-    <row r="32" customFormat="1" ht="15.75" spans="3:10">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="31" ht="15.3"/>
+    <row r="32" customFormat="1" ht="15.3" spans="3:10">
       <c r="C32" s="10" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>178</v>
@@ -9188,7 +9495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="3:8">
+    <row r="33" customFormat="1" ht="15.3" spans="3:8">
       <c r="C33">
         <v>0</v>
       </c>
@@ -9207,7 +9514,7 @@
     </row>
     <row r="34" customFormat="1" spans="1:10">
       <c r="A34" s="10" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -9225,10 +9532,10 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>392</v>
+        <v>410</v>
       </c>
       <c r="I34" t="s">
-        <v>393</v>
+        <v>411</v>
       </c>
       <c r="J34" s="24">
         <v>6</v>
@@ -9236,7 +9543,7 @@
     </row>
     <row r="35" customFormat="1" spans="1:10">
       <c r="A35" s="10" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -9252,10 +9559,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>394</v>
+        <v>412</v>
       </c>
       <c r="I35" t="s">
-        <v>395</v>
+        <v>413</v>
       </c>
       <c r="J35" s="24">
         <v>24</v>
@@ -9263,7 +9570,7 @@
     </row>
     <row r="36" customFormat="1" spans="1:10">
       <c r="A36" s="10" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -9277,18 +9584,18 @@
         <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="I36" t="s">
-        <v>397</v>
+        <v>415</v>
       </c>
       <c r="J36" s="24">
         <v>36</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15.75" spans="1:6">
+    <row r="37" customFormat="1" ht="15.3" spans="1:6">
       <c r="A37" s="10" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -9300,35 +9607,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="15.75" spans="8:8">
+    <row r="38" customFormat="1" ht="15.3" spans="8:8">
       <c r="H38" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="39" ht="15.75" spans="2:11">
+    <row r="39" ht="15.3" spans="2:11">
       <c r="B39" s="22" t="s">
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>398</v>
+        <v>416</v>
       </c>
       <c r="D39" t="s">
         <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>399</v>
+        <v>417</v>
       </c>
       <c r="F39" t="s">
-        <v>400</v>
+        <v>418</v>
       </c>
       <c r="H39" t="s">
-        <v>398</v>
+        <v>416</v>
       </c>
       <c r="I39" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="J39" t="s">
-        <v>402</v>
+        <v>420</v>
       </c>
       <c r="K39">
         <v>32</v>
@@ -9336,13 +9643,13 @@
     </row>
     <row r="40" spans="4:11">
       <c r="D40" t="s">
-        <v>403</v>
+        <v>421</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="J40" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="K40" s="24">
         <v>18</v>
@@ -9350,7 +9657,7 @@
     </row>
     <row r="41" customFormat="1" spans="4:4">
       <c r="D41" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
     </row>
     <row r="42" spans="4:11">
@@ -9358,19 +9665,19 @@
         <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="F42" t="s">
-        <v>400</v>
+        <v>418</v>
       </c>
       <c r="H42" t="s">
-        <v>408</v>
+        <v>426</v>
       </c>
       <c r="I42" t="s">
-        <v>409</v>
+        <v>427</v>
       </c>
       <c r="J42" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="K42">
         <v>54</v>
@@ -9378,39 +9685,39 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="J43" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="K43" s="24">
         <v>48</v>
       </c>
     </row>
-    <row r="44" ht="15.75"/>
-    <row r="45" customFormat="1" ht="15.75" spans="7:7">
+    <row r="44" ht="15.3"/>
+    <row r="45" customFormat="1" ht="15.3" spans="7:7">
       <c r="G45" s="11" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="2:10">
       <c r="B46" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="C46" t="s">
-        <v>416</v>
+        <v>434</v>
       </c>
       <c r="G46" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="H46" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="I46" t="s">
-        <v>418</v>
+        <v>436</v>
       </c>
       <c r="J46">
         <v>54</v>
@@ -9418,16 +9725,16 @@
     </row>
     <row r="47" customFormat="1" spans="2:10">
       <c r="B47" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="C47" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="H47" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="I47" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="J47">
         <v>51</v>
@@ -9435,31 +9742,31 @@
     </row>
     <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="23" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
       <c r="C48" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
       <c r="I48" t="s">
-        <v>424</v>
+        <v>442</v>
       </c>
       <c r="J48" s="24">
         <v>30</v>
       </c>
     </row>
-    <row r="50" customFormat="1" ht="15.75" spans="1:6">
+    <row r="50" customFormat="1" ht="15.3" spans="1:6">
       <c r="A50" s="22" t="s">
         <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>425</v>
+        <v>443</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>426</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dp approach for target sum problem
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="462">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -829,6 +829,81 @@
   </si>
   <si>
     <t>u2 = i1+o1</t>
+  </si>
+  <si>
+    <t>Target Sum</t>
+  </si>
+  <si>
+    <t>nums = [1,1,1,1,1], target = 3</t>
+  </si>
+  <si>
+    <t>total=[-sum,+sum]</t>
+  </si>
+  <si>
+    <t>(index,total)</t>
+  </si>
+  <si>
+    <t>(0,0)</t>
+  </si>
+  <si>
+    <t>(0,0+1) = (0,1)</t>
+  </si>
+  <si>
+    <t>(0,0-1) = (0,-1)</t>
+  </si>
+  <si>
+    <t>(1,1+1)= (1,2)</t>
+  </si>
+  <si>
+    <t>(1,1-1)=(1,0)</t>
+  </si>
+  <si>
+    <t>(1,-1+1)=(1,0)</t>
+  </si>
+  <si>
+    <t>(1,-1-1)=(1,-2)</t>
+  </si>
+  <si>
+    <t>(2,0+1)=(2,1)</t>
+  </si>
+  <si>
+    <t>(2,0-1)=(2,-1)</t>
+  </si>
+  <si>
+    <t>(3,1+1)=(3,2)</t>
+  </si>
+  <si>
+    <t>(3,1-1)=(3,0)</t>
+  </si>
+  <si>
+    <r>
+      <t>(4,2+1)=(4,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>(4,2-1)=(4,1)</t>
   </si>
   <si>
     <t>fib(n)</t>
@@ -1364,10 +1439,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="28">
@@ -1433,26 +1508,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1471,15 +1530,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1493,13 +1554,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1508,8 +1562,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1525,7 +1586,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1534,7 +1595,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1556,6 +1624,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1564,14 +1647,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1616,7 +1691,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,13 +1709,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1646,7 +1751,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1664,7 +1781,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1676,7 +1799,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1688,61 +1835,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1754,43 +1865,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2347,17 +2422,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2386,11 +2457,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2410,21 +2511,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2433,27 +2519,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2465,134 +2540,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="44" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2755,6 +2830,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -3169,21 +3256,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z413"/>
+  <dimension ref="A1:Z438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="D413" sqref="D413"/>
+    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
+      <selection activeCell="E434" sqref="E434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.7809523809524" customWidth="1"/>
     <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="12.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="18.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="26.2857142857143" customWidth="1"/>
-    <col min="6" max="7" width="12.3142857142857" customWidth="1"/>
-    <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
+    <col min="6" max="6" width="20.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="17.2857142857143" customWidth="1"/>
+    <col min="8" max="8" width="21.1428571428571" customWidth="1"/>
     <col min="9" max="9" width="16.2857142857143" customWidth="1"/>
     <col min="11" max="11" width="13.7428571428571" customWidth="1"/>
   </cols>
@@ -6959,6 +7047,117 @@
       </c>
       <c r="D413" s="135" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1">
+      <c r="A423" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="424" spans="4:4">
+      <c r="D424" s="136" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6">
+      <c r="A426" t="s">
+        <v>12</v>
+      </c>
+      <c r="B426">
+        <v>0</v>
+      </c>
+      <c r="C426">
+        <v>1</v>
+      </c>
+      <c r="D426">
+        <v>2</v>
+      </c>
+      <c r="E426">
+        <v>3</v>
+      </c>
+      <c r="F426">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6">
+      <c r="A427" t="s">
+        <v>13</v>
+      </c>
+      <c r="B427" s="137">
+        <v>1</v>
+      </c>
+      <c r="C427" s="137">
+        <v>1</v>
+      </c>
+      <c r="D427" s="137">
+        <v>1</v>
+      </c>
+      <c r="E427" s="137">
+        <v>1</v>
+      </c>
+      <c r="F427" s="137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="3:6">
+      <c r="C429" t="s">
+        <v>271</v>
+      </c>
+      <c r="F429" s="138" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="430" spans="6:6">
+      <c r="F430" s="137" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="431" spans="5:7">
+      <c r="E431" s="139" t="s">
+        <v>274</v>
+      </c>
+      <c r="G431" s="140" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="432" spans="2:8">
+      <c r="B432" s="141"/>
+      <c r="C432" s="141"/>
+      <c r="D432" s="137" t="s">
+        <v>276</v>
+      </c>
+      <c r="E432" s="142" t="s">
+        <v>277</v>
+      </c>
+      <c r="G432" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="H432" s="137" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="434" spans="6:8">
+      <c r="F434" s="143" t="s">
+        <v>280</v>
+      </c>
+      <c r="H434" s="137" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="436" spans="5:7">
+      <c r="E436" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G436" s="62" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="438" spans="4:6">
+      <c r="D438" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F438" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -7024,7 +7223,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="B2" s="50">
         <v>0</v>
@@ -7098,22 +7297,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>2</v>
@@ -7130,7 +7329,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
@@ -7144,7 +7343,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>2</v>
@@ -7155,7 +7354,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -7175,12 +7374,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -7284,7 +7483,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -7304,17 +7503,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
@@ -7326,18 +7525,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>6</v>
@@ -7345,18 +7544,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -7368,7 +7567,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -7376,12 +7575,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -7389,7 +7588,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -7451,7 +7650,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="24" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="C51" s="16">
         <v>1</v>
@@ -7485,7 +7684,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -7497,7 +7696,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -7525,12 +7724,12 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="25" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -7623,10 +7822,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -7641,7 +7840,7 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="s">
-        <v>288</v>
+        <v>305</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -7661,7 +7860,7 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="s">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="K11" s="24">
         <v>3</v>
@@ -7688,13 +7887,13 @@
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="F14" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
       <c r="M14" s="47">
         <v>2</v>
@@ -7702,7 +7901,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
       <c r="G15" s="24">
         <v>2</v>
@@ -7720,7 +7919,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="G17" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -7728,7 +7927,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="I18" s="24">
         <v>2</v>
@@ -7739,25 +7938,25 @@
         <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="C20" s="16">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
       <c r="K20" s="16">
         <v>3</v>
@@ -7766,21 +7965,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="C21" s="16">
         <v>3</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="G21" s="16">
         <v>3</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="K21" s="16">
         <v>2</v>
@@ -7789,21 +7988,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="G22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
       <c r="K22" s="28">
         <v>2</v>
@@ -7811,28 +8010,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="C24" s="16">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="G24" s="16">
         <v>4</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>311</v>
+        <v>328</v>
       </c>
       <c r="K24" s="16">
         <v>4</v>
@@ -7841,21 +8040,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
       <c r="C25" s="16">
         <v>3</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="G25" s="16">
         <v>3</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="K25" s="16">
         <v>4</v>
@@ -7864,21 +8063,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="C26" s="28">
         <v>3</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="G26" s="28">
         <v>3</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="K26" s="28">
         <v>2</v>
@@ -7908,7 +8107,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>335</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>31</v>
@@ -7928,7 +8127,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>336</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -7973,27 +8172,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>321</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -8143,7 +8342,7 @@
     </row>
     <row r="3" ht="15.75" spans="2:12">
       <c r="B3" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="L3" s="46">
         <v>5</v>
@@ -8157,7 +8356,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="2:9">
@@ -8204,7 +8403,7 @@
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:2">
       <c r="B10" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="2:9">
@@ -8214,7 +8413,7 @@
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="H11" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="I11" s="45">
         <v>10</v>
@@ -8222,7 +8421,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>329</v>
+        <v>346</v>
       </c>
       <c r="I12" s="45">
         <v>11</v>
@@ -8230,7 +8429,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="I13" s="45">
         <v>11</v>
@@ -8238,7 +8437,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
       <c r="I14" s="45">
         <v>10</v>
@@ -8254,7 +8453,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="I16" s="43">
         <v>12</v>
@@ -8262,7 +8461,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="I17" s="43">
         <v>12</v>
@@ -8315,7 +8514,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>334</v>
+        <v>351</v>
       </c>
       <c r="G25" s="43">
         <v>5</v>
@@ -8324,7 +8523,7 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" ht="15.75" spans="12:13">
@@ -8382,7 +8581,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="H29" s="43">
         <v>7</v>
@@ -8450,7 +8649,7 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>337</v>
+        <v>354</v>
       </c>
       <c r="I35" s="45">
         <v>8</v>
@@ -8469,10 +8668,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
       <c r="I38" t="s">
-        <v>338</v>
+        <v>355</v>
       </c>
       <c r="J38" s="45">
         <v>12</v>
@@ -8480,10 +8679,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="I39" t="s">
-        <v>339</v>
+        <v>356</v>
       </c>
       <c r="J39" s="45">
         <v>12</v>
@@ -8491,10 +8690,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="I40" t="s">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="J40" s="43">
         <v>12</v>
@@ -8502,10 +8701,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="I41" t="s">
-        <v>343</v>
+        <v>360</v>
       </c>
       <c r="J41" s="45">
         <v>10</v>
@@ -8513,10 +8712,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>344</v>
+        <v>361</v>
       </c>
       <c r="I42" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
       <c r="J42" s="45">
         <v>10</v>
@@ -8546,7 +8745,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>346</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="12:12">
@@ -8556,7 +8755,7 @@
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>347</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -8581,7 +8780,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="M15" s="16">
         <v>4</v>
@@ -8599,12 +8798,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>350</v>
+        <v>367</v>
       </c>
       <c r="M16" s="16">
         <v>12</v>
@@ -8622,12 +8821,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>351</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="M19" s="30">
         <v>15</v>
@@ -8635,10 +8834,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -8691,7 +8890,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -8747,7 +8946,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>356</v>
+        <v>373</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -8803,7 +9002,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>357</v>
+        <v>374</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8859,7 +9058,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>358</v>
+        <v>375</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -8915,7 +9114,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>359</v>
+        <v>376</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -8971,7 +9170,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -9027,17 +9226,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>361</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="136" t="s">
-        <v>362</v>
+      <c r="A38" s="144" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="136" t="s">
-        <v>363</v>
+      <c r="A39" s="144" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -9065,7 +9264,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>364</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -9100,7 +9299,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>365</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -9132,10 +9331,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>366</v>
+        <v>383</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -9175,15 +9374,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
       <c r="E12" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -9193,7 +9392,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -9224,13 +9423,13 @@
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" ht="15.75"/>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -9242,7 +9441,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>374</v>
+        <v>391</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -9278,39 +9477,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>375</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" ht="15.75"/>
     <row r="9" customFormat="1" spans="1:5">
       <c r="A9" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>377</v>
+        <v>394</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="E9" t="s">
-        <v>379</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10" customFormat="1" ht="15.75" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>380</v>
+        <v>397</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>381</v>
+        <v>398</v>
       </c>
       <c r="E10" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" ht="15.75"/>
     <row r="12" customFormat="1" spans="1:3">
       <c r="A12" t="s">
-        <v>376</v>
+        <v>393</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -9329,41 +9528,41 @@
     </row>
     <row r="16" customFormat="1" spans="1:3">
       <c r="A16" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="B16" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="C16" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
       <c r="B17" t="s">
-        <v>386</v>
+        <v>403</v>
       </c>
       <c r="F17" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="I17" t="s">
-        <v>388</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="B18" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="C18" t="s">
-        <v>391</v>
+        <v>408</v>
       </c>
       <c r="F18" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -9371,21 +9570,21 @@
     </row>
     <row r="19" customFormat="1" spans="6:6">
       <c r="F19" t="s">
-        <v>393</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
       <c r="A20" t="s">
-        <v>394</v>
+        <v>411</v>
       </c>
       <c r="C20" t="s">
-        <v>395</v>
+        <v>412</v>
       </c>
       <c r="D20" t="s">
-        <v>396</v>
+        <v>413</v>
       </c>
       <c r="F20" t="s">
-        <v>397</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:9">
@@ -9393,19 +9592,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>398</v>
+        <v>415</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="F22" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
       <c r="G22" t="s">
-        <v>400</v>
+        <v>417</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -9416,15 +9615,15 @@
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="C23" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="3:4">
       <c r="C24" t="s">
-        <v>403</v>
+        <v>420</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -9432,7 +9631,7 @@
     </row>
     <row r="27" customFormat="1" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>404</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:5">
@@ -9457,34 +9656,34 @@
         <v>174</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>407</v>
+        <v>424</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>408</v>
+        <v>425</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
     </row>
     <row r="31" ht="15.75"/>
     <row r="32" customFormat="1" ht="15.75" spans="3:10">
       <c r="C32" s="10" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>407</v>
+        <v>424</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>408</v>
+        <v>425</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>178</v>
@@ -9512,7 +9711,7 @@
     </row>
     <row r="34" customFormat="1" spans="1:10">
       <c r="A34" s="10" t="s">
-        <v>405</v>
+        <v>422</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -9530,10 +9729,10 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="I34" t="s">
-        <v>411</v>
+        <v>428</v>
       </c>
       <c r="J34" s="24">
         <v>6</v>
@@ -9541,7 +9740,7 @@
     </row>
     <row r="35" customFormat="1" spans="1:10">
       <c r="A35" s="10" t="s">
-        <v>406</v>
+        <v>423</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -9557,10 +9756,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>412</v>
+        <v>429</v>
       </c>
       <c r="I35" t="s">
-        <v>413</v>
+        <v>430</v>
       </c>
       <c r="J35" s="24">
         <v>24</v>
@@ -9568,7 +9767,7 @@
     </row>
     <row r="36" customFormat="1" spans="1:10">
       <c r="A36" s="10" t="s">
-        <v>407</v>
+        <v>424</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -9582,10 +9781,10 @@
         <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="I36" t="s">
-        <v>415</v>
+        <v>432</v>
       </c>
       <c r="J36" s="24">
         <v>36</v>
@@ -9593,7 +9792,7 @@
     </row>
     <row r="37" customFormat="1" ht="15.75" spans="1:6">
       <c r="A37" s="10" t="s">
-        <v>408</v>
+        <v>425</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -9615,25 +9814,25 @@
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="D39" t="s">
         <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="F39" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="H39" t="s">
-        <v>416</v>
+        <v>433</v>
       </c>
       <c r="I39" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="J39" t="s">
-        <v>420</v>
+        <v>437</v>
       </c>
       <c r="K39">
         <v>32</v>
@@ -9641,13 +9840,13 @@
     </row>
     <row r="40" spans="4:11">
       <c r="D40" t="s">
-        <v>421</v>
+        <v>438</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>422</v>
+        <v>439</v>
       </c>
       <c r="J40" t="s">
-        <v>423</v>
+        <v>440</v>
       </c>
       <c r="K40" s="24">
         <v>18</v>
@@ -9655,7 +9854,7 @@
     </row>
     <row r="41" customFormat="1" spans="4:4">
       <c r="D41" t="s">
-        <v>424</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="4:11">
@@ -9663,19 +9862,19 @@
         <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>425</v>
+        <v>442</v>
       </c>
       <c r="F42" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="H42" t="s">
-        <v>426</v>
+        <v>443</v>
       </c>
       <c r="I42" t="s">
-        <v>427</v>
+        <v>444</v>
       </c>
       <c r="J42" t="s">
-        <v>428</v>
+        <v>445</v>
       </c>
       <c r="K42">
         <v>54</v>
@@ -9683,13 +9882,13 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" t="s">
-        <v>429</v>
+        <v>446</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>430</v>
+        <v>447</v>
       </c>
       <c r="J43" t="s">
-        <v>431</v>
+        <v>448</v>
       </c>
       <c r="K43" s="24">
         <v>48</v>
@@ -9698,24 +9897,24 @@
     <row r="44" ht="15.75"/>
     <row r="45" customFormat="1" ht="15.75" spans="7:7">
       <c r="G45" s="11" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="2:10">
       <c r="B46" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="C46" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
       <c r="G46" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
       <c r="H46" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="I46" t="s">
-        <v>436</v>
+        <v>453</v>
       </c>
       <c r="J46">
         <v>54</v>
@@ -9723,16 +9922,16 @@
     </row>
     <row r="47" customFormat="1" spans="2:10">
       <c r="B47" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="C47" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="H47" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="I47" t="s">
-        <v>439</v>
+        <v>456</v>
       </c>
       <c r="J47">
         <v>51</v>
@@ -9740,17 +9939,17 @@
     </row>
     <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="23" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
       <c r="C48" t="s">
-        <v>441</v>
+        <v>458</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
       <c r="I48" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
       <c r="J48" s="24">
         <v>30</v>
@@ -9761,10 +9960,10 @@
         <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>443</v>
+        <v>460</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>444</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solved jump game 2
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -877,6 +877,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>(4,2+1)=(4,</t>
     </r>
     <r>
@@ -1439,8 +1447,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
@@ -1522,6 +1530,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1530,17 +1546,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1562,18 +1577,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1595,21 +1610,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1617,21 +1618,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1647,6 +1633,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1691,13 +1699,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1709,31 +1717,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1751,7 +1759,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1763,7 +1813,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1775,97 +1861,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2424,11 +2432,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2472,30 +2493,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2516,6 +2513,17 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2540,134 +2548,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="48" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2830,18 +2838,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -3259,7 +3263,7 @@
   <dimension ref="A1:Z438"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="E434" sqref="E434"/>
+      <selection activeCell="D424" sqref="D424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7055,7 +7059,7 @@
       </c>
     </row>
     <row r="424" spans="4:4">
-      <c r="D424" s="136" t="s">
+      <c r="D424" s="25" t="s">
         <v>270</v>
       </c>
     </row>
@@ -7083,19 +7087,19 @@
       <c r="A427" t="s">
         <v>13</v>
       </c>
-      <c r="B427" s="137">
-        <v>1</v>
-      </c>
-      <c r="C427" s="137">
-        <v>1</v>
-      </c>
-      <c r="D427" s="137">
-        <v>1</v>
-      </c>
-      <c r="E427" s="137">
-        <v>1</v>
-      </c>
-      <c r="F427" s="137">
+      <c r="B427" s="16">
+        <v>1</v>
+      </c>
+      <c r="C427" s="16">
+        <v>1</v>
+      </c>
+      <c r="D427" s="16">
+        <v>1</v>
+      </c>
+      <c r="E427" s="16">
+        <v>1</v>
+      </c>
+      <c r="F427" s="16">
         <v>1</v>
       </c>
     </row>
@@ -7103,44 +7107,44 @@
       <c r="C429" t="s">
         <v>271</v>
       </c>
-      <c r="F429" s="138" t="s">
+      <c r="F429" s="136" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="430" spans="6:6">
-      <c r="F430" s="137" t="s">
+      <c r="F430" s="16" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="431" spans="5:7">
-      <c r="E431" s="139" t="s">
+      <c r="E431" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="G431" s="140" t="s">
+      <c r="G431" s="137" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="432" spans="2:8">
-      <c r="B432" s="141"/>
-      <c r="C432" s="141"/>
-      <c r="D432" s="137" t="s">
+      <c r="B432" s="138"/>
+      <c r="C432" s="138"/>
+      <c r="D432" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="E432" s="142" t="s">
+      <c r="E432" s="139" t="s">
         <v>277</v>
       </c>
-      <c r="G432" s="142" t="s">
+      <c r="G432" s="139" t="s">
         <v>278</v>
       </c>
-      <c r="H432" s="137" t="s">
+      <c r="H432" s="16" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="434" spans="6:8">
-      <c r="F434" s="143" t="s">
+      <c r="F434" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="H434" s="137" t="s">
+      <c r="H434" s="16" t="s">
         <v>281</v>
       </c>
     </row>
@@ -9230,12 +9234,12 @@
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="140" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="144" t="s">
+      <c r="A39" s="140" t="s">
         <v>380</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dp approach done for jump game problems
</commit_message>
<xml_diff>
--- a/DP.xlsx
+++ b/DP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView windowWidth="27428" windowHeight="11734"/>
   </bookViews>
   <sheets>
     <sheet name="DP" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="483">
   <si>
     <t>LongestCommonSubsequence</t>
   </si>
@@ -914,6 +914,91 @@
     <t>(4,2-1)=(4,1)</t>
   </si>
   <si>
+    <t>Jump Game</t>
+  </si>
+  <si>
+    <t>target=nums.length - 1</t>
+  </si>
+  <si>
+    <t>if ((i + nums[i]) &gt;= target) {</t>
+  </si>
+  <si>
+    <t>i-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    target = i;</t>
+  </si>
+  <si>
+    <t>i-2</t>
+  </si>
+  <si>
+    <t>i-3</t>
+  </si>
+  <si>
+    <t>i==0</t>
+  </si>
+  <si>
+    <t>return target == 0;</t>
+  </si>
+  <si>
+    <t>Jump Game II</t>
+  </si>
+  <si>
+    <t>level=0</t>
+  </si>
+  <si>
+    <t>l=0</t>
+  </si>
+  <si>
+    <t>r=0</t>
+  </si>
+  <si>
+    <t>level=1</t>
+  </si>
+  <si>
+    <t>l=1</t>
+  </si>
+  <si>
+    <t>(3,1)</t>
+  </si>
+  <si>
+    <t>r=2</t>
+  </si>
+  <si>
+    <t>level=2</t>
+  </si>
+  <si>
+    <t>l=3</t>
+  </si>
+  <si>
+    <r>
+      <t>(1,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>r=4</t>
+  </si>
+  <si>
     <t>fib(n)</t>
   </si>
   <si>
@@ -1447,10 +1532,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="28">
@@ -1516,8 +1601,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1530,24 +1623,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1577,18 +1654,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1608,9 +1693,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1631,6 +1723,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1638,23 +1738,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1699,13 +1784,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1717,31 +1814,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1759,19 +1856,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1795,79 +1952,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2426,15 +2511,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2493,6 +2569,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2516,21 +2612,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2548,134 +2633,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="48" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2846,6 +2931,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -2938,8 +3031,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="929005" y="770255"/>
-          <a:ext cx="4342130" cy="2425700"/>
+          <a:off x="963930" y="747395"/>
+          <a:ext cx="4586605" cy="2357120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2985,8 +3078,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1584325" y="723265"/>
-          <a:ext cx="4304030" cy="3704590"/>
+          <a:off x="1647190" y="706120"/>
+          <a:ext cx="4572000" cy="3590290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3260,24 +3353,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z438"/>
+  <dimension ref="A1:Z473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="D424" sqref="D424"/>
+    <sheetView tabSelected="1" topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="E471" sqref="E471"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="24.7809523809524" customWidth="1"/>
-    <col min="2" max="2" width="19.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.2857142857143" customWidth="1"/>
-    <col min="4" max="4" width="27.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="26.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="20.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="17.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="21.1428571428571" customWidth="1"/>
-    <col min="9" max="9" width="16.2857142857143" customWidth="1"/>
-    <col min="11" max="11" width="13.7428571428571" customWidth="1"/>
+    <col min="1" max="1" width="24.7837837837838" customWidth="1"/>
+    <col min="2" max="2" width="19.1441441441441" customWidth="1"/>
+    <col min="3" max="3" width="18.2882882882883" customWidth="1"/>
+    <col min="4" max="4" width="27.5675675675676" customWidth="1"/>
+    <col min="5" max="5" width="26.2882882882883" customWidth="1"/>
+    <col min="6" max="6" width="20.7117117117117" customWidth="1"/>
+    <col min="7" max="7" width="17.2882882882883" customWidth="1"/>
+    <col min="8" max="8" width="21.1441441441441" customWidth="1"/>
+    <col min="9" max="9" width="16.2882882882883" customWidth="1"/>
+    <col min="11" max="11" width="13.7387387387387" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -3858,26 +3951,26 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" ht="15.75"/>
-    <row r="67" ht="15.75" spans="7:7">
+    <row r="66" ht="15.3"/>
+    <row r="67" ht="15.3" spans="7:7">
       <c r="G67" s="53"/>
     </row>
-    <row r="68" ht="15.75" spans="6:7">
+    <row r="68" ht="15.3" spans="6:7">
       <c r="F68" s="54"/>
       <c r="G68" s="55"/>
     </row>
-    <row r="69" ht="15.75" spans="5:7">
+    <row r="69" ht="15.3" spans="5:7">
       <c r="E69" s="54"/>
       <c r="F69" s="56"/>
       <c r="G69" s="55"/>
     </row>
-    <row r="70" ht="15.75" spans="4:7">
+    <row r="70" ht="15.3" spans="4:7">
       <c r="D70" s="54"/>
       <c r="E70" s="56"/>
       <c r="F70" s="56"/>
       <c r="G70" s="55"/>
     </row>
-    <row r="71" ht="15.75" spans="2:7">
+    <row r="71" ht="15.3" spans="2:7">
       <c r="B71" s="20"/>
       <c r="C71" s="37"/>
       <c r="D71" s="57"/>
@@ -3950,26 +4043,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" ht="15.75"/>
-    <row r="80" ht="15.75" spans="7:7">
+    <row r="79" ht="15.3"/>
+    <row r="80" ht="15.3" spans="7:7">
       <c r="G80" s="53"/>
     </row>
-    <row r="81" ht="15.75" spans="6:7">
+    <row r="81" ht="15.3" spans="6:7">
       <c r="F81" s="54"/>
       <c r="G81" s="55"/>
     </row>
-    <row r="82" ht="15.75" spans="5:7">
+    <row r="82" ht="15.3" spans="5:7">
       <c r="E82" s="54"/>
       <c r="F82" s="56"/>
       <c r="G82" s="55"/>
     </row>
-    <row r="83" ht="15.75" spans="4:7">
+    <row r="83" ht="15.3" spans="4:7">
       <c r="D83" s="54"/>
       <c r="E83" s="56"/>
       <c r="F83" s="56"/>
       <c r="G83" s="55"/>
     </row>
-    <row r="84" ht="15.75" spans="2:7">
+    <row r="84" ht="15.3" spans="2:7">
       <c r="B84" s="20"/>
       <c r="C84" s="37"/>
       <c r="D84" s="57"/>
@@ -5548,10 +5641,10 @@
         <v>158</v>
       </c>
     </row>
-    <row r="250" ht="15.75" spans="1:1">
+    <row r="250" ht="15.3" spans="1:1">
       <c r="A250" s="1"/>
     </row>
-    <row r="251" ht="15.75" spans="1:10">
+    <row r="251" ht="15.3" spans="1:10">
       <c r="A251" s="66" t="s">
         <v>159</v>
       </c>
@@ -5568,7 +5661,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="252" ht="15.75" spans="1:7">
+    <row r="252" ht="15.3" spans="1:7">
       <c r="A252" s="1">
         <v>0</v>
       </c>
@@ -5588,7 +5681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" ht="15.75" spans="1:12">
+    <row r="253" ht="15.3" spans="1:12">
       <c r="A253" s="11">
         <v>1</v>
       </c>
@@ -5646,7 +5739,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="255" ht="15.75" spans="1:12">
+    <row r="255" ht="15.3" spans="1:12">
       <c r="A255" s="1">
         <v>3</v>
       </c>
@@ -5759,7 +5852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" ht="15.75" spans="1:10">
+    <row r="259" ht="15.3" spans="1:10">
       <c r="A259" s="86">
         <v>7</v>
       </c>
@@ -5934,7 +6027,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="267" ht="15.75" spans="1:8">
+    <row r="267" ht="15.3" spans="1:8">
       <c r="A267" s="94">
         <v>15</v>
       </c>
@@ -6009,7 +6102,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="279" ht="15.75" spans="3:7">
+    <row r="279" ht="15.3" spans="3:7">
       <c r="C279">
         <v>0</v>
       </c>
@@ -6073,7 +6166,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="282" ht="15.75" spans="1:5">
+    <row r="282" ht="15.3" spans="1:5">
       <c r="A282" s="10" t="s">
         <v>177</v>
       </c>
@@ -6119,7 +6212,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="287" ht="15.75" spans="8:8">
+    <row r="287" ht="15.3" spans="8:8">
       <c r="H287" s="1" t="s">
         <v>190</v>
       </c>
@@ -6135,7 +6228,7 @@
       <c r="O288" s="36"/>
       <c r="P288" s="35"/>
     </row>
-    <row r="289" ht="15.75" spans="10:16">
+    <row r="289" ht="15.3" spans="10:16">
       <c r="J289" s="94" t="s">
         <v>192</v>
       </c>
@@ -6250,8 +6343,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="308" ht="15.75"/>
-    <row r="309" customFormat="1" ht="15.75" spans="1:10">
+    <row r="308" ht="15.3"/>
+    <row r="309" customFormat="1" ht="15.3" spans="1:10">
       <c r="A309" t="s">
         <v>60</v>
       </c>
@@ -6268,7 +6361,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="310" customFormat="1" ht="15.75" spans="1:10">
+    <row r="310" customFormat="1" ht="15.3" spans="1:10">
       <c r="A310" t="s">
         <v>64</v>
       </c>
@@ -6288,7 +6381,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="311" ht="15.75" spans="1:11">
+    <row r="311" ht="15.3" spans="1:11">
       <c r="A311" t="s">
         <v>70</v>
       </c>
@@ -6314,7 +6407,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="312" ht="15.75" spans="1:11">
+    <row r="312" ht="15.3" spans="1:11">
       <c r="A312" t="s">
         <v>78</v>
       </c>
@@ -6340,7 +6433,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="313" customFormat="1" ht="15.75" spans="1:8">
+    <row r="313" customFormat="1" ht="15.3" spans="1:8">
       <c r="A313" t="s">
         <v>216</v>
       </c>
@@ -6370,7 +6463,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="321" ht="15.75" spans="1:4">
+    <row r="321" ht="15.3" spans="1:4">
       <c r="A321" t="s">
         <v>12</v>
       </c>
@@ -6384,7 +6477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" ht="15.75" spans="1:5">
+    <row r="322" ht="15.3" spans="1:5">
       <c r="A322" t="s">
         <v>33</v>
       </c>
@@ -6495,7 +6588,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="341" ht="15.75" spans="1:6">
+    <row r="341" ht="15.3" spans="1:6">
       <c r="A341" t="s">
         <v>12</v>
       </c>
@@ -6515,7 +6608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" ht="15.75" spans="1:6">
+    <row r="342" ht="15.3" spans="1:6">
       <c r="A342" t="s">
         <v>33</v>
       </c>
@@ -6614,8 +6707,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" ht="15.75"/>
-    <row r="354" ht="15.75" spans="1:8">
+    <row r="353" ht="15.3"/>
+    <row r="354" ht="15.3" spans="1:8">
       <c r="A354" t="s">
         <v>60</v>
       </c>
@@ -6646,8 +6739,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" ht="15.75"/>
-    <row r="357" ht="15.75" spans="1:9">
+    <row r="356" ht="15.3"/>
+    <row r="357" ht="15.3" spans="1:9">
       <c r="A357" t="s">
         <v>59</v>
       </c>
@@ -6689,7 +6782,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="368" ht="15.75" spans="3:9">
+    <row r="368" ht="15.3" spans="3:9">
       <c r="C368" t="s">
         <v>231</v>
       </c>
@@ -6764,7 +6857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" ht="15.75" spans="2:9">
+    <row r="371" ht="15.3" spans="2:9">
       <c r="B371" t="s">
         <v>241</v>
       </c>
@@ -6795,7 +6888,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="381" ht="15.75"/>
+    <row r="381" ht="15.3"/>
     <row r="382" spans="2:4">
       <c r="B382" s="117">
         <v>1</v>
@@ -6818,7 +6911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" ht="15.75" spans="2:4">
+    <row r="384" ht="15.3" spans="2:4">
       <c r="B384" s="122">
         <v>4</v>
       </c>
@@ -6829,7 +6922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" ht="15.75"/>
+    <row r="386" ht="15.3"/>
     <row r="387" spans="2:6">
       <c r="B387" s="126">
         <v>7</v>
@@ -6861,7 +6954,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="389" ht="15.75" spans="2:5">
+    <row r="389" ht="15.3" spans="2:5">
       <c r="B389" s="122" t="s">
         <v>246</v>
       </c>
@@ -7162,6 +7255,205 @@
       </c>
       <c r="F438" t="s">
         <v>285</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1">
+      <c r="A445" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="447" ht="15.3" spans="1:6">
+      <c r="A447" t="s">
+        <v>12</v>
+      </c>
+      <c r="B447">
+        <v>0</v>
+      </c>
+      <c r="C447">
+        <v>1</v>
+      </c>
+      <c r="D447">
+        <v>2</v>
+      </c>
+      <c r="E447">
+        <v>3</v>
+      </c>
+      <c r="F447">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="448" ht="15.3" spans="1:6">
+      <c r="A448" t="s">
+        <v>13</v>
+      </c>
+      <c r="B448" s="140">
+        <v>2</v>
+      </c>
+      <c r="C448" s="141">
+        <v>3</v>
+      </c>
+      <c r="D448" s="141">
+        <v>1</v>
+      </c>
+      <c r="E448" s="141">
+        <v>1</v>
+      </c>
+      <c r="F448" s="142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6">
+      <c r="A450" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B450" t="s">
+        <v>12</v>
+      </c>
+      <c r="C450" s="143">
+        <v>4</v>
+      </c>
+      <c r="F450" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="451" spans="2:6">
+      <c r="B451" t="s">
+        <v>289</v>
+      </c>
+      <c r="C451" s="143">
+        <v>3</v>
+      </c>
+      <c r="F451" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="452" spans="2:6">
+      <c r="B452" t="s">
+        <v>291</v>
+      </c>
+      <c r="C452" s="143">
+        <v>2</v>
+      </c>
+      <c r="F452" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="453" spans="2:3">
+      <c r="B453" t="s">
+        <v>292</v>
+      </c>
+      <c r="C453" s="143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="2:6">
+      <c r="B454" t="s">
+        <v>293</v>
+      </c>
+      <c r="C454" s="143">
+        <v>0</v>
+      </c>
+      <c r="E454" s="144" t="b">
+        <v>1</v>
+      </c>
+      <c r="F454" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1">
+      <c r="A461" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="463" ht="15.3" spans="1:6">
+      <c r="A463" t="s">
+        <v>12</v>
+      </c>
+      <c r="B463">
+        <v>0</v>
+      </c>
+      <c r="C463">
+        <v>1</v>
+      </c>
+      <c r="D463">
+        <v>2</v>
+      </c>
+      <c r="E463">
+        <v>3</v>
+      </c>
+      <c r="F463">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="464" ht="15.3" spans="1:6">
+      <c r="A464" t="s">
+        <v>13</v>
+      </c>
+      <c r="B464" s="140">
+        <v>2</v>
+      </c>
+      <c r="C464" s="141">
+        <v>3</v>
+      </c>
+      <c r="D464" s="141">
+        <v>1</v>
+      </c>
+      <c r="E464" s="141">
+        <v>1</v>
+      </c>
+      <c r="F464" s="142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3">
+      <c r="A466" t="s">
+        <v>296</v>
+      </c>
+      <c r="B466" t="s">
+        <v>297</v>
+      </c>
+      <c r="C466">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="467" spans="2:2">
+      <c r="B467" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3">
+      <c r="A469" t="s">
+        <v>299</v>
+      </c>
+      <c r="B469" t="s">
+        <v>300</v>
+      </c>
+      <c r="C469" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="470" spans="2:2">
+      <c r="B470" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4">
+      <c r="A472" s="145" t="s">
+        <v>303</v>
+      </c>
+      <c r="B472" t="s">
+        <v>304</v>
+      </c>
+      <c r="C472" s="62" t="s">
+        <v>305</v>
+      </c>
+      <c r="D472" s="146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="473" spans="2:2">
+      <c r="B473" s="147" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -7182,7 +7474,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -7227,7 +7519,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="B2" s="50">
         <v>0</v>
@@ -7292,7 +7584,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -7301,22 +7593,22 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>289</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>2</v>
@@ -7333,7 +7625,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>4</v>
@@ -7347,7 +7639,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>2</v>
@@ -7358,7 +7650,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -7378,12 +7670,12 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>294</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -7487,7 +7779,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -7507,17 +7799,17 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>296</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>297</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>51</v>
@@ -7529,18 +7821,18 @@
         <v>6</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>6</v>
@@ -7548,18 +7840,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="B40" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="B41" t="s">
         <v>51</v>
@@ -7571,7 +7863,7 @@
         <v>6</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="F41" t="s">
         <v>6</v>
@@ -7579,12 +7871,12 @@
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>299</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>300</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47" spans="3:6">
@@ -7592,7 +7884,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="E47" t="s">
         <v>6</v>
@@ -7654,7 +7946,7 @@
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="24" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="C51" s="16">
         <v>1</v>
@@ -7688,7 +7980,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>293</v>
+        <v>314</v>
       </c>
       <c r="B55" t="s">
         <v>51</v>
@@ -7700,7 +7992,7 @@
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>298</v>
+        <v>319</v>
       </c>
       <c r="F55" t="s">
         <v>6</v>
@@ -7721,19 +8013,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="10" max="10" width="10.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="10.1441441441441" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:1">
       <c r="A3" s="25" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -7826,10 +8118,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -7844,7 +8136,7 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="s">
-        <v>305</v>
+        <v>326</v>
       </c>
       <c r="K10">
         <v>4</v>
@@ -7864,7 +8156,7 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="K11" s="24">
         <v>3</v>
@@ -7891,13 +8183,13 @@
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="F14" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="M14" s="47">
         <v>2</v>
@@ -7905,7 +8197,7 @@
     </row>
     <row r="15" spans="6:13">
       <c r="F15" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="G15" s="24">
         <v>2</v>
@@ -7923,7 +8215,7 @@
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="G17" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="I17">
         <v>3</v>
@@ -7931,7 +8223,7 @@
     </row>
     <row r="18" customFormat="1" spans="7:9">
       <c r="G18" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="I18" s="24">
         <v>2</v>
@@ -7942,25 +8234,25 @@
         <v>216</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="C20" s="16">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
       <c r="G20" s="16">
         <v>2</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>315</v>
+        <v>336</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>316</v>
+        <v>337</v>
       </c>
       <c r="K20" s="16">
         <v>3</v>
@@ -7969,21 +8261,21 @@
     <row r="21" spans="1:11">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
-        <v>317</v>
+        <v>338</v>
       </c>
       <c r="C21" s="16">
         <v>3</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="G21" s="16">
         <v>3</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="K21" s="16">
         <v>2</v>
@@ -7992,21 +8284,21 @@
     <row r="22" spans="1:11">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="C22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="G22" s="28">
         <v>2</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="K22" s="28">
         <v>2</v>
@@ -8014,28 +8306,28 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="16" t="s">
-        <v>323</v>
+        <v>344</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c r="C24" s="16">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>326</v>
+        <v>347</v>
       </c>
       <c r="G24" s="16">
         <v>4</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>328</v>
+        <v>349</v>
       </c>
       <c r="K24" s="16">
         <v>4</v>
@@ -8044,21 +8336,21 @@
     <row r="25" spans="1:11">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="C25" s="16">
         <v>3</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="G25" s="16">
         <v>3</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="s">
-        <v>331</v>
+        <v>352</v>
       </c>
       <c r="K25" s="16">
         <v>4</v>
@@ -8067,21 +8359,21 @@
     <row r="26" spans="1:11">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="C26" s="28">
         <v>3</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16" t="s">
-        <v>333</v>
+        <v>354</v>
       </c>
       <c r="G26" s="28">
         <v>3</v>
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="s">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c r="K26" s="28">
         <v>2</v>
@@ -8102,7 +8394,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -8111,7 +8403,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>31</v>
@@ -8131,7 +8423,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>357</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>28</v>
@@ -8176,27 +8468,27 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>337</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>339</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>340</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>341</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="3:6">
@@ -8330,13 +8622,13 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
     <col min="4" max="4" width="14.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="15.047619047619" customWidth="1"/>
+    <col min="6" max="6" width="15.045045045045" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.8095238095238" customWidth="1"/>
-    <col min="9" max="9" width="18.0952380952381" customWidth="1"/>
+    <col min="8" max="8" width="13.8108108108108" customWidth="1"/>
+    <col min="9" max="9" width="18.0990990990991" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
@@ -8344,15 +8636,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="2:12">
+    <row r="3" ht="15.3" spans="2:12">
       <c r="B3" t="s">
-        <v>342</v>
+        <v>363</v>
       </c>
       <c r="L3" s="46">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="2:12">
+    <row r="4" ht="15.3" spans="2:12">
       <c r="B4" s="33">
         <v>1</v>
       </c>
@@ -8360,10 +8652,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="2:9">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" ht="15.3" spans="2:9">
       <c r="B5" s="34"/>
       <c r="C5" s="35">
         <v>2</v>
@@ -8372,7 +8664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="2:9">
+    <row r="6" ht="15.3" spans="2:9">
       <c r="B6" s="34"/>
       <c r="C6" s="36"/>
       <c r="D6" s="35">
@@ -8382,7 +8674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="2:9">
+    <row r="7" ht="15.3" spans="2:9">
       <c r="B7" s="34"/>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -8393,7 +8685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="2:9">
+    <row r="8" ht="15.3" spans="2:9">
       <c r="B8" s="37"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8405,19 +8697,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="1" ht="15.75" spans="2:2">
+    <row r="10" customFormat="1" ht="15.3" spans="2:2">
       <c r="B10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" spans="2:9">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="11" ht="15.3" spans="2:9">
       <c r="B11" s="40"/>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="H11" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="I11" s="45">
         <v>10</v>
@@ -8425,7 +8717,7 @@
     </row>
     <row r="12" spans="8:9">
       <c r="H12" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="I12" s="45">
         <v>11</v>
@@ -8433,7 +8725,7 @@
     </row>
     <row r="13" spans="8:9">
       <c r="H13" t="s">
-        <v>347</v>
+        <v>368</v>
       </c>
       <c r="I13" s="45">
         <v>11</v>
@@ -8441,7 +8733,7 @@
     </row>
     <row r="14" spans="8:9">
       <c r="H14" t="s">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="I14" s="45">
         <v>10</v>
@@ -8457,7 +8749,7 @@
     </row>
     <row r="16" spans="8:9">
       <c r="H16" t="s">
-        <v>349</v>
+        <v>370</v>
       </c>
       <c r="I16" s="43">
         <v>12</v>
@@ -8465,7 +8757,7 @@
     </row>
     <row r="17" spans="8:9">
       <c r="H17" t="s">
-        <v>350</v>
+        <v>371</v>
       </c>
       <c r="I17" s="43">
         <v>12</v>
@@ -8479,8 +8771,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="15.75"/>
-    <row r="22" customFormat="1" ht="15.75" spans="1:5">
+    <row r="21" ht="15.3"/>
+    <row r="22" customFormat="1" ht="15.3" spans="1:5">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -8494,8 +8786,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" ht="15.75"/>
-    <row r="24" customFormat="1" ht="15.75" spans="1:7">
+    <row r="23" ht="15.3"/>
+    <row r="24" customFormat="1" ht="15.3" spans="1:7">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -8518,7 +8810,7 @@
         <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>351</v>
+        <v>372</v>
       </c>
       <c r="G25" s="43">
         <v>5</v>
@@ -8527,10 +8819,10 @@
         <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" spans="12:13">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" ht="15.3" spans="12:13">
       <c r="L26">
         <v>1</v>
       </c>
@@ -8538,7 +8830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:13">
+    <row r="27" ht="15.3" spans="1:13">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -8585,7 +8877,7 @@
         <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
       <c r="H29" s="43">
         <v>7</v>
@@ -8605,8 +8897,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" ht="15.75"/>
-    <row r="32" ht="15.75" spans="1:9">
+    <row r="31" ht="15.3"/>
+    <row r="32" ht="15.3" spans="1:9">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -8653,14 +8945,14 @@
         <v>86</v>
       </c>
       <c r="H35" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
       <c r="I35" s="45">
         <v>8</v>
       </c>
     </row>
-    <row r="37" ht="15.75"/>
-    <row r="38" ht="15.75" spans="1:10">
+    <row r="37" ht="15.3"/>
+    <row r="38" ht="15.3" spans="1:10">
       <c r="A38" t="s">
         <v>216</v>
       </c>
@@ -8672,10 +8964,10 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="I38" t="s">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="J38" s="45">
         <v>12</v>
@@ -8683,10 +8975,10 @@
     </row>
     <row r="39" spans="8:10">
       <c r="H39" t="s">
-        <v>349</v>
+        <v>370</v>
       </c>
       <c r="I39" t="s">
-        <v>356</v>
+        <v>377</v>
       </c>
       <c r="J39" s="45">
         <v>12</v>
@@ -8694,10 +8986,10 @@
     </row>
     <row r="40" spans="8:10">
       <c r="H40" t="s">
-        <v>357</v>
+        <v>378</v>
       </c>
       <c r="I40" t="s">
-        <v>358</v>
+        <v>379</v>
       </c>
       <c r="J40" s="43">
         <v>12</v>
@@ -8705,10 +8997,10 @@
     </row>
     <row r="41" spans="8:10">
       <c r="H41" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="I41" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="J41" s="45">
         <v>10</v>
@@ -8716,10 +9008,10 @@
     </row>
     <row r="42" spans="8:10">
       <c r="H42" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="I42" t="s">
-        <v>362</v>
+        <v>383</v>
       </c>
       <c r="J42" s="45">
         <v>10</v>
@@ -8740,16 +9032,16 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="15.2857142857143" customWidth="1"/>
-    <col min="12" max="12" width="12.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="16.4324324324324" customWidth="1"/>
+    <col min="2" max="2" width="15.2882882882883" customWidth="1"/>
+    <col min="12" max="12" width="12.7117117117117" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>363</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="12:12">
@@ -8759,7 +9051,7 @@
     </row>
     <row r="12" spans="12:12">
       <c r="L12" t="s">
-        <v>364</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="12:17">
@@ -8784,7 +9076,7 @@
     </row>
     <row r="15" spans="12:18">
       <c r="L15" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
       <c r="M15" s="16">
         <v>4</v>
@@ -8802,12 +9094,12 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>366</v>
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="12:18">
       <c r="L16" t="s">
-        <v>367</v>
+        <v>388</v>
       </c>
       <c r="M16" s="16">
         <v>12</v>
@@ -8825,12 +9117,12 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>368</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="12:13">
       <c r="L19" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
       <c r="M19" s="30">
         <v>15</v>
@@ -8838,10 +9130,10 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>370</v>
+        <v>391</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>371</v>
+        <v>392</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -8894,7 +9186,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>372</v>
+        <v>393</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -8950,7 +9242,7 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" t="s">
-        <v>373</v>
+        <v>394</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -9006,7 +9298,7 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" t="s">
-        <v>374</v>
+        <v>395</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -9062,7 +9354,7 @@
     </row>
     <row r="32" spans="1:18">
       <c r="A32" t="s">
-        <v>375</v>
+        <v>396</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -9118,7 +9410,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>376</v>
+        <v>397</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -9174,7 +9466,7 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" t="s">
-        <v>377</v>
+        <v>398</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -9230,17 +9522,17 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>378</v>
+        <v>399</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="140" t="s">
-        <v>379</v>
+      <c r="A38" s="148" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="140" t="s">
-        <v>380</v>
+      <c r="A39" s="148" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -9259,7 +9551,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
@@ -9268,7 +9560,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -9303,7 +9595,7 @@
         <v>8</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -9335,10 +9627,10 @@
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>383</v>
+        <v>404</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>384</v>
+        <v>405</v>
       </c>
     </row>
     <row r="9" spans="13:13">
@@ -9378,15 +9670,15 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>385</v>
+        <v>406</v>
       </c>
       <c r="E12" t="s">
-        <v>386</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="5:5">
       <c r="E13" t="s">
-        <v>387</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14" spans="5:5">
@@ -9396,7 +9688,7 @@
     </row>
     <row r="15" spans="5:5">
       <c r="E15" t="s">
-        <v>388</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -9414,26 +9706,26 @@
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14414414414414" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="9.57142857142857" customWidth="1"/>
+    <col min="1" max="1" width="9.56756756756757" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="22.352380952381" customWidth="1"/>
-    <col min="6" max="6" width="10.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="10.5047619047619" customWidth="1"/>
-    <col min="9" max="9" width="12.5714285714286" customWidth="1"/>
-    <col min="10" max="10" width="11.4952380952381" customWidth="1"/>
+    <col min="3" max="3" width="22.3513513513514" customWidth="1"/>
+    <col min="6" max="6" width="10.8558558558559" customWidth="1"/>
+    <col min="8" max="8" width="10.5045045045045" customWidth="1"/>
+    <col min="9" max="9" width="12.5675675675676" customWidth="1"/>
+    <col min="10" max="10" width="11.4954954954955" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" ht="15.3"/>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>390</v>
+        <v>411</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -9445,7 +9737,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>391</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2">
         <v>7</v>
@@ -9454,7 +9746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="1" ht="15.75" spans="2:8">
+    <row r="4" customFormat="1" ht="15.3" spans="2:8">
       <c r="B4" s="5">
         <v>4</v>
       </c>
@@ -9471,7 +9763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="1" ht="15.75" spans="7:8">
+    <row r="5" customFormat="1" ht="15.3" spans="7:8">
       <c r="G5" s="5">
         <v>11</v>
       </c>
@@ -9481,39 +9773,39 @@
     </row>
     <row r="7" customFormat="1" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75"/>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" ht="15.3"/>
     <row r="9" customFormat="1" spans="1:5">
       <c r="A9" t="s">
-        <v>393</v>
+        <v>414</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>394</v>
+        <v>415</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>395</v>
+        <v>416</v>
       </c>
       <c r="E9" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="10" customFormat="1" ht="15.75" spans="2:5">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" ht="15.3" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>397</v>
+        <v>418</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="E10" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" ht="15.3"/>
     <row r="12" customFormat="1" spans="1:3">
       <c r="A12" t="s">
-        <v>393</v>
+        <v>414</v>
       </c>
       <c r="B12" s="2">
         <v>58</v>
@@ -9522,7 +9814,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" customFormat="1" ht="15.75" spans="2:3">
+    <row r="13" customFormat="1" ht="15.3" spans="2:3">
       <c r="B13" s="5">
         <v>139</v>
       </c>
@@ -9532,41 +9824,41 @@
     </row>
     <row r="16" customFormat="1" spans="1:3">
       <c r="A16" t="s">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="B16" t="s">
-        <v>401</v>
+        <v>422</v>
       </c>
       <c r="C16" t="s">
-        <v>401</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>402</v>
+        <v>423</v>
       </c>
       <c r="B17" t="s">
-        <v>403</v>
+        <v>424</v>
       </c>
       <c r="F17" t="s">
-        <v>404</v>
+        <v>425</v>
       </c>
       <c r="I17" t="s">
-        <v>405</v>
+        <v>426</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:9">
       <c r="A18" t="s">
-        <v>406</v>
+        <v>427</v>
       </c>
       <c r="B18" t="s">
-        <v>407</v>
+        <v>428</v>
       </c>
       <c r="C18" t="s">
-        <v>408</v>
+        <v>429</v>
       </c>
       <c r="F18" t="s">
-        <v>409</v>
+        <v>430</v>
       </c>
       <c r="I18">
         <v>3</v>
@@ -9574,21 +9866,21 @@
     </row>
     <row r="19" customFormat="1" spans="6:6">
       <c r="F19" t="s">
-        <v>410</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
       <c r="A20" t="s">
-        <v>411</v>
+        <v>432</v>
       </c>
       <c r="C20" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="D20" t="s">
-        <v>413</v>
+        <v>434</v>
       </c>
       <c r="F20" t="s">
-        <v>414</v>
+        <v>435</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:9">
@@ -9596,19 +9888,19 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>415</v>
+        <v>436</v>
       </c>
       <c r="D22">
         <v>6000</v>
       </c>
       <c r="E22" t="s">
-        <v>416</v>
+        <v>437</v>
       </c>
       <c r="F22" t="s">
-        <v>407</v>
+        <v>428</v>
       </c>
       <c r="G22" t="s">
-        <v>417</v>
+        <v>438</v>
       </c>
       <c r="H22">
         <v>12000</v>
@@ -9619,15 +9911,15 @@
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" t="s">
-        <v>418</v>
+        <v>439</v>
       </c>
       <c r="C23" t="s">
-        <v>419</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="3:4">
       <c r="C24" t="s">
-        <v>420</v>
+        <v>441</v>
       </c>
       <c r="D24" s="1">
         <v>32000</v>
@@ -9635,7 +9927,7 @@
     </row>
     <row r="27" customFormat="1" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>421</v>
+        <v>442</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:5">
@@ -9660,34 +9952,34 @@
         <v>174</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>422</v>
+        <v>443</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>423</v>
+        <v>444</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>424</v>
+        <v>445</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>425</v>
+        <v>446</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75"/>
-    <row r="32" customFormat="1" ht="15.75" spans="3:10">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="31" ht="15.3"/>
+    <row r="32" customFormat="1" ht="15.3" spans="3:10">
       <c r="C32" s="10" t="s">
-        <v>422</v>
+        <v>443</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>423</v>
+        <v>444</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>424</v>
+        <v>445</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>425</v>
+        <v>446</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>178</v>
@@ -9696,7 +9988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="1" ht="15.75" spans="3:8">
+    <row r="33" customFormat="1" ht="15.3" spans="3:8">
       <c r="C33">
         <v>0</v>
       </c>
@@ -9715,7 +10007,7 @@
     </row>
     <row r="34" customFormat="1" spans="1:10">
       <c r="A34" s="10" t="s">
-        <v>422</v>
+        <v>443</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -9733,10 +10025,10 @@
         <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>427</v>
+        <v>448</v>
       </c>
       <c r="I34" t="s">
-        <v>428</v>
+        <v>449</v>
       </c>
       <c r="J34" s="24">
         <v>6</v>
@@ -9744,7 +10036,7 @@
     </row>
     <row r="35" customFormat="1" spans="1:10">
       <c r="A35" s="10" t="s">
-        <v>423</v>
+        <v>444</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -9760,10 +10052,10 @@
         <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>429</v>
+        <v>450</v>
       </c>
       <c r="I35" t="s">
-        <v>430</v>
+        <v>451</v>
       </c>
       <c r="J35" s="24">
         <v>24</v>
@@ -9771,7 +10063,7 @@
     </row>
     <row r="36" customFormat="1" spans="1:10">
       <c r="A36" s="10" t="s">
-        <v>424</v>
+        <v>445</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -9785,18 +10077,18 @@
         <v>36</v>
       </c>
       <c r="H36" t="s">
-        <v>431</v>
+        <v>452</v>
       </c>
       <c r="I36" t="s">
-        <v>432</v>
+        <v>453</v>
       </c>
       <c r="J36" s="24">
         <v>36</v>
       </c>
     </row>
-    <row r="37" customFormat="1" ht="15.75" spans="1:6">
+    <row r="37" customFormat="1" ht="15.3" spans="1:6">
       <c r="A37" s="10" t="s">
-        <v>425</v>
+        <v>446</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -9808,35 +10100,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="1" ht="15.75" spans="8:8">
+    <row r="38" customFormat="1" ht="15.3" spans="8:8">
       <c r="H38" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="39" ht="15.75" spans="2:11">
+    <row r="39" ht="15.3" spans="2:11">
       <c r="B39" s="22" t="s">
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
       <c r="D39" t="s">
         <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>434</v>
+        <v>455</v>
       </c>
       <c r="F39" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="H39" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
       <c r="I39" t="s">
-        <v>436</v>
+        <v>457</v>
       </c>
       <c r="J39" t="s">
-        <v>437</v>
+        <v>458</v>
       </c>
       <c r="K39">
         <v>32</v>
@@ -9844,13 +10136,13 @@
     </row>
     <row r="40" spans="4:11">
       <c r="D40" t="s">
-        <v>438</v>
+        <v>459</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>439</v>
+        <v>460</v>
       </c>
       <c r="J40" t="s">
-        <v>440</v>
+        <v>461</v>
       </c>
       <c r="K40" s="24">
         <v>18</v>
@@ -9858,7 +10150,7 @@
     </row>
     <row r="41" customFormat="1" spans="4:4">
       <c r="D41" t="s">
-        <v>441</v>
+        <v>462</v>
       </c>
     </row>
     <row r="42" spans="4:11">
@@ -9866,19 +10158,19 @@
         <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>442</v>
+        <v>463</v>
       </c>
       <c r="F42" t="s">
-        <v>435</v>
+        <v>456</v>
       </c>
       <c r="H42" t="s">
-        <v>443</v>
+        <v>464</v>
       </c>
       <c r="I42" t="s">
-        <v>444</v>
+        <v>465</v>
       </c>
       <c r="J42" t="s">
-        <v>445</v>
+        <v>466</v>
       </c>
       <c r="K42">
         <v>54</v>
@@ -9886,39 +10178,39 @@
     </row>
     <row r="43" spans="4:11">
       <c r="D43" t="s">
-        <v>446</v>
+        <v>467</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>447</v>
+        <v>468</v>
       </c>
       <c r="J43" t="s">
-        <v>448</v>
+        <v>469</v>
       </c>
       <c r="K43" s="24">
         <v>48</v>
       </c>
     </row>
-    <row r="44" ht="15.75"/>
-    <row r="45" customFormat="1" ht="15.75" spans="7:7">
+    <row r="44" ht="15.3"/>
+    <row r="45" customFormat="1" ht="15.3" spans="7:7">
       <c r="G45" s="11" t="s">
-        <v>449</v>
+        <v>470</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="2:10">
       <c r="B46" t="s">
-        <v>450</v>
+        <v>471</v>
       </c>
       <c r="C46" t="s">
-        <v>451</v>
+        <v>472</v>
       </c>
       <c r="G46" t="s">
-        <v>452</v>
+        <v>473</v>
       </c>
       <c r="H46" t="s">
-        <v>450</v>
+        <v>471</v>
       </c>
       <c r="I46" t="s">
-        <v>453</v>
+        <v>474</v>
       </c>
       <c r="J46">
         <v>54</v>
@@ -9926,16 +10218,16 @@
     </row>
     <row r="47" customFormat="1" spans="2:10">
       <c r="B47" t="s">
-        <v>454</v>
+        <v>475</v>
       </c>
       <c r="C47" t="s">
-        <v>455</v>
+        <v>476</v>
       </c>
       <c r="H47" t="s">
-        <v>454</v>
+        <v>475</v>
       </c>
       <c r="I47" t="s">
-        <v>456</v>
+        <v>477</v>
       </c>
       <c r="J47">
         <v>51</v>
@@ -9943,31 +10235,31 @@
     </row>
     <row r="48" customFormat="1" spans="2:10">
       <c r="B48" s="23" t="s">
-        <v>457</v>
+        <v>478</v>
       </c>
       <c r="C48" t="s">
-        <v>458</v>
+        <v>479</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>457</v>
+        <v>478</v>
       </c>
       <c r="I48" t="s">
-        <v>459</v>
+        <v>480</v>
       </c>
       <c r="J48" s="24">
         <v>30</v>
       </c>
     </row>
-    <row r="50" customFormat="1" ht="15.75" spans="1:6">
+    <row r="50" customFormat="1" ht="15.3" spans="1:6">
       <c r="A50" s="22" t="s">
         <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>460</v>
+        <v>481</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>461</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>